<commit_message>
Minimum AF and Max Retrofits type per archeytype
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
@@ -3,9 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D24FBF-8858-46BD-A9F5-D21590347A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25839AB9-0AA1-4702-89A1-AC80056A6BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="224">
   <si>
     <t>Document type:</t>
   </si>
@@ -758,17 +757,27 @@
   <si>
     <t>http://www.esru.strath.ac.uk/EandE/Web_sites/16-17/Retrofit/uploads/1/0/5/7/105723345/phpp_sap_and_sbem_comparison_study.pdf</t>
   </si>
+  <si>
+    <t>No Retrofit Required for Heat Pump</t>
+  </si>
+  <si>
+    <t>Shallow Retrofit Required for Heat Pump</t>
+  </si>
+  <si>
+    <t>Deep Retrofit Required for Heat Pump</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
   <fonts count="47" x14ac:knownFonts="1">
     <font>
@@ -2164,9 +2173,6 @@
     <xf numFmtId="1" fontId="5" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="22" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2262,6 +2268,9 @@
     </xf>
     <xf numFmtId="9" fontId="9" fillId="15" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3750,10 +3759,7 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:F17"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4205,10 +4211,7 @@
   </sheetPr>
   <dimension ref="B1:T45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4942,10 +4945,7 @@
   </sheetPr>
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:U12"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5090,7 +5090,7 @@
       <c r="O6" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="P6" s="161" t="s">
+      <c r="P6" s="160" t="s">
         <v>142</v>
       </c>
       <c r="R6" s="89"/>
@@ -5148,7 +5148,7 @@
         <f>V7</f>
         <v>5.9072960538612464E-3</v>
       </c>
-      <c r="P7" s="162">
+      <c r="P7" s="161">
         <f>Data!U59/1000</f>
         <v>11.196414691601362</v>
       </c>
@@ -5161,7 +5161,7 @@
       <c r="T7" s="85">
         <v>1.6E-2</v>
       </c>
-      <c r="U7" s="164">
+      <c r="U7" s="163">
         <f>Data!X59</f>
         <v>0.36920600336632792</v>
       </c>
@@ -5213,7 +5213,7 @@
         <f t="shared" ref="O8:O12" si="4">V8</f>
         <v>8.1965689357556444E-3</v>
       </c>
-      <c r="P8" s="163">
+      <c r="P8" s="162">
         <f>Data!U60/1000</f>
         <v>15.982779351113084</v>
       </c>
@@ -5226,7 +5226,7 @@
       <c r="T8" s="86">
         <v>1.6E-2</v>
       </c>
-      <c r="U8" s="165">
+      <c r="U8" s="164">
         <f>Data!X60</f>
         <v>0.51228555848472779</v>
       </c>
@@ -5278,7 +5278,7 @@
         <f t="shared" si="4"/>
         <v>9.413814304323951E-3</v>
       </c>
-      <c r="P9" s="162">
+      <c r="P9" s="161">
         <f>Data!S59/1000</f>
         <v>9.6084735804205188</v>
       </c>
@@ -5291,7 +5291,7 @@
       <c r="T9" s="85">
         <v>2.69E-2</v>
       </c>
-      <c r="U9" s="164">
+      <c r="U9" s="163">
         <f>Data!V59</f>
         <v>0.3499559220938272</v>
       </c>
@@ -5343,7 +5343,7 @@
         <f t="shared" si="4"/>
         <v>1.5328198459374942E-2</v>
       </c>
-      <c r="P10" s="163">
+      <c r="P10" s="162">
         <f>Data!S60/1000</f>
         <v>20.5630239417189</v>
       </c>
@@ -5356,7 +5356,7 @@
       <c r="T10" s="86">
         <v>2.69E-2</v>
       </c>
-      <c r="U10" s="165">
+      <c r="U10" s="164">
         <f>Data!V60</f>
         <v>0.56982150406598298</v>
       </c>
@@ -5408,7 +5408,7 @@
         <f t="shared" si="4"/>
         <v>1.6649605686878701E-2</v>
       </c>
-      <c r="P11" s="162">
+      <c r="P11" s="161">
         <f>Data!T59/1000</f>
         <v>14.333869646601945</v>
       </c>
@@ -5421,7 +5421,7 @@
       <c r="T11" s="85">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="U11" s="164">
+      <c r="U11" s="163">
         <f>Data!W59</f>
         <v>0.34759093292022342</v>
       </c>
@@ -5473,7 +5473,7 @@
         <f t="shared" si="4"/>
         <v>2.7503185042088787E-2</v>
       </c>
-      <c r="P12" s="163">
+      <c r="P12" s="162">
         <f>Data!T60/1000</f>
         <v>22.25938755708523</v>
       </c>
@@ -5486,7 +5486,7 @@
       <c r="T12" s="86">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="U12" s="165">
+      <c r="U12" s="164">
         <f>Data!W60</f>
         <v>0.57417922843609159</v>
       </c>
@@ -5736,10 +5736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="W59" sqref="W59"/>
     </sheetView>
   </sheetViews>
@@ -5782,7 +5779,7 @@
       </c>
       <c r="S2" s="184"/>
       <c r="T2" s="185"/>
-      <c r="Y2" s="126" t="s">
+      <c r="Y2" s="125" t="s">
         <v>206</v>
       </c>
     </row>
@@ -5824,7 +5821,7 @@
       <c r="U3" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="Y3" s="127"/>
+      <c r="Y3" s="126"/>
       <c r="AB3" s="5" t="s">
         <v>134</v>
       </c>
@@ -5890,11 +5887,11 @@
       <c r="T4" s="100">
         <v>56</v>
       </c>
-      <c r="U4" s="146">
+      <c r="U4" s="145">
         <f>AVERAGE(R4:T4)</f>
         <v>54.181824878333337</v>
       </c>
-      <c r="Y4" s="128"/>
+      <c r="Y4" s="127"/>
     </row>
     <row r="5" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C5" s="97" t="s">
@@ -5942,27 +5939,27 @@
       <c r="T5" s="105">
         <v>90</v>
       </c>
-      <c r="U5" s="146">
+      <c r="U5" s="145">
         <f t="shared" ref="U5:U12" si="0">AVERAGE(R5:T5)</f>
         <v>90.104603265666654</v>
       </c>
-      <c r="AA5" s="129" t="s">
+      <c r="AA5" s="128" t="s">
         <v>145</v>
       </c>
       <c r="AB5">
         <f>AVERAGE(AH5:AI5)</f>
         <v>235</v>
       </c>
-      <c r="AC5" s="130">
+      <c r="AC5" s="129">
         <v>400</v>
       </c>
-      <c r="AD5" s="130">
+      <c r="AD5" s="129">
         <v>140</v>
       </c>
-      <c r="AH5" s="131">
+      <c r="AH5" s="130">
         <v>190</v>
       </c>
-      <c r="AI5" s="130">
+      <c r="AI5" s="129">
         <v>280</v>
       </c>
     </row>
@@ -6012,27 +6009,27 @@
       <c r="T6" s="110">
         <v>116</v>
       </c>
-      <c r="U6" s="146">
+      <c r="U6" s="145">
         <f t="shared" si="0"/>
         <v>115.45560966933333</v>
       </c>
-      <c r="AA6" s="132" t="s">
+      <c r="AA6" s="131" t="s">
         <v>147</v>
       </c>
       <c r="AB6">
         <f t="shared" ref="AB6:AB19" si="1">AVERAGE(AH6:AI6)</f>
         <v>470</v>
       </c>
-      <c r="AC6" s="133">
+      <c r="AC6" s="132">
         <v>800</v>
       </c>
-      <c r="AD6" s="133">
+      <c r="AD6" s="132">
         <v>280</v>
       </c>
-      <c r="AH6" s="134">
+      <c r="AH6" s="133">
         <v>380</v>
       </c>
-      <c r="AI6" s="133">
+      <c r="AI6" s="132">
         <v>560</v>
       </c>
     </row>
@@ -6082,27 +6079,27 @@
       <c r="T7" s="105">
         <v>140</v>
       </c>
-      <c r="U7" s="146">
+      <c r="U7" s="145">
         <f t="shared" si="0"/>
         <v>139.59487310199998</v>
       </c>
-      <c r="AA7" s="132" t="s">
+      <c r="AA7" s="131" t="s">
         <v>148</v>
       </c>
       <c r="AB7">
         <f t="shared" si="1"/>
         <v>585</v>
       </c>
-      <c r="AC7" s="133">
+      <c r="AC7" s="132">
         <v>900</v>
       </c>
-      <c r="AD7" s="133">
+      <c r="AD7" s="132">
         <v>350</v>
       </c>
-      <c r="AH7" s="134">
+      <c r="AH7" s="133">
         <v>470</v>
       </c>
-      <c r="AI7" s="133">
+      <c r="AI7" s="132">
         <v>700</v>
       </c>
     </row>
@@ -6152,27 +6149,27 @@
       <c r="T8" s="110">
         <v>190</v>
       </c>
-      <c r="U8" s="146">
+      <c r="U8" s="145">
         <f t="shared" si="0"/>
         <v>188.85972977266667</v>
       </c>
-      <c r="AA8" s="132" t="s">
+      <c r="AA8" s="131" t="s">
         <v>149</v>
       </c>
       <c r="AB8">
         <f t="shared" si="1"/>
         <v>745</v>
       </c>
-      <c r="AC8" s="135">
+      <c r="AC8" s="134">
         <v>1200</v>
       </c>
-      <c r="AD8" s="133">
+      <c r="AD8" s="132">
         <v>440</v>
       </c>
-      <c r="AH8" s="134">
+      <c r="AH8" s="133">
         <v>590</v>
       </c>
-      <c r="AI8" s="133">
+      <c r="AI8" s="132">
         <v>900</v>
       </c>
     </row>
@@ -6225,27 +6222,27 @@
       <c r="T9" s="105">
         <v>261</v>
       </c>
-      <c r="U9" s="146">
+      <c r="U9" s="145">
         <f t="shared" si="0"/>
         <v>260.5202750266667</v>
       </c>
-      <c r="AA9" s="132" t="s">
+      <c r="AA9" s="131" t="s">
         <v>150</v>
       </c>
       <c r="AB9">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="AC9" s="135">
+      <c r="AC9" s="134">
         <v>1500</v>
       </c>
-      <c r="AD9" s="133">
+      <c r="AD9" s="132">
         <v>570</v>
       </c>
-      <c r="AH9" s="134">
+      <c r="AH9" s="133">
         <v>800</v>
       </c>
-      <c r="AI9" s="135">
+      <c r="AI9" s="134">
         <v>1100</v>
       </c>
     </row>
@@ -6295,27 +6292,27 @@
       <c r="T10" s="110">
         <v>338</v>
       </c>
-      <c r="U10" s="146">
+      <c r="U10" s="145">
         <f t="shared" si="0"/>
         <v>337.60044621333333</v>
       </c>
-      <c r="AA10" s="132" t="s">
+      <c r="AA10" s="131" t="s">
         <v>151</v>
       </c>
       <c r="AB10">
         <f t="shared" si="1"/>
         <v>1150</v>
       </c>
-      <c r="AC10" s="135">
+      <c r="AC10" s="134">
         <v>1900</v>
       </c>
-      <c r="AD10" s="133">
+      <c r="AD10" s="132">
         <v>700</v>
       </c>
-      <c r="AH10" s="134">
+      <c r="AH10" s="133">
         <v>900</v>
       </c>
-      <c r="AI10" s="135">
+      <c r="AI10" s="134">
         <v>1400</v>
       </c>
     </row>
@@ -6365,27 +6362,27 @@
       <c r="T11" s="105">
         <v>415</v>
       </c>
-      <c r="U11" s="146">
+      <c r="U11" s="145">
         <f t="shared" si="0"/>
         <v>413.55162632333332</v>
       </c>
-      <c r="AA11" s="132" t="s">
+      <c r="AA11" s="131" t="s">
         <v>152</v>
       </c>
       <c r="AB11">
         <f t="shared" si="1"/>
         <v>1350</v>
       </c>
-      <c r="AC11" s="135">
+      <c r="AC11" s="134">
         <v>2200</v>
       </c>
-      <c r="AD11" s="133">
+      <c r="AD11" s="132">
         <v>800</v>
       </c>
-      <c r="AH11" s="136">
+      <c r="AH11" s="135">
         <v>1100</v>
       </c>
-      <c r="AI11" s="135">
+      <c r="AI11" s="134">
         <v>1600</v>
       </c>
     </row>
@@ -6435,27 +6432,27 @@
       <c r="T12" s="116">
         <v>673</v>
       </c>
-      <c r="U12" s="146">
+      <c r="U12" s="145">
         <f t="shared" si="0"/>
         <v>626.50035470099999</v>
       </c>
-      <c r="AA12" s="132" t="s">
+      <c r="AA12" s="131" t="s">
         <v>154</v>
       </c>
       <c r="AB12">
         <f t="shared" si="1"/>
         <v>1600</v>
       </c>
-      <c r="AC12" s="135">
+      <c r="AC12" s="134">
         <v>2600</v>
       </c>
-      <c r="AD12" s="135">
+      <c r="AD12" s="134">
         <v>1000</v>
       </c>
-      <c r="AH12" s="136">
+      <c r="AH12" s="135">
         <v>1300</v>
       </c>
-      <c r="AI12" s="135">
+      <c r="AI12" s="134">
         <v>1900</v>
       </c>
     </row>
@@ -6484,23 +6481,23 @@
       <c r="Q13" s="119">
         <v>0.71303848954914961</v>
       </c>
-      <c r="AA13" s="132" t="s">
+      <c r="AA13" s="131" t="s">
         <v>155</v>
       </c>
       <c r="AB13">
         <f t="shared" si="1"/>
         <v>1850</v>
       </c>
-      <c r="AC13" s="135">
+      <c r="AC13" s="134">
         <v>2900</v>
       </c>
-      <c r="AD13" s="135">
+      <c r="AD13" s="134">
         <v>1100</v>
       </c>
-      <c r="AH13" s="136">
+      <c r="AH13" s="135">
         <v>1500</v>
       </c>
-      <c r="AI13" s="135">
+      <c r="AI13" s="134">
         <v>2200</v>
       </c>
     </row>
@@ -6508,35 +6505,38 @@
       <c r="C14" s="120" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="121">
+      <c r="D14" s="145">
+        <f>SUM(D5:D13)</f>
+        <v>766351.72099999979</v>
+      </c>
+      <c r="E14" s="145">
+        <f t="shared" ref="E14:F14" si="2">SUM(E5:E13)</f>
+        <v>724429.72899999993</v>
+      </c>
+      <c r="F14" s="145">
+        <f t="shared" si="2"/>
         <v>206798.88499999998</v>
       </c>
-      <c r="E14" s="121">
-        <v>766351.72099999979</v>
-      </c>
-      <c r="F14" s="121">
-        <v>724429.72899999993</v>
-      </c>
-      <c r="G14" s="122">
+      <c r="G14" s="121">
         <v>1697580.3349999997</v>
       </c>
-      <c r="AA14" s="132" t="s">
+      <c r="AA14" s="131" t="s">
         <v>156</v>
       </c>
       <c r="AB14">
         <f t="shared" si="1"/>
         <v>2150</v>
       </c>
-      <c r="AC14" s="135">
+      <c r="AC14" s="134">
         <v>3500</v>
       </c>
-      <c r="AD14" s="135">
+      <c r="AD14" s="134">
         <v>1300</v>
       </c>
-      <c r="AH14" s="136">
+      <c r="AH14" s="135">
         <v>1700</v>
       </c>
-      <c r="AI14" s="135">
+      <c r="AI14" s="134">
         <v>2600</v>
       </c>
     </row>
@@ -6544,52 +6544,61 @@
       <c r="L15" t="s">
         <v>212</v>
       </c>
-      <c r="AA15" s="132" t="s">
+      <c r="AA15" s="131" t="s">
         <v>158</v>
       </c>
       <c r="AB15">
         <f t="shared" si="1"/>
         <v>2550</v>
       </c>
-      <c r="AC15" s="135">
+      <c r="AC15" s="134">
         <v>4100</v>
       </c>
-      <c r="AD15" s="135">
+      <c r="AD15" s="134">
         <v>1500</v>
       </c>
-      <c r="AH15" s="136">
+      <c r="AH15" s="135">
         <v>2000</v>
       </c>
-      <c r="AI15" s="135">
+      <c r="AI15" s="134">
         <v>3100</v>
       </c>
     </row>
-    <row r="16" spans="3:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L16" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="AA16" s="132" t="s">
+      <c r="AA16" s="131" t="s">
         <v>159</v>
       </c>
       <c r="AB16">
         <f t="shared" si="1"/>
         <v>2900</v>
       </c>
-      <c r="AC16" s="135">
+      <c r="AC16" s="134">
         <v>4700</v>
       </c>
-      <c r="AD16" s="135">
+      <c r="AD16" s="134">
         <v>1800</v>
       </c>
-      <c r="AH16" s="136">
+      <c r="AH16" s="135">
         <v>2300</v>
       </c>
-      <c r="AI16" s="135">
+      <c r="AI16" s="134">
         <v>3500</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L17" s="124" t="s">
+    <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="G17" s="94" t="s">
+        <v>194</v>
+      </c>
+      <c r="H17" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="L17" s="123" t="s">
         <v>205</v>
       </c>
       <c r="O17" s="5" t="s">
@@ -6619,28 +6628,43 @@
       <c r="W17" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="AA17" s="132" t="s">
+      <c r="AA17" s="131" t="s">
         <v>161</v>
       </c>
       <c r="AB17">
         <f t="shared" si="1"/>
         <v>3300</v>
       </c>
-      <c r="AC17" s="135">
+      <c r="AC17" s="134">
         <v>5300</v>
       </c>
-      <c r="AD17" s="135">
+      <c r="AD17" s="134">
         <v>2000</v>
       </c>
-      <c r="AH17" s="136">
+      <c r="AH17" s="135">
         <v>2600</v>
       </c>
-      <c r="AI17" s="135">
+      <c r="AI17" s="134">
         <v>4000</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.2">
-      <c r="L18" s="123" t="s">
+      <c r="C18" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="145">
+        <f>SUM(D5:D8)</f>
+        <v>92323.794764485472</v>
+      </c>
+      <c r="G18" s="145">
+        <f>SUM(E5:E8)</f>
+        <v>103369.76677783766</v>
+      </c>
+      <c r="H18" s="145">
+        <f>SUM(F5:F8)</f>
+        <v>50844.518002144141</v>
+      </c>
+      <c r="L18" s="122" t="s">
         <v>204</v>
       </c>
       <c r="O18" s="97" t="s">
@@ -6654,223 +6678,308 @@
         <f>1-U4/$U$11</f>
         <v>0.86898413298471344</v>
       </c>
-      <c r="R18" s="125">
+      <c r="R18" s="124">
         <f>1-U4/$U$10</f>
         <v>0.83950902468862476</v>
       </c>
-      <c r="S18" s="125">
+      <c r="S18" s="124">
         <f>1-U4/$U$9</f>
         <v>0.79202453677439377</v>
       </c>
-      <c r="T18" s="125">
+      <c r="T18" s="124">
         <f>1-U4/$U$8</f>
         <v>0.71311075715530881</v>
       </c>
-      <c r="U18" s="125">
+      <c r="U18" s="124">
         <f>1-U4/$U$7</f>
         <v>0.61186379073718955</v>
       </c>
-      <c r="V18" s="125">
+      <c r="V18" s="124">
         <f>1-U4/$U$6</f>
         <v>0.53071292912045642</v>
       </c>
-      <c r="W18" s="125">
+      <c r="W18" s="124">
         <f>1-U4/$U$5</f>
         <v>0.39867861447009212</v>
       </c>
-      <c r="AA18" s="132" t="s">
+      <c r="AA18" s="131" t="s">
         <v>162</v>
       </c>
       <c r="AB18">
         <f t="shared" si="1"/>
         <v>3950</v>
       </c>
-      <c r="AC18" s="135">
+      <c r="AC18" s="134">
         <v>6300</v>
       </c>
-      <c r="AD18" s="135">
+      <c r="AD18" s="134">
         <v>2400</v>
       </c>
-      <c r="AH18" s="136">
+      <c r="AH18" s="135">
         <v>3200</v>
       </c>
-      <c r="AI18" s="135">
+      <c r="AI18" s="134">
         <v>4700</v>
       </c>
     </row>
     <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="145">
+        <f>D9</f>
+        <v>282151.52747564798</v>
+      </c>
+      <c r="G19" s="145">
+        <f t="shared" ref="G19:H19" si="3">E9</f>
+        <v>251318.93361374349</v>
+      </c>
+      <c r="H19" s="145">
+        <f t="shared" si="3"/>
+        <v>58904.8034364337</v>
+      </c>
       <c r="O19" s="102" t="s">
         <v>149</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P25" si="2">1-U5/$U$12</f>
+        <f t="shared" ref="P19:P25" si="4">1-U5/$U$12</f>
         <v>0.85617788946237794</v>
       </c>
-      <c r="Q19" s="125">
-        <f t="shared" ref="Q19:Q24" si="3">1-U5/$U$11</f>
+      <c r="Q19" s="124">
+        <f t="shared" ref="Q19:Q24" si="5">1-U5/$U$11</f>
         <v>0.78212006063973538</v>
       </c>
-      <c r="R19" s="125">
-        <f t="shared" ref="R19:R23" si="4">1-U5/$U$10</f>
+      <c r="R19" s="124">
+        <f t="shared" ref="R19:R23" si="6">1-U5/$U$10</f>
         <v>0.73310283124232423</v>
       </c>
-      <c r="S19" s="125">
-        <f t="shared" ref="S19:S22" si="5">1-U5/$U$9</f>
+      <c r="S19" s="124">
+        <f t="shared" ref="S19:S22" si="7">1-U5/$U$9</f>
         <v>0.65413592759164874</v>
       </c>
-      <c r="T19" s="125">
-        <f t="shared" ref="T19:T21" si="6">1-U5/$U$8</f>
+      <c r="T19" s="124">
+        <f t="shared" ref="T19:T21" si="8">1-U5/$U$8</f>
         <v>0.5229019792936962</v>
       </c>
-      <c r="U19" s="125">
-        <f t="shared" ref="U19:U20" si="7">1-U5/$U$7</f>
+      <c r="U19" s="124">
+        <f t="shared" ref="U19:U20" si="9">1-U5/$U$7</f>
         <v>0.35452784716650365</v>
       </c>
       <c r="V19" s="93">
         <f>1-U5/$U$6</f>
         <v>0.21957362207234754</v>
       </c>
-      <c r="AA19" s="137" t="s">
+      <c r="AA19" s="136" t="s">
         <v>163</v>
       </c>
       <c r="AB19">
         <f t="shared" si="1"/>
         <v>4950</v>
       </c>
-      <c r="AC19" s="138">
+      <c r="AC19" s="137">
         <v>7900</v>
       </c>
-      <c r="AD19" s="138">
+      <c r="AD19" s="137">
         <v>3000</v>
       </c>
-      <c r="AH19" s="139">
+      <c r="AH19" s="138">
         <v>4000</v>
       </c>
-      <c r="AI19" s="138">
+      <c r="AI19" s="137">
         <v>5900</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="145">
+        <f>SUM(D10:D13)</f>
+        <v>391876.39875986642</v>
+      </c>
+      <c r="G20" s="145">
+        <f t="shared" ref="G20:H20" si="10">SUM(E10:E13)</f>
+        <v>369741.02860841871</v>
+      </c>
+      <c r="H20" s="145">
+        <f t="shared" si="10"/>
+        <v>97049.563561422125</v>
+      </c>
       <c r="O20" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="P20" s="125">
-        <f t="shared" si="2"/>
+      <c r="P20" s="124">
+        <f t="shared" si="4"/>
         <v>0.81571341691508692</v>
       </c>
-      <c r="Q20" s="125">
-        <f t="shared" si="3"/>
+      <c r="Q20" s="124">
+        <f t="shared" si="5"/>
         <v>0.72081935526215313</v>
       </c>
-      <c r="R20" s="125">
-        <f t="shared" si="4"/>
+      <c r="R20" s="124">
+        <f t="shared" si="6"/>
         <v>0.658011086879975</v>
       </c>
-      <c r="S20" s="125">
-        <f t="shared" si="5"/>
+      <c r="S20" s="124">
+        <f t="shared" si="7"/>
         <v>0.55682677804053693</v>
       </c>
-      <c r="T20" s="125">
-        <f t="shared" si="6"/>
+      <c r="T20" s="124">
+        <f t="shared" si="8"/>
         <v>0.388670047297489</v>
       </c>
       <c r="U20" s="93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.17292371056513256</v>
       </c>
-      <c r="Y20" s="140" t="s">
+      <c r="Y20" s="139" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="145">
+        <f>SUM(F18:F20)</f>
+        <v>766351.7209999999</v>
+      </c>
       <c r="G21" s="85"/>
       <c r="O21" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="P21" s="125">
-        <f t="shared" si="2"/>
+      <c r="P21" s="124">
+        <f t="shared" si="4"/>
         <v>0.77718309007403152</v>
       </c>
-      <c r="Q21" s="125">
-        <f t="shared" si="3"/>
+      <c r="Q21" s="124">
+        <f t="shared" si="5"/>
         <v>0.66244873864222598</v>
       </c>
-      <c r="R21" s="125">
-        <f t="shared" si="4"/>
+      <c r="R21" s="124">
+        <f t="shared" si="6"/>
         <v>0.58650862382513413</v>
       </c>
-      <c r="S21" s="125">
-        <f t="shared" si="5"/>
+      <c r="S21" s="124">
+        <f t="shared" si="7"/>
         <v>0.46416887097285942</v>
       </c>
       <c r="T21" s="93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.26085421561265365</v>
       </c>
-      <c r="Y21" s="141" t="s">
+      <c r="Y21" s="140" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.2">
-      <c r="G22" s="85"/>
+      <c r="F22" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="94" t="s">
+        <v>194</v>
+      </c>
+      <c r="H22" s="94" t="s">
+        <v>192</v>
+      </c>
       <c r="O22" s="107" t="s">
         <v>153</v>
       </c>
-      <c r="P22" s="125">
-        <f t="shared" si="2"/>
+      <c r="P22" s="124">
+        <f t="shared" si="4"/>
         <v>0.69854808803292578</v>
       </c>
-      <c r="Q22" s="125">
-        <f t="shared" si="3"/>
+      <c r="Q22" s="124">
+        <f t="shared" si="5"/>
         <v>0.54332248321275467</v>
       </c>
-      <c r="R22" s="125">
-        <f t="shared" si="4"/>
+      <c r="R22" s="124">
+        <f t="shared" si="6"/>
         <v>0.44058210855170443</v>
       </c>
       <c r="S22" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.27506705666829534</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.2">
-      <c r="G23" s="85"/>
+      <c r="C23" t="s">
+        <v>221</v>
+      </c>
+      <c r="F23" s="165">
+        <f>F18/$D$14</f>
+        <v>0.12047183066805627</v>
+      </c>
+      <c r="G23" s="165">
+        <f>G18/$E$14</f>
+        <v>0.14269122682268837</v>
+      </c>
+      <c r="H23" s="165">
+        <f>H18/$F$14</f>
+        <v>0.24586456547937455</v>
+      </c>
       <c r="O23" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="P23" s="125">
-        <f t="shared" si="2"/>
+      <c r="P23" s="124">
+        <f t="shared" si="4"/>
         <v>0.58416579803693625</v>
       </c>
-      <c r="Q23" s="125">
-        <f t="shared" si="3"/>
+      <c r="Q23" s="124">
+        <f t="shared" si="5"/>
         <v>0.37004171077063985</v>
       </c>
       <c r="R23" s="93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.22831774084196221</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.2">
-      <c r="G24" s="85"/>
+      <c r="C24" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" s="165">
+        <f t="shared" ref="F24:F25" si="11">F19/$D$14</f>
+        <v>0.36817497729041837</v>
+      </c>
+      <c r="G24" s="165">
+        <f t="shared" ref="G24:G25" si="12">G19/$E$14</f>
+        <v>0.34691968530979972</v>
+      </c>
+      <c r="H24" s="165">
+        <f t="shared" ref="H24:H25" si="13">H19/$F$14</f>
+        <v>0.28484101080348528</v>
+      </c>
       <c r="O24" s="107" t="s">
         <v>160</v>
       </c>
-      <c r="P24" s="125">
-        <f t="shared" si="2"/>
+      <c r="P24" s="124">
+        <f t="shared" si="4"/>
         <v>0.46113287298224337</v>
       </c>
       <c r="Q24" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.18365586126511313</v>
       </c>
     </row>
     <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F25" s="165">
+        <f t="shared" si="11"/>
+        <v>0.51135319204152541</v>
+      </c>
+      <c r="G25" s="165">
+        <f t="shared" si="12"/>
+        <v>0.5103890878675118</v>
+      </c>
+      <c r="H25" s="165">
+        <f t="shared" si="13"/>
+        <v>0.46929442371714014</v>
+      </c>
       <c r="O25" s="102" t="s">
         <v>162</v>
       </c>
       <c r="P25" s="93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.33990200768409362</v>
       </c>
     </row>
@@ -6880,12 +6989,12 @@
     </row>
     <row r="28" spans="1:35" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="91"/>
-      <c r="H28" s="145"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="144"/>
+      <c r="J28" s="144"/>
     </row>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="124" t="s">
+      <c r="A29" s="123" t="s">
         <v>205</v>
       </c>
       <c r="C29" s="186" t="s">
@@ -6924,1622 +7033,1622 @@
       <c r="X29" s="181"/>
     </row>
     <row r="30" spans="1:35" ht="21" x14ac:dyDescent="0.2">
-      <c r="A30" s="123" t="s">
+      <c r="A30" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="142"/>
-      <c r="D30" s="142"/>
-      <c r="E30" s="143" t="s">
+      <c r="C30" s="141"/>
+      <c r="D30" s="141"/>
+      <c r="E30" s="142" t="s">
         <v>200</v>
       </c>
-      <c r="F30" s="143" t="s">
+      <c r="F30" s="142" t="s">
         <v>199</v>
       </c>
-      <c r="G30" s="143" t="s">
+      <c r="G30" s="142" t="s">
         <v>201</v>
       </c>
-      <c r="H30" s="143" t="s">
+      <c r="H30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="I30" s="143" t="s">
+      <c r="I30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="J30" s="143" t="s">
+      <c r="J30" s="142" t="s">
         <v>135</v>
       </c>
-      <c r="K30" s="143" t="s">
+      <c r="K30" s="142" t="s">
         <v>135</v>
       </c>
-      <c r="L30" s="143" t="s">
+      <c r="L30" s="142" t="s">
         <v>133</v>
       </c>
-      <c r="M30" s="143" t="s">
+      <c r="M30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="N30" s="143" t="s">
+      <c r="N30" s="142" t="s">
         <v>135</v>
       </c>
-      <c r="O30" s="143" t="s">
+      <c r="O30" s="142" t="s">
         <v>133</v>
       </c>
-      <c r="P30" s="151" t="s">
+      <c r="P30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="Q30" s="151" t="s">
+      <c r="Q30" s="150" t="s">
         <v>135</v>
       </c>
-      <c r="R30" s="151" t="s">
+      <c r="R30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="S30" s="151" t="s">
+      <c r="S30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="T30" s="151" t="s">
+      <c r="T30" s="150" t="s">
         <v>135</v>
       </c>
-      <c r="U30" s="151" t="s">
+      <c r="U30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="V30" s="151" t="s">
+      <c r="V30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="W30" s="151" t="s">
+      <c r="W30" s="150" t="s">
         <v>135</v>
       </c>
-      <c r="X30" s="151" t="s">
+      <c r="X30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="AA30" s="144" t="s">
+      <c r="AA30" s="143" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="C31" s="147" t="s">
+      <c r="C31" s="146" t="s">
         <v>164</v>
       </c>
-      <c r="D31" s="147"/>
-      <c r="E31" s="147">
+      <c r="D31" s="146"/>
+      <c r="E31" s="146">
         <v>14978</v>
       </c>
-      <c r="F31" s="147">
+      <c r="F31" s="146">
         <v>6086</v>
       </c>
-      <c r="G31" s="147">
-        <f t="shared" ref="G31:G56" si="8">SUM(E31:F31)</f>
+      <c r="G31" s="146">
+        <f t="shared" ref="G31:G56" si="14">SUM(E31:F31)</f>
         <v>21064</v>
       </c>
-      <c r="H31" s="147"/>
-      <c r="I31" s="147"/>
-      <c r="J31" s="147"/>
-      <c r="K31" s="147"/>
-      <c r="L31" s="147"/>
-      <c r="M31" s="147">
-        <f t="shared" ref="M31:M44" si="9">AVERAGE(G31:I31)</f>
+      <c r="H31" s="146"/>
+      <c r="I31" s="146"/>
+      <c r="J31" s="146"/>
+      <c r="K31" s="146"/>
+      <c r="L31" s="146"/>
+      <c r="M31" s="146">
+        <f t="shared" ref="M31:M44" si="15">AVERAGE(G31:I31)</f>
         <v>21064</v>
       </c>
-      <c r="N31" s="147">
+      <c r="N31" s="146">
         <f>AVERAGE(G31*1.1,J31:K31)</f>
         <v>23170.400000000001</v>
       </c>
-      <c r="O31" s="147">
+      <c r="O31" s="146">
         <f>AVERAGE(G31*0.9,L31)</f>
         <v>18957.600000000002</v>
       </c>
-      <c r="P31" s="152"/>
-      <c r="Q31" s="152"/>
-      <c r="R31" s="152"/>
-      <c r="S31" s="147"/>
-      <c r="T31" s="147"/>
-      <c r="U31" s="147"/>
+      <c r="P31" s="151"/>
+      <c r="Q31" s="151"/>
+      <c r="R31" s="151"/>
+      <c r="S31" s="146"/>
+      <c r="T31" s="146"/>
+      <c r="U31" s="146"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="C32" s="148" t="s">
+      <c r="C32" s="147" t="s">
         <v>165</v>
       </c>
-      <c r="D32" s="148"/>
-      <c r="E32" s="148">
+      <c r="D32" s="147"/>
+      <c r="E32" s="147">
         <v>24338</v>
       </c>
-      <c r="F32" s="148">
+      <c r="F32" s="147">
         <v>6086</v>
       </c>
-      <c r="G32" s="148">
-        <f t="shared" si="8"/>
+      <c r="G32" s="147">
+        <f t="shared" si="14"/>
         <v>30424</v>
       </c>
-      <c r="H32" s="148"/>
-      <c r="I32" s="148"/>
-      <c r="J32" s="148"/>
-      <c r="K32" s="148"/>
-      <c r="L32" s="148"/>
-      <c r="M32" s="148">
-        <f t="shared" si="9"/>
+      <c r="H32" s="147"/>
+      <c r="I32" s="147"/>
+      <c r="J32" s="147"/>
+      <c r="K32" s="147"/>
+      <c r="L32" s="147"/>
+      <c r="M32" s="147">
+        <f t="shared" si="15"/>
         <v>30424</v>
       </c>
-      <c r="N32" s="148">
-        <f t="shared" ref="N32:N57" si="10">AVERAGE(G32*1.1,J32:K32)</f>
+      <c r="N32" s="147">
+        <f t="shared" ref="N32:N57" si="16">AVERAGE(G32*1.1,J32:K32)</f>
         <v>33466.400000000001</v>
       </c>
-      <c r="O32" s="148">
-        <f t="shared" ref="O32:O57" si="11">AVERAGE(G32*0.9,L32)</f>
+      <c r="O32" s="147">
+        <f t="shared" ref="O32:O57" si="17">AVERAGE(G32*0.9,L32)</f>
         <v>27381.600000000002</v>
       </c>
-      <c r="P32" s="153"/>
-      <c r="Q32" s="153"/>
-      <c r="R32" s="153"/>
-      <c r="S32" s="148"/>
-      <c r="T32" s="148"/>
-      <c r="U32" s="148"/>
+      <c r="P32" s="152"/>
+      <c r="Q32" s="152"/>
+      <c r="R32" s="152"/>
+      <c r="S32" s="147"/>
+      <c r="T32" s="147"/>
+      <c r="U32" s="147"/>
     </row>
     <row r="33" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C33" s="148" t="s">
+      <c r="C33" s="147" t="s">
         <v>166</v>
       </c>
-      <c r="D33" s="148"/>
-      <c r="E33" s="148">
+      <c r="D33" s="147"/>
+      <c r="E33" s="147">
         <v>24338</v>
       </c>
-      <c r="F33" s="148">
+      <c r="F33" s="147">
         <v>6086</v>
       </c>
-      <c r="G33" s="148">
-        <f t="shared" si="8"/>
+      <c r="G33" s="147">
+        <f t="shared" si="14"/>
         <v>30424</v>
       </c>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="148"/>
-      <c r="K33" s="148"/>
-      <c r="L33" s="148"/>
-      <c r="M33" s="148">
-        <f t="shared" si="9"/>
+      <c r="H33" s="147"/>
+      <c r="I33" s="147"/>
+      <c r="J33" s="147"/>
+      <c r="K33" s="147"/>
+      <c r="L33" s="147"/>
+      <c r="M33" s="147">
+        <f t="shared" si="15"/>
         <v>30424</v>
       </c>
-      <c r="N33" s="148">
-        <f t="shared" si="10"/>
+      <c r="N33" s="147">
+        <f t="shared" si="16"/>
         <v>33466.400000000001</v>
       </c>
-      <c r="O33" s="148">
-        <f t="shared" si="11"/>
+      <c r="O33" s="147">
+        <f t="shared" si="17"/>
         <v>27381.600000000002</v>
       </c>
-      <c r="P33" s="153"/>
-      <c r="Q33" s="153"/>
-      <c r="R33" s="153"/>
-      <c r="S33" s="148"/>
-      <c r="T33" s="148"/>
-      <c r="U33" s="148"/>
-      <c r="AA33" s="144" t="s">
+      <c r="P33" s="152"/>
+      <c r="Q33" s="152"/>
+      <c r="R33" s="152"/>
+      <c r="S33" s="147"/>
+      <c r="T33" s="147"/>
+      <c r="U33" s="147"/>
+      <c r="AA33" s="143" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="34" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C34" s="148" t="s">
+      <c r="C34" s="147" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="148"/>
-      <c r="E34" s="148">
+      <c r="D34" s="147"/>
+      <c r="E34" s="147">
         <v>26211</v>
       </c>
-      <c r="F34" s="148">
+      <c r="F34" s="147">
         <v>6086</v>
       </c>
-      <c r="G34" s="148">
-        <f t="shared" si="8"/>
+      <c r="G34" s="147">
+        <f t="shared" si="14"/>
         <v>32297</v>
       </c>
-      <c r="H34" s="148"/>
-      <c r="I34" s="148"/>
-      <c r="J34" s="148"/>
-      <c r="K34" s="148"/>
-      <c r="L34" s="148"/>
-      <c r="M34" s="148">
-        <f t="shared" si="9"/>
+      <c r="H34" s="147"/>
+      <c r="I34" s="147"/>
+      <c r="J34" s="147"/>
+      <c r="K34" s="147"/>
+      <c r="L34" s="147"/>
+      <c r="M34" s="147">
+        <f t="shared" si="15"/>
         <v>32297</v>
       </c>
-      <c r="N34" s="148">
-        <f t="shared" si="10"/>
+      <c r="N34" s="147">
+        <f t="shared" si="16"/>
         <v>35526.700000000004</v>
       </c>
-      <c r="O34" s="148">
-        <f t="shared" si="11"/>
+      <c r="O34" s="147">
+        <f t="shared" si="17"/>
         <v>29067.3</v>
       </c>
-      <c r="P34" s="153"/>
-      <c r="Q34" s="153"/>
-      <c r="R34" s="153"/>
-      <c r="S34" s="148"/>
-      <c r="T34" s="148"/>
-      <c r="U34" s="148"/>
+      <c r="P34" s="152"/>
+      <c r="Q34" s="152"/>
+      <c r="R34" s="152"/>
+      <c r="S34" s="147"/>
+      <c r="T34" s="147"/>
+      <c r="U34" s="147"/>
     </row>
     <row r="35" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C35" s="148" t="s">
+      <c r="C35" s="147" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="148"/>
-      <c r="E35" s="148">
+      <c r="D35" s="147"/>
+      <c r="E35" s="147">
         <v>28083</v>
       </c>
-      <c r="F35" s="148">
+      <c r="F35" s="147">
         <v>6086</v>
       </c>
-      <c r="G35" s="148">
-        <f t="shared" si="8"/>
+      <c r="G35" s="147">
+        <f t="shared" si="14"/>
         <v>34169</v>
       </c>
-      <c r="H35" s="148"/>
-      <c r="I35" s="148"/>
-      <c r="J35" s="148"/>
-      <c r="K35" s="148"/>
-      <c r="L35" s="148"/>
-      <c r="M35" s="148">
-        <f t="shared" si="9"/>
+      <c r="H35" s="147"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="147"/>
+      <c r="K35" s="147"/>
+      <c r="L35" s="147"/>
+      <c r="M35" s="147">
+        <f t="shared" si="15"/>
         <v>34169</v>
       </c>
-      <c r="N35" s="148">
-        <f t="shared" si="10"/>
+      <c r="N35" s="147">
+        <f t="shared" si="16"/>
         <v>37585.9</v>
       </c>
-      <c r="O35" s="148">
-        <f t="shared" si="11"/>
+      <c r="O35" s="147">
+        <f t="shared" si="17"/>
         <v>30752.100000000002</v>
       </c>
-      <c r="P35" s="153"/>
-      <c r="Q35" s="153"/>
-      <c r="R35" s="153"/>
-      <c r="S35" s="148"/>
-      <c r="T35" s="148"/>
-      <c r="U35" s="148"/>
+      <c r="P35" s="152"/>
+      <c r="Q35" s="152"/>
+      <c r="R35" s="152"/>
+      <c r="S35" s="147"/>
+      <c r="T35" s="147"/>
+      <c r="U35" s="147"/>
     </row>
     <row r="36" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C36" s="148" t="s">
+      <c r="C36" s="147" t="s">
         <v>169</v>
       </c>
-      <c r="D36" s="148"/>
-      <c r="E36" s="148">
+      <c r="D36" s="147"/>
+      <c r="E36" s="147">
         <v>29955</v>
       </c>
-      <c r="F36" s="148">
+      <c r="F36" s="147">
         <v>6086</v>
       </c>
-      <c r="G36" s="148">
-        <f t="shared" si="8"/>
+      <c r="G36" s="147">
+        <f t="shared" si="14"/>
         <v>36041</v>
       </c>
-      <c r="H36" s="148"/>
-      <c r="I36" s="148"/>
-      <c r="J36" s="148"/>
-      <c r="K36" s="148"/>
-      <c r="L36" s="148"/>
-      <c r="M36" s="148">
-        <f t="shared" si="9"/>
+      <c r="H36" s="147"/>
+      <c r="I36" s="147"/>
+      <c r="J36" s="147"/>
+      <c r="K36" s="147"/>
+      <c r="L36" s="147"/>
+      <c r="M36" s="147">
+        <f t="shared" si="15"/>
         <v>36041</v>
       </c>
-      <c r="N36" s="148">
-        <f t="shared" si="10"/>
+      <c r="N36" s="147">
+        <f t="shared" si="16"/>
         <v>39645.100000000006</v>
       </c>
-      <c r="O36" s="148">
-        <f t="shared" si="11"/>
+      <c r="O36" s="147">
+        <f t="shared" si="17"/>
         <v>32436.9</v>
       </c>
-      <c r="P36" s="153"/>
-      <c r="Q36" s="153"/>
-      <c r="R36" s="153"/>
-      <c r="S36" s="148"/>
-      <c r="T36" s="148"/>
-      <c r="U36" s="148"/>
+      <c r="P36" s="152"/>
+      <c r="Q36" s="152"/>
+      <c r="R36" s="152"/>
+      <c r="S36" s="147"/>
+      <c r="T36" s="147"/>
+      <c r="U36" s="147"/>
     </row>
     <row r="37" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C37" s="149" t="s">
+      <c r="C37" s="148" t="s">
         <v>170</v>
       </c>
-      <c r="D37" s="149"/>
-      <c r="E37" s="149">
+      <c r="D37" s="148"/>
+      <c r="E37" s="148">
         <v>14978</v>
       </c>
-      <c r="F37" s="149">
+      <c r="F37" s="148">
         <v>6086</v>
       </c>
-      <c r="G37" s="149">
-        <f t="shared" si="8"/>
+      <c r="G37" s="148">
+        <f t="shared" si="14"/>
         <v>21064</v>
       </c>
-      <c r="H37" s="149"/>
-      <c r="I37" s="149"/>
-      <c r="J37" s="149"/>
-      <c r="K37" s="149"/>
-      <c r="L37" s="149"/>
-      <c r="M37" s="149">
-        <f t="shared" si="9"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="148"/>
+      <c r="J37" s="148"/>
+      <c r="K37" s="148"/>
+      <c r="L37" s="148"/>
+      <c r="M37" s="148">
+        <f t="shared" si="15"/>
         <v>21064</v>
       </c>
-      <c r="N37" s="149">
-        <f t="shared" si="10"/>
+      <c r="N37" s="148">
+        <f t="shared" si="16"/>
         <v>23170.400000000001</v>
       </c>
-      <c r="O37" s="149">
+      <c r="O37" s="148">
         <f>AVERAGE(G37*0.9,L37)</f>
         <v>18957.600000000002</v>
       </c>
-      <c r="P37" s="154">
+      <c r="P37" s="153">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$8:$AB$10))</f>
         <v>0.5465729349736379</v>
       </c>
-      <c r="Q37" s="154">
+      <c r="Q37" s="153">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$8:$AC$10))</f>
         <v>0.54347826086956519</v>
       </c>
-      <c r="R37" s="154">
+      <c r="R37" s="153">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$8:$AD$10))</f>
         <v>0.54970760233918126</v>
       </c>
-      <c r="S37" s="149">
+      <c r="S37" s="148">
         <f>SUM(D6:D8)/SUM(D6:D13)*M37</f>
         <v>2155.8776533753853</v>
       </c>
-      <c r="T37" s="149">
+      <c r="T37" s="148">
         <f>SUM(E6:E8)/SUM(E6:E13)*N37</f>
         <v>2731.2453287173885</v>
       </c>
-      <c r="U37" s="149">
+      <c r="U37" s="148">
         <f>SUM(F6:F8)/SUM(F6:F13)*O37</f>
         <v>3978.7737999936576</v>
       </c>
-      <c r="V37" s="154">
+      <c r="V37" s="153">
         <f>SUM(D6:D8)/SUM(D6:D13)*P37</f>
         <v>5.5941149660532832E-2</v>
       </c>
-      <c r="W37" s="154">
+      <c r="W37" s="153">
         <f>SUM(E6:E8)/SUM(E6:E13)*Q37</f>
         <v>6.4063307550126458E-2</v>
       </c>
-      <c r="X37" s="154">
+      <c r="X37" s="153">
         <f>SUM(F6:F8)/SUM(F6:F13)*R37</f>
         <v>0.11537126038340646</v>
       </c>
     </row>
     <row r="38" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C38" s="147" t="s">
+      <c r="C38" s="146" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="147"/>
-      <c r="E38" s="147">
+      <c r="D38" s="146"/>
+      <c r="E38" s="146">
         <v>24338</v>
       </c>
-      <c r="F38" s="147">
+      <c r="F38" s="146">
         <v>6086</v>
       </c>
-      <c r="G38" s="147">
-        <f t="shared" si="8"/>
+      <c r="G38" s="146">
+        <f t="shared" si="14"/>
         <v>30424</v>
       </c>
-      <c r="H38" s="147"/>
-      <c r="I38" s="147"/>
-      <c r="J38" s="147"/>
-      <c r="K38" s="147"/>
-      <c r="L38" s="147"/>
-      <c r="M38" s="147">
-        <f t="shared" si="9"/>
+      <c r="H38" s="146"/>
+      <c r="I38" s="146"/>
+      <c r="J38" s="146"/>
+      <c r="K38" s="146"/>
+      <c r="L38" s="146"/>
+      <c r="M38" s="146">
+        <f t="shared" si="15"/>
         <v>30424</v>
       </c>
-      <c r="N38" s="147">
-        <f t="shared" si="10"/>
+      <c r="N38" s="146">
+        <f t="shared" si="16"/>
         <v>33466.400000000001</v>
       </c>
-      <c r="O38" s="147">
-        <f t="shared" si="11"/>
+      <c r="O38" s="146">
+        <f t="shared" si="17"/>
         <v>27381.600000000002</v>
       </c>
-      <c r="P38" s="155">
+      <c r="P38" s="154">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$11:$AB$13))</f>
         <v>0.73124999999999996</v>
       </c>
-      <c r="Q38" s="155">
+      <c r="Q38" s="154">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$11:$AC$13))</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="R38" s="155">
+      <c r="R38" s="154">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$11:$AD$13))</f>
         <v>0.73448275862068968</v>
       </c>
-      <c r="S38" s="147">
+      <c r="S38" s="146">
         <f>SUM(D9)/SUM(D6:D13)*M38</f>
         <v>11432.162401919726</v>
       </c>
-      <c r="T38" s="147">
-        <f t="shared" ref="T38:U38" si="12">SUM(E9)/SUM(E6:E13)*N38</f>
+      <c r="T38" s="146">
+        <f t="shared" ref="T38:U38" si="18">SUM(E9)/SUM(E6:E13)*N38</f>
         <v>11946.208000785055</v>
       </c>
-      <c r="U38" s="147">
-        <f t="shared" si="12"/>
+      <c r="U38" s="146">
+        <f t="shared" si="18"/>
         <v>8171.5871871879508</v>
       </c>
-      <c r="V38" s="155">
+      <c r="V38" s="154">
         <f>SUM(D9)/SUM(D6:D13)*P37</f>
         <v>0.20538096756220545</v>
       </c>
-      <c r="W38" s="155">
-        <f t="shared" ref="W38:X38" si="13">SUM(E9)/SUM(E6:E13)*Q37</f>
+      <c r="W38" s="154">
+        <f t="shared" ref="W38:X38" si="19">SUM(E9)/SUM(E6:E13)*Q37</f>
         <v>0.19400067973408391</v>
       </c>
-      <c r="X38" s="155">
-        <f t="shared" si="13"/>
+      <c r="X38" s="154">
+        <f t="shared" si="19"/>
         <v>0.16405117304959033</v>
       </c>
     </row>
     <row r="39" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C39" s="149" t="s">
+      <c r="C39" s="148" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="149"/>
-      <c r="E39" s="149">
+      <c r="D39" s="148"/>
+      <c r="E39" s="148">
         <v>7489</v>
       </c>
-      <c r="F39" s="149">
+      <c r="F39" s="148">
         <v>5326</v>
       </c>
-      <c r="G39" s="149">
-        <f t="shared" si="8"/>
+      <c r="G39" s="148">
+        <f t="shared" si="14"/>
         <v>12815</v>
       </c>
-      <c r="H39" s="149">
+      <c r="H39" s="148">
         <v>5200</v>
       </c>
-      <c r="I39" s="149"/>
-      <c r="J39" s="149"/>
-      <c r="K39" s="149"/>
-      <c r="L39" s="149"/>
-      <c r="M39" s="149">
+      <c r="I39" s="148"/>
+      <c r="J39" s="148"/>
+      <c r="K39" s="148"/>
+      <c r="L39" s="148"/>
+      <c r="M39" s="148">
         <f>AVERAGE(G39:I39)</f>
         <v>9007.5</v>
       </c>
-      <c r="N39" s="149">
-        <f t="shared" si="10"/>
+      <c r="N39" s="148">
+        <f t="shared" si="16"/>
         <v>14096.500000000002</v>
       </c>
-      <c r="O39" s="149">
+      <c r="O39" s="148">
         <f>AVERAGE(G39*0.9,L39)</f>
         <v>11533.5</v>
       </c>
-      <c r="P39" s="154">
+      <c r="P39" s="153">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$11:$AB$13))</f>
         <v>0.40729166666666661</v>
       </c>
-      <c r="Q39" s="154">
+      <c r="Q39" s="153">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$11:$AC$13))</f>
         <v>0.40259740259740262</v>
       </c>
-      <c r="R39" s="154">
+      <c r="R39" s="153">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$11:$AD$13))</f>
         <v>0.41034482758620683</v>
       </c>
-      <c r="S39" s="149">
+      <c r="S39" s="148">
         <f>D9/SUM(D6:D13)*M39</f>
         <v>3384.6700905631055</v>
       </c>
-      <c r="T39" s="149">
+      <c r="T39" s="148">
         <f>E9/SUM(E6:E13)*N39</f>
         <v>5031.9042706435866</v>
       </c>
-      <c r="U39" s="149">
+      <c r="U39" s="148">
         <f>F9/SUM(F6:F13)*O39</f>
         <v>3441.9829675195106</v>
       </c>
-      <c r="V39" s="154">
+      <c r="V39" s="153">
         <f>D9/SUM(D6:D13)*P39</f>
         <v>0.15304445432165026</v>
       </c>
-      <c r="W39" s="154">
-        <f t="shared" ref="W39:X39" si="14">E9/SUM(E6:E13)*Q39</f>
+      <c r="W39" s="153">
+        <f t="shared" ref="W39:X39" si="20">E9/SUM(E6:E13)*Q39</f>
         <v>0.14371167236405388</v>
       </c>
-      <c r="X39" s="154">
+      <c r="X39" s="153">
+        <f t="shared" si="20"/>
+        <v>0.12246065005084789</v>
+      </c>
+    </row>
+    <row r="40" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="C40" s="147" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="147"/>
+      <c r="E40" s="147">
+        <v>24338</v>
+      </c>
+      <c r="F40" s="147">
+        <v>6086</v>
+      </c>
+      <c r="G40" s="147">
         <f t="shared" si="14"/>
-        <v>0.12246065005084789</v>
-      </c>
-    </row>
-    <row r="40" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C40" s="148" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="148"/>
-      <c r="E40" s="148">
-        <v>24338</v>
-      </c>
-      <c r="F40" s="148">
-        <v>6086</v>
-      </c>
-      <c r="G40" s="148">
-        <f t="shared" si="8"/>
         <v>30424</v>
       </c>
-      <c r="H40" s="148"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="148"/>
-      <c r="K40" s="148"/>
-      <c r="L40" s="148"/>
-      <c r="M40" s="148">
-        <f t="shared" si="9"/>
+      <c r="H40" s="147"/>
+      <c r="I40" s="147"/>
+      <c r="J40" s="147"/>
+      <c r="K40" s="147"/>
+      <c r="L40" s="147"/>
+      <c r="M40" s="147">
+        <f t="shared" si="15"/>
         <v>30424</v>
       </c>
-      <c r="N40" s="148">
-        <f t="shared" si="10"/>
+      <c r="N40" s="147">
+        <f t="shared" si="16"/>
         <v>33466.400000000001</v>
       </c>
-      <c r="O40" s="148">
-        <f t="shared" si="11"/>
+      <c r="O40" s="147">
+        <f t="shared" si="17"/>
         <v>27381.600000000002</v>
       </c>
-      <c r="P40" s="156">
+      <c r="P40" s="155">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$14:$AB$15))</f>
         <v>0.81702127659574475</v>
       </c>
-      <c r="Q40" s="156">
+      <c r="Q40" s="155">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$14:$AC$15))</f>
         <v>0.81578947368421051</v>
       </c>
-      <c r="R40" s="156">
+      <c r="R40" s="155">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$14:$AD$15))</f>
         <v>0.81666666666666665</v>
       </c>
-      <c r="S40" s="148"/>
-      <c r="T40" s="148"/>
-      <c r="U40" s="148"/>
+      <c r="S40" s="147"/>
+      <c r="T40" s="147"/>
+      <c r="U40" s="147"/>
     </row>
     <row r="41" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C41" s="147" t="s">
+      <c r="C41" s="146" t="s">
         <v>174</v>
       </c>
-      <c r="D41" s="147"/>
-      <c r="E41" s="147">
+      <c r="D41" s="146"/>
+      <c r="E41" s="146">
         <v>7489</v>
       </c>
-      <c r="F41" s="147">
+      <c r="F41" s="146">
         <v>5326</v>
       </c>
-      <c r="G41" s="147">
-        <f t="shared" si="8"/>
+      <c r="G41" s="146">
+        <f t="shared" si="14"/>
         <v>12815</v>
       </c>
-      <c r="H41" s="147"/>
-      <c r="I41" s="147"/>
-      <c r="J41" s="147"/>
-      <c r="K41" s="147"/>
-      <c r="L41" s="147"/>
-      <c r="M41" s="147">
-        <f t="shared" si="9"/>
+      <c r="H41" s="146"/>
+      <c r="I41" s="146"/>
+      <c r="J41" s="146"/>
+      <c r="K41" s="146"/>
+      <c r="L41" s="146"/>
+      <c r="M41" s="146">
+        <f t="shared" si="15"/>
         <v>12815</v>
       </c>
-      <c r="N41" s="147">
-        <f t="shared" si="10"/>
+      <c r="N41" s="146">
+        <f t="shared" si="16"/>
         <v>14096.500000000002</v>
       </c>
-      <c r="O41" s="147">
-        <f t="shared" si="11"/>
+      <c r="O41" s="146">
+        <f t="shared" si="17"/>
         <v>11533.5</v>
       </c>
-      <c r="P41" s="155">
+      <c r="P41" s="154">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$14:$AB$15))</f>
         <v>0.59645390070921978</v>
       </c>
-      <c r="Q41" s="155">
+      <c r="Q41" s="154">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$14:$AC$15))</f>
         <v>0.59649122807017552</v>
       </c>
-      <c r="R41" s="155">
+      <c r="R41" s="154">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$14:$AD$15))</f>
         <v>0.59285714285714286</v>
       </c>
-      <c r="S41" s="147">
+      <c r="S41" s="146">
         <f>SUM(D10)/SUM(D6:D13)*M41</f>
         <v>3202.1646884279426</v>
       </c>
-      <c r="T41" s="147">
-        <f t="shared" ref="T41:U41" si="15">SUM(E10)/SUM(E6:E13)*N41</f>
+      <c r="T41" s="146">
+        <f t="shared" ref="T41:U41" si="21">SUM(E10)/SUM(E6:E13)*N41</f>
         <v>3337.0202528302325</v>
       </c>
-      <c r="U41" s="147">
-        <f t="shared" si="15"/>
+      <c r="U41" s="146">
+        <f t="shared" si="21"/>
         <v>2555.819902348102</v>
       </c>
-      <c r="V41" s="155">
+      <c r="V41" s="154">
         <f>SUM(D10)/SUM(D6:D13)*P41</f>
         <v>0.14903968935826528</v>
       </c>
-      <c r="W41" s="155">
-        <f t="shared" ref="W41:X41" si="16">SUM(E10)/SUM(E6:E13)*Q41</f>
+      <c r="W41" s="154">
+        <f t="shared" ref="W41:X41" si="22">SUM(E10)/SUM(E6:E13)*Q41</f>
         <v>0.14120549843619004</v>
       </c>
-      <c r="X41" s="155">
+      <c r="X41" s="154">
+        <f t="shared" si="22"/>
+        <v>0.13137695278653641</v>
+      </c>
+    </row>
+    <row r="42" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="C42" s="148" t="s">
+        <v>175</v>
+      </c>
+      <c r="D42" s="148"/>
+      <c r="E42" s="148">
+        <v>3744</v>
+      </c>
+      <c r="F42" s="148">
+        <v>4565</v>
+      </c>
+      <c r="G42" s="148">
+        <f t="shared" si="14"/>
+        <v>8309</v>
+      </c>
+      <c r="H42" s="148">
+        <v>5000</v>
+      </c>
+      <c r="I42" s="148">
+        <v>9300</v>
+      </c>
+      <c r="J42" s="148">
+        <v>30000</v>
+      </c>
+      <c r="K42" s="148"/>
+      <c r="L42" s="148"/>
+      <c r="M42" s="148">
+        <f t="shared" si="15"/>
+        <v>7536.333333333333</v>
+      </c>
+      <c r="N42" s="148">
         <f t="shared" si="16"/>
-        <v>0.13137695278653641</v>
-      </c>
-    </row>
-    <row r="42" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C42" s="149" t="s">
-        <v>175</v>
-      </c>
-      <c r="D42" s="149"/>
-      <c r="E42" s="149">
-        <v>3744</v>
-      </c>
-      <c r="F42" s="149">
-        <v>4565</v>
-      </c>
-      <c r="G42" s="149">
-        <f t="shared" si="8"/>
-        <v>8309</v>
-      </c>
-      <c r="H42" s="149">
-        <v>5000</v>
-      </c>
-      <c r="I42" s="149">
-        <v>9300</v>
-      </c>
-      <c r="J42" s="149">
-        <v>30000</v>
-      </c>
-      <c r="K42" s="149"/>
-      <c r="L42" s="149"/>
-      <c r="M42" s="149">
-        <f t="shared" si="9"/>
-        <v>7536.333333333333</v>
-      </c>
-      <c r="N42" s="149">
-        <f t="shared" si="10"/>
         <v>19569.95</v>
       </c>
-      <c r="O42" s="149">
-        <f t="shared" si="11"/>
+      <c r="O42" s="148">
+        <f t="shared" si="17"/>
         <v>7478.1</v>
       </c>
-      <c r="P42" s="154">
+      <c r="P42" s="153">
         <f>1-(AVERAGE(AB11:AB13)/AVERAGE($AB$14:$AB$15))</f>
         <v>0.31914893617021278</v>
       </c>
-      <c r="Q42" s="154">
+      <c r="Q42" s="153">
         <f>1-(AVERAGE(AC11:AC13)/AVERAGE($AC$14:$AC$15))</f>
         <v>0.32456140350877194</v>
       </c>
-      <c r="R42" s="154">
+      <c r="R42" s="153">
         <f>1-(AVERAGE(AD11:AD13)/AVERAGE($AD$14:$AD$15))</f>
         <v>0.30952380952380953</v>
       </c>
-      <c r="S42" s="149">
+      <c r="S42" s="148">
         <f>D10/SUM(D6:D13)*M42</f>
         <v>1883.1510324012836</v>
       </c>
-      <c r="T42" s="149">
+      <c r="T42" s="148">
         <f>E10/SUM(E6:E13)*N42</f>
         <v>4632.7329122033843</v>
       </c>
-      <c r="U42" s="149">
+      <c r="U42" s="148">
         <f>F10/SUM(F6:F13)*O42</f>
         <v>1657.1445625134904</v>
       </c>
-      <c r="V42" s="154">
+      <c r="V42" s="153">
         <f>D10/SUM(D6:D13)*P42</f>
         <v>7.9747752926539114E-2</v>
       </c>
-      <c r="W42" s="154">
-        <f t="shared" ref="W42:X42" si="17">E10/SUM(E6:E13)*Q42</f>
+      <c r="W42" s="153">
+        <f t="shared" ref="W42:X42" si="23">E10/SUM(E6:E13)*Q42</f>
         <v>7.6832403560868096E-2</v>
       </c>
-      <c r="X42" s="154">
+      <c r="X42" s="153">
+        <f t="shared" si="23"/>
+        <v>6.8590376956826238E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="C43" s="147" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43" s="147"/>
+      <c r="E43" s="147">
+        <v>26211</v>
+      </c>
+      <c r="F43" s="147">
+        <v>6086</v>
+      </c>
+      <c r="G43" s="147">
+        <f t="shared" si="14"/>
+        <v>32297</v>
+      </c>
+      <c r="H43" s="147"/>
+      <c r="I43" s="147"/>
+      <c r="J43" s="147"/>
+      <c r="K43" s="147"/>
+      <c r="L43" s="147"/>
+      <c r="M43" s="147">
+        <f t="shared" si="15"/>
+        <v>32297</v>
+      </c>
+      <c r="N43" s="147">
+        <f t="shared" si="16"/>
+        <v>35526.700000000004</v>
+      </c>
+      <c r="O43" s="147">
         <f t="shared" si="17"/>
-        <v>6.8590376956826238E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C43" s="148" t="s">
-        <v>176</v>
-      </c>
-      <c r="D43" s="148"/>
-      <c r="E43" s="148">
-        <v>26211</v>
-      </c>
-      <c r="F43" s="148">
-        <v>6086</v>
-      </c>
-      <c r="G43" s="148">
-        <f t="shared" si="8"/>
-        <v>32297</v>
-      </c>
-      <c r="H43" s="148"/>
-      <c r="I43" s="148"/>
-      <c r="J43" s="148"/>
-      <c r="K43" s="148"/>
-      <c r="L43" s="148"/>
-      <c r="M43" s="148">
-        <f t="shared" si="9"/>
-        <v>32297</v>
-      </c>
-      <c r="N43" s="148">
-        <f t="shared" si="10"/>
-        <v>35526.700000000004</v>
-      </c>
-      <c r="O43" s="148">
-        <f t="shared" si="11"/>
         <v>29067.3</v>
       </c>
-      <c r="P43" s="156">
+      <c r="P43" s="155">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$16:$AB$17))</f>
         <v>0.8612903225806452</v>
       </c>
-      <c r="Q43" s="156">
+      <c r="Q43" s="155">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$16:$AC$17))</f>
         <v>0.86</v>
       </c>
-      <c r="R43" s="156">
+      <c r="R43" s="155">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$16:$AD$17))</f>
         <v>0.86491228070175441</v>
       </c>
-      <c r="S43" s="148"/>
-      <c r="T43" s="148"/>
-      <c r="U43" s="148"/>
+      <c r="S43" s="147"/>
+      <c r="T43" s="147"/>
+      <c r="U43" s="147"/>
     </row>
     <row r="44" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C44" s="147" t="s">
+      <c r="C44" s="146" t="s">
         <v>177</v>
       </c>
-      <c r="D44" s="147"/>
-      <c r="E44" s="147">
+      <c r="D44" s="146"/>
+      <c r="E44" s="146">
         <v>14978</v>
       </c>
-      <c r="F44" s="147">
+      <c r="F44" s="146">
         <v>5326</v>
       </c>
-      <c r="G44" s="147">
-        <f t="shared" si="8"/>
+      <c r="G44" s="146">
+        <f t="shared" si="14"/>
         <v>20304</v>
       </c>
-      <c r="H44" s="147"/>
-      <c r="I44" s="147"/>
-      <c r="J44" s="147"/>
-      <c r="K44" s="147"/>
-      <c r="L44" s="147"/>
-      <c r="M44" s="147">
-        <f t="shared" si="9"/>
+      <c r="H44" s="146"/>
+      <c r="I44" s="146"/>
+      <c r="J44" s="146"/>
+      <c r="K44" s="146"/>
+      <c r="L44" s="146"/>
+      <c r="M44" s="146">
+        <f t="shared" si="15"/>
         <v>20304</v>
       </c>
-      <c r="N44" s="147">
-        <f t="shared" si="10"/>
+      <c r="N44" s="146">
+        <f t="shared" si="16"/>
         <v>22334.400000000001</v>
       </c>
-      <c r="O44" s="147">
-        <f t="shared" si="11"/>
+      <c r="O44" s="146">
+        <f t="shared" si="17"/>
         <v>18273.600000000002</v>
       </c>
-      <c r="P44" s="155">
+      <c r="P44" s="154">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$16:$AB$17))</f>
         <v>0.69408602150537635</v>
       </c>
-      <c r="Q44" s="155">
+      <c r="Q44" s="154">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$16:$AC$17))</f>
         <v>0.69333333333333336</v>
       </c>
-      <c r="R44" s="155">
+      <c r="R44" s="154">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$16:$AD$17))</f>
         <v>0.7</v>
       </c>
-      <c r="S44" s="147">
+      <c r="S44" s="146">
         <f>SUM(D11)/SUM(D6:D13)*M44</f>
         <v>2742.3958967170497</v>
       </c>
-      <c r="T44" s="147">
-        <f t="shared" ref="T44:U44" si="18">SUM(E11)/SUM(E6:E13)*N44</f>
+      <c r="T44" s="146">
+        <f t="shared" ref="T44:U44" si="24">SUM(E11)/SUM(E6:E13)*N44</f>
         <v>2582.1231033841427</v>
       </c>
-      <c r="U44" s="147">
-        <f t="shared" si="18"/>
+      <c r="U44" s="146">
+        <f t="shared" si="24"/>
         <v>2385.6110070402383</v>
       </c>
-      <c r="V44" s="155">
+      <c r="V44" s="154">
         <f>SUM(D11)/SUM(D6:D13)*P44</f>
         <v>9.3747963817228427E-2</v>
       </c>
-      <c r="W44" s="155">
-        <f t="shared" ref="W44:X44" si="19">SUM(E11)/SUM(E6:E13)*Q44</f>
+      <c r="W44" s="154">
+        <f t="shared" ref="W44:X44" si="25">SUM(E11)/SUM(E6:E13)*Q44</f>
         <v>8.0157605234362189E-2</v>
       </c>
-      <c r="X44" s="155">
-        <f t="shared" si="19"/>
+      <c r="X44" s="154">
+        <f t="shared" si="25"/>
         <v>9.1384713736109291E-2</v>
       </c>
     </row>
     <row r="45" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C45" s="148" t="s">
+      <c r="C45" s="147" t="s">
         <v>178</v>
       </c>
-      <c r="D45" s="148"/>
-      <c r="E45" s="148">
+      <c r="D45" s="147"/>
+      <c r="E45" s="147">
         <v>9361</v>
       </c>
-      <c r="F45" s="148">
+      <c r="F45" s="147">
         <v>4565</v>
       </c>
-      <c r="G45" s="148">
-        <f t="shared" si="8"/>
+      <c r="G45" s="147">
+        <f t="shared" si="14"/>
         <v>13926</v>
       </c>
-      <c r="H45" s="148">
+      <c r="H45" s="147">
         <f>H46+12600</f>
         <v>24800</v>
       </c>
-      <c r="I45" s="148"/>
-      <c r="J45" s="148"/>
-      <c r="K45" s="148">
+      <c r="I45" s="147"/>
+      <c r="J45" s="147"/>
+      <c r="K45" s="147">
         <v>15500</v>
       </c>
-      <c r="L45" s="148"/>
-      <c r="M45" s="148">
-        <f t="shared" ref="M45:M57" si="20">AVERAGE(G45:I45)</f>
+      <c r="L45" s="147"/>
+      <c r="M45" s="147">
+        <f t="shared" ref="M45:M57" si="26">AVERAGE(G45:I45)</f>
         <v>19363</v>
       </c>
-      <c r="N45" s="148">
-        <f t="shared" si="10"/>
+      <c r="N45" s="147">
+        <f t="shared" si="16"/>
         <v>15409.3</v>
       </c>
-      <c r="O45" s="148">
-        <f t="shared" si="11"/>
+      <c r="O45" s="147">
+        <f t="shared" si="17"/>
         <v>12533.4</v>
       </c>
-      <c r="P45" s="156">
+      <c r="P45" s="155">
         <f>1-(AVERAGE(AB11:AB13)/AVERAGE($AB$16:$AB$17))</f>
         <v>0.4838709677419355</v>
       </c>
-      <c r="Q45" s="156">
+      <c r="Q45" s="155">
         <f>1-(AVERAGE(AC11:AC13)/AVERAGE($AC$16:$AC$17))</f>
         <v>0.48666666666666669</v>
       </c>
-      <c r="R45" s="156">
+      <c r="R45" s="155">
         <f>1-(AVERAGE(AD11:AD13)/AVERAGE($AD$16:$AD$17))</f>
         <v>0.49122807017543857</v>
       </c>
-      <c r="S45" s="148"/>
-      <c r="T45" s="148"/>
-      <c r="U45" s="148"/>
+      <c r="S45" s="147"/>
+      <c r="T45" s="147"/>
+      <c r="U45" s="147"/>
     </row>
     <row r="46" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C46" s="149" t="s">
+      <c r="C46" s="148" t="s">
         <v>179</v>
       </c>
-      <c r="D46" s="149"/>
-      <c r="E46" s="149">
+      <c r="D46" s="148"/>
+      <c r="E46" s="148">
         <v>9361</v>
       </c>
-      <c r="F46" s="149">
+      <c r="F46" s="148">
         <v>3804</v>
       </c>
-      <c r="G46" s="149">
-        <f t="shared" si="8"/>
+      <c r="G46" s="148">
+        <f t="shared" si="14"/>
         <v>13165</v>
       </c>
-      <c r="H46" s="149">
+      <c r="H46" s="148">
         <v>12200</v>
       </c>
-      <c r="I46" s="149"/>
-      <c r="J46" s="149">
+      <c r="I46" s="148"/>
+      <c r="J46" s="148">
         <v>14000</v>
       </c>
-      <c r="K46" s="149">
+      <c r="K46" s="148">
         <v>2000</v>
       </c>
-      <c r="L46" s="149"/>
-      <c r="M46" s="149">
-        <f t="shared" si="20"/>
+      <c r="L46" s="148"/>
+      <c r="M46" s="148">
+        <f t="shared" si="26"/>
         <v>12682.5</v>
       </c>
-      <c r="N46" s="149">
-        <f t="shared" si="10"/>
+      <c r="N46" s="148">
+        <f t="shared" si="16"/>
         <v>10160.5</v>
       </c>
-      <c r="O46" s="149">
-        <f t="shared" si="11"/>
+      <c r="O46" s="148">
+        <f t="shared" si="17"/>
         <v>11848.5</v>
       </c>
-      <c r="P46" s="154">
+      <c r="P46" s="153">
         <f>1-(AVERAGE(AB14:AB15)/AVERAGE($AB$16:$AB$17))</f>
         <v>0.24193548387096775</v>
       </c>
-      <c r="Q46" s="154">
+      <c r="Q46" s="153">
         <f>1-(AVERAGE(AC14:AC15)/AVERAGE($AC$16:$AC$17))</f>
         <v>0.24</v>
       </c>
-      <c r="R46" s="154">
+      <c r="R46" s="153">
         <f>1-(AVERAGE(AD14:AD15)/AVERAGE($AD$16:$AD$17))</f>
         <v>0.26315789473684215</v>
       </c>
-      <c r="S46" s="149">
+      <c r="S46" s="148">
         <f>D11/SUM(D6:D13)*M46</f>
         <v>1712.9844345997824</v>
       </c>
-      <c r="T46" s="149">
+      <c r="T46" s="148">
         <f>E11/SUM(E6:E13)*N46</f>
         <v>1174.67502113039</v>
       </c>
-      <c r="U46" s="149">
+      <c r="U46" s="148">
         <f>F11/SUM(F6:F13)*O46</f>
         <v>1546.8168295747014</v>
       </c>
-      <c r="V46" s="154">
+      <c r="V46" s="153">
         <f>D11/SUM(D6:D13)*P46</f>
         <v>3.2677446721729508E-2</v>
       </c>
-      <c r="W46" s="154">
-        <f t="shared" ref="W46:X46" si="21">E11/SUM(E6:E13)*Q46</f>
+      <c r="W46" s="153">
+        <f t="shared" ref="W46:X46" si="27">E11/SUM(E6:E13)*Q46</f>
         <v>2.774686335035614E-2</v>
       </c>
-      <c r="X46" s="154">
-        <f t="shared" si="21"/>
+      <c r="X46" s="153">
+        <f t="shared" si="27"/>
         <v>3.4355155539890714E-2</v>
       </c>
     </row>
     <row r="47" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C47" s="148" t="s">
+      <c r="C47" s="147" t="s">
         <v>180</v>
       </c>
-      <c r="D47" s="148"/>
-      <c r="E47" s="148">
+      <c r="D47" s="147"/>
+      <c r="E47" s="147">
         <v>28083</v>
       </c>
-      <c r="F47" s="148">
+      <c r="F47" s="147">
         <v>6086</v>
       </c>
-      <c r="G47" s="148">
-        <f t="shared" si="8"/>
+      <c r="G47" s="147">
+        <f t="shared" si="14"/>
         <v>34169</v>
       </c>
-      <c r="H47" s="148"/>
-      <c r="I47" s="148"/>
-      <c r="J47" s="148"/>
-      <c r="K47" s="148"/>
-      <c r="L47" s="148"/>
-      <c r="M47" s="148">
-        <f t="shared" si="20"/>
+      <c r="H47" s="147"/>
+      <c r="I47" s="147"/>
+      <c r="J47" s="147"/>
+      <c r="K47" s="147"/>
+      <c r="L47" s="147"/>
+      <c r="M47" s="147">
+        <f t="shared" si="26"/>
         <v>34169</v>
       </c>
-      <c r="N47" s="148">
-        <f t="shared" si="10"/>
+      <c r="N47" s="147">
+        <f t="shared" si="16"/>
         <v>37585.9</v>
       </c>
-      <c r="O47" s="148">
-        <f t="shared" si="11"/>
+      <c r="O47" s="147">
+        <f t="shared" si="17"/>
         <v>30752.100000000002</v>
       </c>
-      <c r="P47" s="156">
+      <c r="P47" s="155">
         <f>1-(AVERAGE(AB5:AB7)/$AB$18)</f>
         <v>0.89113924050632909</v>
       </c>
-      <c r="Q47" s="156">
+      <c r="Q47" s="155">
         <f>1-(AVERAGE(AC5:AC7)/$AC$18)</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="R47" s="156">
+      <c r="R47" s="155">
         <f>1-(AVERAGE(AD5:AD7)/$AD$18)</f>
         <v>0.89305555555555549</v>
       </c>
-      <c r="S47" s="148"/>
-      <c r="T47" s="148"/>
-      <c r="U47" s="148"/>
+      <c r="S47" s="147"/>
+      <c r="T47" s="147"/>
+      <c r="U47" s="147"/>
     </row>
     <row r="48" spans="3:27" x14ac:dyDescent="0.2">
-      <c r="C48" s="147" t="s">
+      <c r="C48" s="146" t="s">
         <v>181</v>
       </c>
-      <c r="D48" s="147"/>
-      <c r="E48" s="147">
+      <c r="D48" s="146"/>
+      <c r="E48" s="146">
         <v>16850</v>
       </c>
-      <c r="F48" s="147">
+      <c r="F48" s="146">
         <v>5326</v>
       </c>
-      <c r="G48" s="147">
-        <f t="shared" si="8"/>
+      <c r="G48" s="146">
+        <f t="shared" si="14"/>
         <v>22176</v>
       </c>
-      <c r="H48" s="147"/>
-      <c r="I48" s="147"/>
-      <c r="J48" s="147"/>
-      <c r="K48" s="147"/>
-      <c r="L48" s="147"/>
-      <c r="M48" s="147">
-        <f t="shared" si="20"/>
+      <c r="H48" s="146"/>
+      <c r="I48" s="146"/>
+      <c r="J48" s="146"/>
+      <c r="K48" s="146"/>
+      <c r="L48" s="146"/>
+      <c r="M48" s="146">
+        <f t="shared" si="26"/>
         <v>22176</v>
       </c>
-      <c r="N48" s="147">
-        <f t="shared" si="10"/>
+      <c r="N48" s="146">
+        <f t="shared" si="16"/>
         <v>24393.600000000002</v>
       </c>
-      <c r="O48" s="147">
-        <f t="shared" si="11"/>
+      <c r="O48" s="146">
+        <f t="shared" si="17"/>
         <v>19958.400000000001</v>
       </c>
-      <c r="P48" s="155">
+      <c r="P48" s="154">
         <f>1-(AVERAGE(AB8:AB10)/$AB$18)</f>
         <v>0.75991561181434597</v>
       </c>
-      <c r="Q48" s="155">
+      <c r="Q48" s="154">
         <f>1-(AVERAGE(AC8:AC10)/$AC$18)</f>
         <v>0.75661375661375663</v>
       </c>
-      <c r="R48" s="155">
+      <c r="R48" s="154">
         <f>1-(AVERAGE(AD8:AD10)/$AD$18)</f>
         <v>0.76249999999999996</v>
       </c>
-      <c r="S48" s="147">
+      <c r="S48" s="146">
         <f>SUM(D12)/SUM(D6:D13)*M48</f>
         <v>1480.3244787616509</v>
       </c>
-      <c r="T48" s="147">
-        <f t="shared" ref="T48:U48" si="22">SUM(E12)/SUM(E6:E13)*N48</f>
+      <c r="T48" s="146">
+        <f t="shared" ref="T48:U48" si="28">SUM(E12)/SUM(E6:E13)*N48</f>
         <v>1498.1922676437027</v>
       </c>
-      <c r="U48" s="147">
-        <f t="shared" si="22"/>
+      <c r="U48" s="146">
+        <f t="shared" si="28"/>
         <v>1246.8867413583491</v>
       </c>
-      <c r="V48" s="155">
+      <c r="V48" s="154">
         <f>SUM(D12)/SUM(D6:D13)*P48</f>
         <v>5.0726987822957821E-2</v>
       </c>
-      <c r="W48" s="155">
-        <f t="shared" ref="W48:X48" si="23">SUM(E12)/SUM(E6:E13)*Q48</f>
+      <c r="W48" s="154">
+        <f t="shared" ref="W48:X48" si="29">SUM(E12)/SUM(E6:E13)*Q48</f>
         <v>4.6469273897726641E-2</v>
       </c>
-      <c r="X48" s="155">
-        <f t="shared" si="23"/>
+      <c r="X48" s="154">
+        <f t="shared" si="29"/>
         <v>4.7636641228041378E-2</v>
       </c>
     </row>
     <row r="49" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C49" s="148" t="s">
+      <c r="C49" s="147" t="s">
         <v>182</v>
       </c>
-      <c r="D49" s="148"/>
-      <c r="E49" s="148">
+      <c r="D49" s="147"/>
+      <c r="E49" s="147">
         <v>11233</v>
       </c>
-      <c r="F49" s="148">
+      <c r="F49" s="147">
         <v>4565</v>
       </c>
-      <c r="G49" s="148">
-        <f t="shared" si="8"/>
+      <c r="G49" s="147">
+        <f t="shared" si="14"/>
         <v>15798</v>
       </c>
-      <c r="H49" s="148">
+      <c r="H49" s="147">
         <v>11000</v>
       </c>
-      <c r="I49" s="148"/>
-      <c r="J49" s="148">
+      <c r="I49" s="147"/>
+      <c r="J49" s="147">
         <f>J50+16375</f>
         <v>35375</v>
       </c>
-      <c r="K49" s="148"/>
-      <c r="L49" s="148"/>
-      <c r="M49" s="148">
-        <f t="shared" si="20"/>
+      <c r="K49" s="147"/>
+      <c r="L49" s="147"/>
+      <c r="M49" s="147">
+        <f t="shared" si="26"/>
         <v>13399</v>
       </c>
-      <c r="N49" s="148">
-        <f t="shared" si="10"/>
+      <c r="N49" s="147">
+        <f t="shared" si="16"/>
         <v>26376.400000000001</v>
       </c>
-      <c r="O49" s="148">
-        <f t="shared" si="11"/>
+      <c r="O49" s="147">
+        <f t="shared" si="17"/>
         <v>14218.2</v>
       </c>
-      <c r="P49" s="156">
+      <c r="P49" s="155">
         <f>1-(AVERAGE(AB11:AB13)/$AB$18)</f>
         <v>0.59493670886075956</v>
       </c>
-      <c r="Q49" s="156">
+      <c r="Q49" s="155">
         <f>1-(AVERAGE(AC11:AC13)/$AC$18)</f>
         <v>0.59259259259259256</v>
       </c>
-      <c r="R49" s="156">
+      <c r="R49" s="155">
         <f>1-(AVERAGE(AD11:AD13)/$AD$18)</f>
         <v>0.59722222222222232</v>
       </c>
-      <c r="S49" s="148"/>
-      <c r="T49" s="148"/>
-      <c r="U49" s="148"/>
+      <c r="S49" s="147"/>
+      <c r="T49" s="147"/>
+      <c r="U49" s="147"/>
     </row>
     <row r="50" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C50" s="148" t="s">
+      <c r="C50" s="147" t="s">
         <v>183</v>
       </c>
-      <c r="D50" s="148"/>
-      <c r="E50" s="148">
+      <c r="D50" s="147"/>
+      <c r="E50" s="147">
         <v>7489</v>
       </c>
-      <c r="F50" s="148">
+      <c r="F50" s="147">
         <v>3804</v>
       </c>
-      <c r="G50" s="148">
-        <f t="shared" si="8"/>
+      <c r="G50" s="147">
+        <f t="shared" si="14"/>
         <v>11293</v>
       </c>
-      <c r="H50" s="148">
+      <c r="H50" s="147">
         <v>9000</v>
       </c>
-      <c r="I50" s="148"/>
-      <c r="J50" s="148">
+      <c r="I50" s="147"/>
+      <c r="J50" s="147">
         <v>19000</v>
       </c>
-      <c r="K50" s="148"/>
-      <c r="L50" s="148"/>
-      <c r="M50" s="148">
-        <f t="shared" si="20"/>
+      <c r="K50" s="147"/>
+      <c r="L50" s="147"/>
+      <c r="M50" s="147">
+        <f t="shared" si="26"/>
         <v>10146.5</v>
       </c>
-      <c r="N50" s="148">
-        <f t="shared" si="10"/>
+      <c r="N50" s="147">
+        <f t="shared" si="16"/>
         <v>15711.150000000001</v>
       </c>
-      <c r="O50" s="148">
-        <f t="shared" si="11"/>
+      <c r="O50" s="147">
+        <f t="shared" si="17"/>
         <v>10163.700000000001</v>
       </c>
-      <c r="P50" s="156">
+      <c r="P50" s="155">
         <f>1-(AVERAGE(AB14:AB15)/$AB$18)</f>
         <v>0.40506329113924056</v>
       </c>
-      <c r="Q50" s="156">
+      <c r="Q50" s="155">
         <f>1-(AVERAGE(AC14:AC15)/$AC$18)</f>
         <v>0.39682539682539686</v>
       </c>
-      <c r="R50" s="156">
+      <c r="R50" s="155">
         <f>1-(AVERAGE(AD14:AD15)/$AD$18)</f>
         <v>0.41666666666666663</v>
       </c>
-      <c r="S50" s="148"/>
-      <c r="T50" s="148"/>
-      <c r="U50" s="148"/>
+      <c r="S50" s="147"/>
+      <c r="T50" s="147"/>
+      <c r="U50" s="147"/>
     </row>
     <row r="51" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C51" s="149" t="s">
+      <c r="C51" s="148" t="s">
         <v>184</v>
       </c>
-      <c r="D51" s="149"/>
-      <c r="E51" s="149">
+      <c r="D51" s="148"/>
+      <c r="E51" s="148">
         <v>5617</v>
       </c>
-      <c r="F51" s="149">
+      <c r="F51" s="148">
         <v>3043</v>
       </c>
-      <c r="G51" s="149">
-        <f t="shared" si="8"/>
+      <c r="G51" s="148">
+        <f t="shared" si="14"/>
         <v>8660</v>
       </c>
-      <c r="H51" s="149">
+      <c r="H51" s="148">
         <v>1000</v>
       </c>
-      <c r="I51" s="149"/>
-      <c r="J51" s="149"/>
-      <c r="K51" s="149"/>
-      <c r="L51" s="149"/>
-      <c r="M51" s="149">
-        <f t="shared" si="20"/>
+      <c r="I51" s="148"/>
+      <c r="J51" s="148"/>
+      <c r="K51" s="148"/>
+      <c r="L51" s="148"/>
+      <c r="M51" s="148">
+        <f t="shared" si="26"/>
         <v>4830</v>
       </c>
-      <c r="N51" s="149">
-        <f t="shared" si="10"/>
+      <c r="N51" s="148">
+        <f t="shared" si="16"/>
         <v>9526</v>
       </c>
-      <c r="O51" s="149">
-        <f t="shared" si="11"/>
+      <c r="O51" s="148">
+        <f t="shared" si="17"/>
         <v>7794</v>
       </c>
-      <c r="P51" s="154">
+      <c r="P51" s="153">
         <f>1-(AVERAGE(AB16:AB17)/$AB$18)</f>
         <v>0.21518987341772156</v>
       </c>
-      <c r="Q51" s="154">
+      <c r="Q51" s="153">
         <f>1-(AVERAGE(AC16:AC17)/$AC$18)</f>
         <v>0.20634920634920639</v>
       </c>
-      <c r="R51" s="154">
+      <c r="R51" s="153">
         <f>1-(AVERAGE(AD16:AD17)/$AD$18)</f>
         <v>0.20833333333333337</v>
       </c>
-      <c r="S51" s="149">
+      <c r="S51" s="148">
         <f>D12/SUM(D6:D13)*M51</f>
         <v>322.41915730604137</v>
       </c>
-      <c r="T51" s="149">
+      <c r="T51" s="148">
         <f>E12/SUM(E6:E13)*N51</f>
         <v>585.0624566105007</v>
       </c>
-      <c r="U51" s="149">
+      <c r="U51" s="148">
         <f>F12/SUM(F6:F13)*O51</f>
         <v>486.9245662050551</v>
       </c>
-      <c r="V51" s="154">
+      <c r="V51" s="153">
         <f>D12/SUM(D6:D13)*P51</f>
         <v>1.4364666179738198E-2</v>
       </c>
-      <c r="W51" s="154">
-        <f t="shared" ref="W51:X51" si="24">E12/SUM(E6:E13)*Q51</f>
+      <c r="W51" s="153">
+        <f t="shared" ref="W51:X51" si="30">E12/SUM(E6:E13)*Q51</f>
         <v>1.2673438335743631E-2</v>
       </c>
-      <c r="X51" s="154">
-        <f t="shared" si="24"/>
+      <c r="X51" s="153">
+        <f t="shared" si="30"/>
         <v>1.30154757453665E-2</v>
       </c>
     </row>
     <row r="52" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C52" s="148" t="s">
+      <c r="C52" s="147" t="s">
         <v>185</v>
       </c>
-      <c r="D52" s="148"/>
-      <c r="E52" s="148">
+      <c r="D52" s="147"/>
+      <c r="E52" s="147">
         <v>29955</v>
       </c>
-      <c r="F52" s="148">
+      <c r="F52" s="147">
         <v>6086</v>
       </c>
-      <c r="G52" s="148">
-        <f t="shared" si="8"/>
+      <c r="G52" s="147">
+        <f t="shared" si="14"/>
         <v>36041</v>
       </c>
-      <c r="H52" s="148"/>
-      <c r="I52" s="148"/>
-      <c r="J52" s="148"/>
-      <c r="K52" s="148"/>
-      <c r="L52" s="148"/>
-      <c r="M52" s="148">
-        <f t="shared" si="20"/>
+      <c r="H52" s="147"/>
+      <c r="I52" s="147"/>
+      <c r="J52" s="147"/>
+      <c r="K52" s="147"/>
+      <c r="L52" s="147"/>
+      <c r="M52" s="147">
+        <f t="shared" si="26"/>
         <v>36041</v>
       </c>
-      <c r="N52" s="148">
-        <f t="shared" si="10"/>
+      <c r="N52" s="147">
+        <f t="shared" si="16"/>
         <v>39645.100000000006</v>
       </c>
-      <c r="O52" s="148">
-        <f t="shared" si="11"/>
+      <c r="O52" s="147">
+        <f t="shared" si="17"/>
         <v>32436.9</v>
       </c>
-      <c r="P52" s="156">
+      <c r="P52" s="155">
         <f>1-(AVERAGE(AB5:AB7)/$AB$19)</f>
         <v>0.91313131313131313</v>
       </c>
-      <c r="Q52" s="156">
+      <c r="Q52" s="155">
         <f>1-(AVERAGE(AC5:AC7)/$AC$19)</f>
         <v>0.91139240506329111</v>
       </c>
-      <c r="R52" s="156">
+      <c r="R52" s="155">
         <f>1-(AVERAGE(AD5:AD7)/$AD$19)</f>
         <v>0.91444444444444439</v>
       </c>
-      <c r="S52" s="148"/>
-      <c r="T52" s="148"/>
-      <c r="U52" s="148"/>
+      <c r="S52" s="147"/>
+      <c r="T52" s="147"/>
+      <c r="U52" s="147"/>
     </row>
     <row r="53" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C53" s="147" t="s">
+      <c r="C53" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="D53" s="147"/>
-      <c r="E53" s="147">
+      <c r="D53" s="146"/>
+      <c r="E53" s="146">
         <v>16850</v>
       </c>
-      <c r="F53" s="147">
+      <c r="F53" s="146">
         <v>5326</v>
       </c>
-      <c r="G53" s="147">
-        <f t="shared" si="8"/>
+      <c r="G53" s="146">
+        <f t="shared" si="14"/>
         <v>22176</v>
       </c>
-      <c r="H53" s="147"/>
-      <c r="I53" s="147"/>
-      <c r="J53" s="147"/>
-      <c r="K53" s="147"/>
-      <c r="L53" s="147"/>
-      <c r="M53" s="147">
-        <f t="shared" si="20"/>
+      <c r="H53" s="146"/>
+      <c r="I53" s="146"/>
+      <c r="J53" s="146"/>
+      <c r="K53" s="146"/>
+      <c r="L53" s="146"/>
+      <c r="M53" s="146">
+        <f t="shared" si="26"/>
         <v>22176</v>
       </c>
-      <c r="N53" s="147">
-        <f t="shared" si="10"/>
+      <c r="N53" s="146">
+        <f t="shared" si="16"/>
         <v>24393.600000000002</v>
       </c>
-      <c r="O53" s="147">
-        <f t="shared" si="11"/>
+      <c r="O53" s="146">
+        <f t="shared" si="17"/>
         <v>19958.400000000001</v>
       </c>
-      <c r="P53" s="155">
+      <c r="P53" s="154">
         <f>1-(AVERAGE(AB8:AB10)/$AB$19)</f>
         <v>0.80841750841750848</v>
       </c>
-      <c r="Q53" s="155">
+      <c r="Q53" s="154">
         <f>1-(AVERAGE(AC8:AC10)/$AC$19)</f>
         <v>0.80590717299578063</v>
       </c>
-      <c r="R53" s="155">
+      <c r="R53" s="154">
         <f>1-(AVERAGE(AD8:AD10)/$AD$19)</f>
         <v>0.81</v>
       </c>
-      <c r="S53" s="147">
+      <c r="S53" s="146">
         <f>SUM(D13)/SUM(D6:D13)*M48</f>
         <v>1556.6052637176085</v>
       </c>
-      <c r="T53" s="147">
-        <f t="shared" ref="T53:U53" si="25">SUM(E13)/SUM(E6:E13)*N48</f>
+      <c r="T53" s="146">
+        <f t="shared" ref="T53:U53" si="31">SUM(E13)/SUM(E6:E13)*N48</f>
         <v>2717.5942751454008</v>
       </c>
-      <c r="U53" s="147">
-        <f t="shared" si="25"/>
+      <c r="U53" s="146">
+        <f t="shared" si="31"/>
         <v>1538.1025473834977</v>
       </c>
-      <c r="V53" s="155">
+      <c r="V53" s="154">
         <f>SUM(D13)/SUM(D6:D13)*P53</f>
         <v>5.6745443221688667E-2</v>
       </c>
-      <c r="W53" s="155">
-        <f t="shared" ref="W53:X53" si="26">SUM(E13)/SUM(E6:E13)*Q53</f>
+      <c r="W53" s="154">
+        <f t="shared" ref="W53:X53" si="32">SUM(E13)/SUM(E6:E13)*Q53</f>
         <v>8.9782923374653489E-2</v>
       </c>
-      <c r="X53" s="155">
+      <c r="X53" s="154">
+        <f t="shared" si="32"/>
+        <v>6.2422992994460136E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="C54" s="147" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="147"/>
+      <c r="E54" s="147">
+        <v>11233</v>
+      </c>
+      <c r="F54" s="147">
+        <v>4565</v>
+      </c>
+      <c r="G54" s="147">
+        <f t="shared" si="14"/>
+        <v>15798</v>
+      </c>
+      <c r="H54" s="147"/>
+      <c r="I54" s="147">
+        <v>23500</v>
+      </c>
+      <c r="J54" s="147"/>
+      <c r="K54" s="147"/>
+      <c r="L54" s="147">
+        <v>8100</v>
+      </c>
+      <c r="M54" s="147">
         <f t="shared" si="26"/>
-        <v>6.2422992994460136E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C54" s="148" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" s="148"/>
-      <c r="E54" s="148">
-        <v>11233</v>
-      </c>
-      <c r="F54" s="148">
-        <v>4565</v>
-      </c>
-      <c r="G54" s="148">
-        <f t="shared" si="8"/>
-        <v>15798</v>
-      </c>
-      <c r="H54" s="148"/>
-      <c r="I54" s="148">
-        <v>23500</v>
-      </c>
-      <c r="J54" s="148"/>
-      <c r="K54" s="148"/>
-      <c r="L54" s="148">
-        <v>8100</v>
-      </c>
-      <c r="M54" s="148">
-        <f t="shared" si="20"/>
         <v>19649</v>
       </c>
-      <c r="N54" s="148">
-        <f t="shared" si="10"/>
+      <c r="N54" s="147">
+        <f t="shared" si="16"/>
         <v>17377.800000000003</v>
       </c>
-      <c r="O54" s="148">
-        <f t="shared" si="11"/>
+      <c r="O54" s="147">
+        <f t="shared" si="17"/>
         <v>11159.1</v>
       </c>
-      <c r="P54" s="156">
+      <c r="P54" s="155">
         <f>1-(AVERAGE(AB11:AB13)/$AB$19)</f>
         <v>0.67676767676767668</v>
       </c>
-      <c r="Q54" s="156">
+      <c r="Q54" s="155">
         <f>1-(AVERAGE(AC11:AC13)/$AC$19)</f>
         <v>0.67510548523206748</v>
       </c>
-      <c r="R54" s="156">
+      <c r="R54" s="155">
         <f>1-(AVERAGE(AD11:AD13)/$AD$19)</f>
         <v>0.67777777777777781</v>
       </c>
-      <c r="S54" s="148"/>
-      <c r="T54" s="148"/>
-      <c r="U54" s="148"/>
+      <c r="S54" s="147"/>
+      <c r="T54" s="147"/>
+      <c r="U54" s="147"/>
     </row>
     <row r="55" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C55" s="148" t="s">
+      <c r="C55" s="147" t="s">
         <v>188</v>
       </c>
-      <c r="D55" s="148"/>
-      <c r="E55" s="148">
+      <c r="D55" s="147"/>
+      <c r="E55" s="147">
         <v>7489</v>
       </c>
-      <c r="F55" s="148">
+      <c r="F55" s="147">
         <v>3804</v>
       </c>
-      <c r="G55" s="148">
-        <f t="shared" si="8"/>
+      <c r="G55" s="147">
+        <f t="shared" si="14"/>
         <v>11293</v>
       </c>
-      <c r="H55" s="148">
+      <c r="H55" s="147">
         <v>24000</v>
       </c>
-      <c r="I55" s="148">
+      <c r="I55" s="147">
         <v>21300</v>
       </c>
-      <c r="J55" s="148">
+      <c r="J55" s="147">
         <f>J56+5184</f>
         <v>31284</v>
       </c>
-      <c r="K55" s="148"/>
-      <c r="L55" s="148">
+      <c r="K55" s="147"/>
+      <c r="L55" s="147">
         <v>4400</v>
       </c>
-      <c r="M55" s="148">
-        <f t="shared" si="20"/>
+      <c r="M55" s="147">
+        <f t="shared" si="26"/>
         <v>18864.333333333332</v>
       </c>
-      <c r="N55" s="148">
-        <f t="shared" si="10"/>
+      <c r="N55" s="147">
+        <f t="shared" si="16"/>
         <v>21853.15</v>
       </c>
-      <c r="O55" s="148">
-        <f t="shared" si="11"/>
+      <c r="O55" s="147">
+        <f t="shared" si="17"/>
         <v>7281.85</v>
       </c>
-      <c r="P55" s="156">
+      <c r="P55" s="155">
         <f>1-(AVERAGE(AB14:AB15)/$AB$19)</f>
         <v>0.5252525252525253</v>
       </c>
-      <c r="Q55" s="156">
+      <c r="Q55" s="155">
         <f>1-(AVERAGE(AC14:AC15)/$AC$19)</f>
         <v>0.51898734177215189</v>
       </c>
-      <c r="R55" s="156">
+      <c r="R55" s="155">
         <f>1-(AVERAGE(AD14:AD15)/$AD$19)</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="S55" s="148"/>
-      <c r="T55" s="148"/>
-      <c r="U55" s="148"/>
+      <c r="S55" s="147"/>
+      <c r="T55" s="147"/>
+      <c r="U55" s="147"/>
     </row>
     <row r="56" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C56" s="148" t="s">
+      <c r="C56" s="147" t="s">
         <v>189</v>
       </c>
-      <c r="D56" s="148"/>
-      <c r="E56" s="148">
+      <c r="D56" s="147"/>
+      <c r="E56" s="147">
         <v>5617</v>
       </c>
-      <c r="F56" s="148">
+      <c r="F56" s="147">
         <v>3043</v>
       </c>
-      <c r="G56" s="148">
-        <f t="shared" si="8"/>
+      <c r="G56" s="147">
+        <f t="shared" si="14"/>
         <v>8660</v>
       </c>
-      <c r="H56" s="148">
+      <c r="H56" s="147">
         <v>17000</v>
       </c>
-      <c r="I56" s="148"/>
-      <c r="J56" s="148">
+      <c r="I56" s="147"/>
+      <c r="J56" s="147">
         <v>26100</v>
       </c>
-      <c r="K56" s="148">
+      <c r="K56" s="147">
         <v>16000</v>
       </c>
-      <c r="L56" s="148"/>
-      <c r="M56" s="148">
-        <f t="shared" si="20"/>
+      <c r="L56" s="147"/>
+      <c r="M56" s="147">
+        <f t="shared" si="26"/>
         <v>12830</v>
       </c>
-      <c r="N56" s="148">
-        <f t="shared" si="10"/>
+      <c r="N56" s="147">
+        <f t="shared" si="16"/>
         <v>17208.666666666668</v>
       </c>
-      <c r="O56" s="148">
-        <f t="shared" si="11"/>
+      <c r="O56" s="147">
+        <f t="shared" si="17"/>
         <v>7794</v>
       </c>
-      <c r="P56" s="156">
+      <c r="P56" s="155">
         <f>1-(AVERAGE(AB16:AB17)/$AB$19)</f>
         <v>0.3737373737373737</v>
       </c>
-      <c r="Q56" s="156">
+      <c r="Q56" s="155">
         <f>1-(AVERAGE(AC16:AC17)/$AC$19)</f>
         <v>0.36708860759493667</v>
       </c>
-      <c r="R56" s="156">
+      <c r="R56" s="155">
         <f>1-(AVERAGE(AD16:AD17)/$AD$19)</f>
         <v>0.3666666666666667</v>
       </c>
-      <c r="S56" s="148"/>
-      <c r="T56" s="148"/>
-      <c r="U56" s="148"/>
+      <c r="S56" s="147"/>
+      <c r="T56" s="147"/>
+      <c r="U56" s="147"/>
     </row>
     <row r="57" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C57" s="150" t="s">
+      <c r="C57" s="149" t="s">
         <v>211</v>
       </c>
-      <c r="D57" s="150"/>
-      <c r="E57" s="150"/>
-      <c r="F57" s="150"/>
-      <c r="G57" s="150"/>
-      <c r="H57" s="150"/>
-      <c r="I57" s="150">
+      <c r="D57" s="149"/>
+      <c r="E57" s="149"/>
+      <c r="F57" s="149"/>
+      <c r="G57" s="149"/>
+      <c r="H57" s="149"/>
+      <c r="I57" s="149">
         <v>2128</v>
       </c>
-      <c r="J57" s="150">
+      <c r="J57" s="149">
         <v>3200</v>
       </c>
-      <c r="K57" s="150"/>
-      <c r="L57" s="150">
+      <c r="K57" s="149"/>
+      <c r="L57" s="149">
         <v>2200</v>
       </c>
-      <c r="M57" s="150">
-        <f t="shared" si="20"/>
+      <c r="M57" s="149">
+        <f t="shared" si="26"/>
         <v>2128</v>
       </c>
-      <c r="N57" s="150">
-        <f t="shared" si="10"/>
+      <c r="N57" s="149">
+        <f t="shared" si="16"/>
         <v>1600</v>
       </c>
-      <c r="O57" s="150">
-        <f t="shared" si="11"/>
+      <c r="O57" s="149">
+        <f t="shared" si="17"/>
         <v>1100</v>
       </c>
-      <c r="P57" s="154">
+      <c r="P57" s="153">
         <f>1-(AB18/$AB$19)</f>
         <v>0.20202020202020199</v>
       </c>
-      <c r="Q57" s="154">
+      <c r="Q57" s="153">
         <f>1-(AC18/$AC$19)</f>
         <v>0.20253164556962022</v>
       </c>
-      <c r="R57" s="154">
+      <c r="R57" s="153">
         <f>1-(AD18/$AD$19)</f>
         <v>0.19999999999999996</v>
       </c>
-      <c r="S57" s="149">
+      <c r="S57" s="148">
         <f>D13/SUM(D6:D13)*M57</f>
         <v>149.37121217492202</v>
       </c>
-      <c r="T57" s="149">
+      <c r="T57" s="148">
         <f>E13/SUM(E6:E13)*N57</f>
         <v>178.24965729669424</v>
       </c>
-      <c r="U57" s="149">
+      <c r="U57" s="148">
         <f>F13/SUM(F6:F13)*O57</f>
         <v>84.771965794945856</v>
       </c>
-      <c r="V57" s="154">
+      <c r="V57" s="153">
         <f>D13/SUM(D6:D13)*P57</f>
         <v>1.4180452283637315E-2</v>
       </c>
-      <c r="W57" s="154">
-        <f t="shared" ref="W57:X57" si="27">E13/SUM(E6:E13)*Q57</f>
+      <c r="W57" s="153">
+        <f t="shared" ref="W57:X57" si="33">E13/SUM(E6:E13)*Q57</f>
         <v>2.2563247759075217E-2</v>
       </c>
-      <c r="X57" s="154">
-        <f t="shared" si="27"/>
+      <c r="X57" s="153">
+        <f t="shared" si="33"/>
         <v>1.5413084689990152E-2</v>
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="S59" s="158">
+      <c r="S59" s="157">
         <f>SUM(S37,S39,S42,S46,S51,S57)</f>
         <v>9608.4735804205193</v>
       </c>
-      <c r="T59" s="158">
-        <f t="shared" ref="T59:U59" si="28">SUM(T37,T39,T42,T46,T51,T57)</f>
+      <c r="T59" s="157">
+        <f t="shared" ref="T59:U59" si="34">SUM(T37,T39,T42,T46,T51,T57)</f>
         <v>14333.869646601945</v>
       </c>
-      <c r="U59" s="158">
-        <f t="shared" si="28"/>
+      <c r="U59" s="157">
+        <f t="shared" si="34"/>
         <v>11196.414691601361</v>
       </c>
-      <c r="V59" s="157">
+      <c r="V59" s="156">
         <f>SUM(V37,V39,V42,V46,V51,V57)</f>
         <v>0.3499559220938272</v>
       </c>
-      <c r="W59" s="157">
-        <f t="shared" ref="W59:X59" si="29">SUM(W37,W39,W42,W46,W51,W57)</f>
+      <c r="W59" s="156">
+        <f t="shared" ref="W59:X59" si="35">SUM(W37,W39,W42,W46,W51,W57)</f>
         <v>0.34759093292022342</v>
       </c>
-      <c r="X59" s="157">
-        <f t="shared" si="29"/>
+      <c r="X59" s="156">
+        <f t="shared" si="35"/>
         <v>0.36920600336632792</v>
       </c>
     </row>
@@ -8547,28 +8656,28 @@
       <c r="C60" t="s">
         <v>210</v>
       </c>
-      <c r="S60" s="159">
+      <c r="S60" s="158">
         <f>SUM(S38,S41,S44,S48,S53,S57)</f>
         <v>20563.0239417189</v>
       </c>
-      <c r="T60" s="159">
-        <f t="shared" ref="T60:X60" si="30">SUM(T38,T41,T44,T48,T53,T57)</f>
+      <c r="T60" s="158">
+        <f t="shared" ref="T60:X60" si="36">SUM(T38,T41,T44,T48,T53,T57)</f>
         <v>22259.387557085229</v>
       </c>
-      <c r="U60" s="159">
-        <f t="shared" si="30"/>
+      <c r="U60" s="158">
+        <f t="shared" si="36"/>
         <v>15982.779351113084</v>
       </c>
-      <c r="V60" s="160">
-        <f t="shared" si="30"/>
+      <c r="V60" s="159">
+        <f t="shared" si="36"/>
         <v>0.56982150406598298</v>
       </c>
-      <c r="W60" s="160">
-        <f t="shared" si="30"/>
+      <c r="W60" s="159">
+        <f t="shared" si="36"/>
         <v>0.57417922843609159</v>
       </c>
-      <c r="X60" s="160">
-        <f t="shared" si="30"/>
+      <c r="X60" s="159">
+        <f t="shared" si="36"/>
         <v>0.51228555848472779</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RSD Retrofit: Switch to DayNite and remove NCAP_AFA
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25839AB9-0AA1-4702-89A1-AC80056A6BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017E8587-D8D2-479E-B68F-8B5B57673F64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{0C9666FB-34CF-4809-B682-F7B52A796689}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{0C9666FB-34CF-4809-B682-F7B52A796689}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="224">
   <si>
     <t>Document type:</t>
   </si>
@@ -479,9 +479,6 @@
     <t>PJ/000dwelling</t>
   </si>
   <si>
-    <t>AFA~FX</t>
-  </si>
-  <si>
     <t>*Technology name</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>Deep Retrofit Required for Heat Pump</t>
+  </si>
+  <si>
+    <t>DayNite</t>
   </si>
 </sst>
 </file>
@@ -772,12 +772,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="0.000%"/>
   </numFmts>
   <fonts count="47" x14ac:knownFonts="1">
     <font>
@@ -1856,7 +1856,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1950,7 +1950,7 @@
     </xf>
     <xf numFmtId="15" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2063,7 +2063,7 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2106,7 +2106,7 @@
     <xf numFmtId="1" fontId="5" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2121,7 +2121,7 @@
     <xf numFmtId="1" fontId="5" fillId="18" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2136,7 +2136,7 @@
     <xf numFmtId="1" fontId="5" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2152,7 +2152,7 @@
     <xf numFmtId="1" fontId="5" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2167,7 +2167,7 @@
     <xf numFmtId="3" fontId="1" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="22" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2236,10 +2236,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="41" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2251,8 +2251,8 @@
     <xf numFmtId="9" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="42" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="42" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="42" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2269,7 +2269,7 @@
     <xf numFmtId="9" fontId="9" fillId="15" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2287,13 +2287,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2305,10 +2305,10 @@
     <xf numFmtId="0" fontId="33" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4943,9 +4943,11 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:AA50"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4956,25 +4958,25 @@
     <col min="9" max="9" width="2" style="85" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.85546875" style="85" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" style="85" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" style="85"/>
-    <col min="16" max="16" width="9.5703125" style="85" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="85"/>
-    <col min="18" max="22" width="11.140625" style="85" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="85"/>
+    <col min="13" max="14" width="9.140625" style="85"/>
+    <col min="15" max="15" width="9.5703125" style="85" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="85"/>
+    <col min="17" max="21" width="11.140625" style="85" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="78"/>
     </row>
-    <row r="2" spans="1:22" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A2" s="79" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="76" t="s">
         <v>27</v>
       </c>
@@ -4985,11 +4987,11 @@
       <c r="K4" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="90" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="90" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -5025,32 +5027,29 @@
         <v>72</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="S5" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="R5" s="84" t="s">
-        <v>132</v>
-      </c>
-      <c r="S5" s="84" t="s">
-        <v>138</v>
-      </c>
-      <c r="T5" s="84" t="s">
+      <c r="T5" s="179" t="s">
         <v>140</v>
       </c>
-      <c r="U5" s="179" t="s">
-        <v>141</v>
-      </c>
-      <c r="V5" s="179"/>
-    </row>
-    <row r="6" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="U5" s="179"/>
+    </row>
+    <row r="6" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="83" t="s">
         <v>74</v>
       </c>
@@ -5067,54 +5066,53 @@
         <v>77</v>
       </c>
       <c r="F6" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="83" t="s">
         <v>130</v>
-      </c>
-      <c r="G6" s="83" t="s">
-        <v>131</v>
       </c>
       <c r="H6" s="83" t="s">
         <v>78</v>
       </c>
       <c r="I6" s="81"/>
       <c r="J6" s="82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K6" s="82" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
+      <c r="M6" s="82" t="s">
+        <v>80</v>
+      </c>
       <c r="N6" s="82" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="P6" s="160" t="s">
         <v>142</v>
       </c>
+      <c r="O6" s="160" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q6" s="89"/>
       <c r="R6" s="89"/>
-      <c r="S6" s="89"/>
+      <c r="S6" s="89" t="s">
+        <v>127</v>
+      </c>
       <c r="T6" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="U6" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="V6" s="89" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="80" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="80" t="str">
-        <f t="shared" ref="B7:B12" si="0">"R-RTFT-"&amp;R7&amp;"_"&amp;S7</f>
+        <f t="shared" ref="B7:B12" si="0">"R-RTFT-"&amp;Q7&amp;"_"&amp;R7</f>
         <v>R-RTFT-Apt_Shallow</v>
       </c>
       <c r="C7" s="80" t="str">
-        <f t="shared" ref="C7:C12" si="1">"Residential "&amp;R7&amp;" - "&amp;S7&amp;" retrofit"</f>
+        <f t="shared" ref="C7:C12" si="1">"Residential "&amp;Q7&amp;" - "&amp;R7&amp;" retrofit"</f>
         <v>Residential Apt - Shallow retrofit</v>
       </c>
       <c r="D7" s="80" t="s">
@@ -5123,7 +5121,9 @@
       <c r="E7" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="80"/>
+      <c r="F7" s="80" t="s">
+        <v>223</v>
+      </c>
       <c r="G7" s="80"/>
       <c r="H7" s="80"/>
       <c r="I7" s="80"/>
@@ -5132,45 +5132,42 @@
         <v>R-RTFT-Apt_Shallow</v>
       </c>
       <c r="K7" s="80" t="str">
-        <f>"RSDSH_"&amp;R7</f>
+        <f>"RSDSH_"&amp;Q7</f>
         <v>RSDSH_Apt</v>
       </c>
       <c r="L7" s="80">
         <v>2020</v>
       </c>
       <c r="M7" s="80">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N7" s="80">
-        <v>50</v>
-      </c>
-      <c r="O7" s="80">
-        <f>V7</f>
+        <f>U7</f>
         <v>5.9072960538612464E-3</v>
       </c>
-      <c r="P7" s="161">
+      <c r="O7" s="161">
         <f>Data!U59/1000</f>
         <v>11.196414691601362</v>
       </c>
+      <c r="Q7" s="85" t="s">
+        <v>132</v>
+      </c>
       <c r="R7" s="85" t="s">
-        <v>133</v>
-      </c>
-      <c r="S7" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="T7" s="85">
+        <v>135</v>
+      </c>
+      <c r="S7" s="85">
         <v>1.6E-2</v>
       </c>
-      <c r="U7" s="163">
+      <c r="T7" s="163">
         <f>Data!X59</f>
         <v>0.36920600336632792</v>
       </c>
-      <c r="V7" s="85">
-        <f>T7*U7</f>
+      <c r="U7" s="85">
+        <f>S7*T7</f>
         <v>5.9072960538612464E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="88" t="s">
         <v>36</v>
       </c>
@@ -5188,7 +5185,9 @@
       <c r="E8" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="88"/>
+      <c r="F8" s="88" t="s">
+        <v>223</v>
+      </c>
       <c r="G8" s="88"/>
       <c r="H8" s="88"/>
       <c r="I8" s="80"/>
@@ -5197,45 +5196,42 @@
         <v>R-RTFT-Apt_Deep</v>
       </c>
       <c r="K8" s="88" t="str">
-        <f t="shared" ref="K8:K12" si="3">"RSDSH_"&amp;R8</f>
+        <f t="shared" ref="K8:K12" si="3">"RSDSH_"&amp;Q8</f>
         <v>RSDSH_Apt</v>
       </c>
       <c r="L8" s="88">
         <v>2020</v>
       </c>
       <c r="M8" s="88">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N8" s="88">
-        <v>50</v>
-      </c>
-      <c r="O8" s="88">
-        <f t="shared" ref="O8:O12" si="4">V8</f>
+        <f t="shared" ref="N8:N12" si="4">U8</f>
         <v>8.1965689357556444E-3</v>
       </c>
-      <c r="P8" s="162">
+      <c r="O8" s="162">
         <f>Data!U60/1000</f>
         <v>15.982779351113084</v>
       </c>
+      <c r="Q8" s="86" t="s">
+        <v>132</v>
+      </c>
       <c r="R8" s="86" t="s">
-        <v>133</v>
-      </c>
-      <c r="S8" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="T8" s="86">
+        <v>136</v>
+      </c>
+      <c r="S8" s="86">
         <v>1.6E-2</v>
       </c>
-      <c r="U8" s="164">
+      <c r="T8" s="164">
         <f>Data!X60</f>
         <v>0.51228555848472779</v>
       </c>
-      <c r="V8" s="86">
-        <f t="shared" ref="V8:V12" si="5">T8*U8</f>
+      <c r="U8" s="86">
+        <f t="shared" ref="U8:U12" si="5">S8*T8</f>
         <v>8.1965689357556444E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="80" t="s">
         <v>36</v>
       </c>
@@ -5253,7 +5249,9 @@
       <c r="E9" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="80"/>
+      <c r="F9" s="80" t="s">
+        <v>223</v>
+      </c>
       <c r="G9" s="80"/>
       <c r="H9" s="80"/>
       <c r="I9" s="80"/>
@@ -5269,38 +5267,35 @@
         <v>2020</v>
       </c>
       <c r="M9" s="80">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N9" s="80">
-        <v>50</v>
-      </c>
-      <c r="O9" s="80">
         <f t="shared" si="4"/>
         <v>9.413814304323951E-3</v>
       </c>
-      <c r="P9" s="161">
+      <c r="O9" s="161">
         <f>Data!S59/1000</f>
         <v>9.6084735804205188</v>
       </c>
+      <c r="Q9" s="85" t="s">
+        <v>133</v>
+      </c>
       <c r="R9" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="S9" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="T9" s="85">
+        <v>135</v>
+      </c>
+      <c r="S9" s="85">
         <v>2.69E-2</v>
       </c>
-      <c r="U9" s="163">
+      <c r="T9" s="163">
         <f>Data!V59</f>
         <v>0.3499559220938272</v>
       </c>
-      <c r="V9" s="85">
+      <c r="U9" s="85">
         <f t="shared" si="5"/>
         <v>9.413814304323951E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="88" t="s">
         <v>36</v>
       </c>
@@ -5318,7 +5313,9 @@
       <c r="E10" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="88"/>
+      <c r="F10" s="88" t="s">
+        <v>223</v>
+      </c>
       <c r="G10" s="88"/>
       <c r="H10" s="88"/>
       <c r="I10" s="80"/>
@@ -5334,38 +5331,35 @@
         <v>2020</v>
       </c>
       <c r="M10" s="88">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N10" s="88">
-        <v>50</v>
-      </c>
-      <c r="O10" s="88">
         <f t="shared" si="4"/>
         <v>1.5328198459374942E-2</v>
       </c>
-      <c r="P10" s="162">
+      <c r="O10" s="162">
         <f>Data!S60/1000</f>
         <v>20.5630239417189</v>
       </c>
+      <c r="Q10" s="86" t="s">
+        <v>133</v>
+      </c>
       <c r="R10" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="S10" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="T10" s="86">
+        <v>136</v>
+      </c>
+      <c r="S10" s="86">
         <v>2.69E-2</v>
       </c>
-      <c r="U10" s="164">
+      <c r="T10" s="164">
         <f>Data!V60</f>
         <v>0.56982150406598298</v>
       </c>
-      <c r="V10" s="86">
+      <c r="U10" s="86">
         <f t="shared" si="5"/>
         <v>1.5328198459374942E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
@@ -5383,7 +5377,9 @@
       <c r="E11" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="80"/>
+      <c r="F11" s="80" t="s">
+        <v>223</v>
+      </c>
       <c r="G11" s="80"/>
       <c r="H11" s="80"/>
       <c r="I11" s="80"/>
@@ -5399,38 +5395,35 @@
         <v>2020</v>
       </c>
       <c r="M11" s="80">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N11" s="80">
-        <v>50</v>
-      </c>
-      <c r="O11" s="80">
         <f t="shared" si="4"/>
         <v>1.6649605686878701E-2</v>
       </c>
-      <c r="P11" s="161">
+      <c r="O11" s="161">
         <f>Data!T59/1000</f>
         <v>14.333869646601945</v>
       </c>
+      <c r="Q11" s="85" t="s">
+        <v>134</v>
+      </c>
       <c r="R11" s="85" t="s">
         <v>135</v>
       </c>
-      <c r="S11" s="85" t="s">
-        <v>136</v>
-      </c>
-      <c r="T11" s="85">
+      <c r="S11" s="85">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="U11" s="163">
+      <c r="T11" s="163">
         <f>Data!W59</f>
         <v>0.34759093292022342</v>
       </c>
-      <c r="V11" s="85">
+      <c r="U11" s="85">
         <f t="shared" si="5"/>
         <v>1.6649605686878701E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="88" t="s">
         <v>36</v>
       </c>
@@ -5448,7 +5441,9 @@
       <c r="E12" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="88"/>
+      <c r="F12" s="88" t="s">
+        <v>223</v>
+      </c>
       <c r="G12" s="88"/>
       <c r="H12" s="88"/>
       <c r="I12" s="80"/>
@@ -5464,266 +5459,263 @@
         <v>2020</v>
       </c>
       <c r="M12" s="88">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="N12" s="88">
-        <v>50</v>
-      </c>
-      <c r="O12" s="88">
         <f t="shared" si="4"/>
         <v>2.7503185042088787E-2</v>
       </c>
-      <c r="P12" s="162">
+      <c r="O12" s="162">
         <f>Data!T60/1000</f>
         <v>22.25938755708523</v>
       </c>
+      <c r="Q12" s="86" t="s">
+        <v>134</v>
+      </c>
       <c r="R12" s="86" t="s">
-        <v>135</v>
-      </c>
-      <c r="S12" s="86" t="s">
-        <v>137</v>
-      </c>
-      <c r="T12" s="86">
+        <v>136</v>
+      </c>
+      <c r="S12" s="86">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="U12" s="164">
+      <c r="T12" s="164">
         <f>Data!W60</f>
         <v>0.57417922843609159</v>
       </c>
-      <c r="V12" s="86">
+      <c r="U12" s="86">
         <f t="shared" si="5"/>
         <v>2.7503185042088787E-2</v>
       </c>
     </row>
-    <row r="19" spans="23:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V19"/>
       <c r="W19"/>
       <c r="X19"/>
       <c r="Y19"/>
       <c r="Z19"/>
-      <c r="AA19"/>
-    </row>
-    <row r="20" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V20"/>
       <c r="W20"/>
       <c r="X20"/>
       <c r="Y20"/>
       <c r="Z20"/>
-      <c r="AA20"/>
-    </row>
-    <row r="21" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V21"/>
       <c r="W21"/>
       <c r="X21"/>
       <c r="Y21"/>
       <c r="Z21"/>
-      <c r="AA21"/>
-    </row>
-    <row r="22" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V22"/>
       <c r="W22"/>
       <c r="X22"/>
       <c r="Y22"/>
       <c r="Z22"/>
-      <c r="AA22"/>
-    </row>
-    <row r="23" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V23"/>
       <c r="W23"/>
       <c r="X23"/>
       <c r="Y23"/>
       <c r="Z23"/>
-      <c r="AA23"/>
-    </row>
-    <row r="24" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V24"/>
       <c r="W24"/>
       <c r="X24"/>
       <c r="Y24"/>
       <c r="Z24"/>
-      <c r="AA24"/>
-    </row>
-    <row r="25" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V25"/>
       <c r="W25"/>
       <c r="X25"/>
       <c r="Y25"/>
       <c r="Z25"/>
-      <c r="AA25"/>
-    </row>
-    <row r="26" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V26"/>
       <c r="W26"/>
       <c r="X26"/>
       <c r="Y26"/>
       <c r="Z26"/>
-      <c r="AA26"/>
-    </row>
-    <row r="27" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V27"/>
       <c r="W27"/>
       <c r="X27"/>
       <c r="Y27"/>
       <c r="Z27"/>
-      <c r="AA27"/>
-    </row>
-    <row r="28" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V28"/>
       <c r="W28"/>
       <c r="X28"/>
       <c r="Y28"/>
       <c r="Z28"/>
-      <c r="AA28"/>
-    </row>
-    <row r="29" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V29"/>
       <c r="W29"/>
       <c r="X29"/>
       <c r="Y29"/>
       <c r="Z29"/>
-      <c r="AA29"/>
-    </row>
-    <row r="30" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V30"/>
       <c r="W30"/>
       <c r="X30"/>
       <c r="Y30"/>
       <c r="Z30"/>
-      <c r="AA30"/>
-    </row>
-    <row r="31" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V31"/>
       <c r="W31"/>
       <c r="X31"/>
       <c r="Y31"/>
       <c r="Z31"/>
-      <c r="AA31"/>
-    </row>
-    <row r="32" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V32"/>
       <c r="W32"/>
       <c r="X32"/>
       <c r="Y32"/>
       <c r="Z32"/>
-      <c r="AA32"/>
-    </row>
-    <row r="33" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V33"/>
       <c r="W33"/>
       <c r="X33"/>
       <c r="Y33"/>
       <c r="Z33"/>
-      <c r="AA33"/>
-    </row>
-    <row r="34" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V34"/>
       <c r="W34"/>
       <c r="X34"/>
       <c r="Y34"/>
       <c r="Z34"/>
-      <c r="AA34"/>
-    </row>
-    <row r="35" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V35"/>
       <c r="W35"/>
       <c r="X35"/>
       <c r="Y35"/>
       <c r="Z35"/>
-      <c r="AA35"/>
-    </row>
-    <row r="36" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V36"/>
       <c r="W36"/>
       <c r="X36"/>
       <c r="Y36"/>
       <c r="Z36"/>
-      <c r="AA36"/>
-    </row>
-    <row r="37" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V37"/>
       <c r="W37"/>
       <c r="X37"/>
       <c r="Y37"/>
       <c r="Z37"/>
-      <c r="AA37"/>
-    </row>
-    <row r="38" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V38"/>
       <c r="W38"/>
       <c r="X38"/>
       <c r="Y38"/>
       <c r="Z38"/>
-      <c r="AA38"/>
-    </row>
-    <row r="39" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V39"/>
       <c r="W39"/>
       <c r="X39"/>
       <c r="Y39"/>
       <c r="Z39"/>
-      <c r="AA39"/>
-    </row>
-    <row r="40" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V40"/>
       <c r="W40"/>
       <c r="X40"/>
       <c r="Y40"/>
       <c r="Z40"/>
-      <c r="AA40"/>
-    </row>
-    <row r="41" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V41"/>
       <c r="W41"/>
       <c r="X41"/>
       <c r="Y41"/>
       <c r="Z41"/>
-      <c r="AA41"/>
-    </row>
-    <row r="42" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V42"/>
       <c r="W42"/>
       <c r="X42"/>
       <c r="Y42"/>
       <c r="Z42"/>
-      <c r="AA42"/>
-    </row>
-    <row r="43" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V43"/>
       <c r="W43"/>
       <c r="X43"/>
       <c r="Y43"/>
       <c r="Z43"/>
-      <c r="AA43"/>
-    </row>
-    <row r="44" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V44"/>
       <c r="W44"/>
       <c r="X44"/>
       <c r="Y44"/>
       <c r="Z44"/>
-      <c r="AA44"/>
-    </row>
-    <row r="45" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V45"/>
       <c r="W45"/>
       <c r="X45"/>
       <c r="Y45"/>
       <c r="Z45"/>
-      <c r="AA45"/>
-    </row>
-    <row r="46" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V46"/>
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
       <c r="Z46"/>
-      <c r="AA46"/>
-    </row>
-    <row r="47" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V47"/>
       <c r="W47"/>
       <c r="X47"/>
       <c r="Y47"/>
       <c r="Z47"/>
-      <c r="AA47"/>
-    </row>
-    <row r="48" spans="23:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="22:26" x14ac:dyDescent="0.2">
+      <c r="V48"/>
       <c r="W48"/>
       <c r="X48"/>
       <c r="Y48"/>
       <c r="Z48"/>
-      <c r="AA48"/>
-    </row>
-    <row r="49" spans="19:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="V49"/>
       <c r="W49"/>
       <c r="X49"/>
       <c r="Y49"/>
       <c r="Z49"/>
-      <c r="AA49"/>
-    </row>
-    <row r="50" spans="19:27" x14ac:dyDescent="0.2">
-      <c r="S50"/>
+    </row>
+    <row r="50" spans="18:26" x14ac:dyDescent="0.2">
+      <c r="R50"/>
+      <c r="U50"/>
       <c r="V50"/>
       <c r="W50"/>
       <c r="X50"/>
       <c r="Y50"/>
       <c r="Z50"/>
-      <c r="AA50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="T5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5736,8 +5728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W59" sqref="W59"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5765,100 +5757,100 @@
     <row r="1" spans="3:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L2" s="183" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M2" s="184"/>
       <c r="N2" s="185"/>
       <c r="O2" s="183" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P2" s="184"/>
       <c r="Q2" s="185"/>
       <c r="R2" s="183" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S2" s="184"/>
       <c r="T2" s="185"/>
       <c r="Y2" s="125" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="3:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="182" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D3" s="182"/>
       <c r="E3" s="182"/>
       <c r="F3" s="182"/>
       <c r="G3" s="182"/>
       <c r="L3" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="M3" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="M3" s="94" t="s">
+      <c r="N3" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="N3" s="94" t="s">
-        <v>194</v>
-      </c>
       <c r="O3" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="P3" s="94" t="s">
+      <c r="Q3" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="Q3" s="94" t="s">
-        <v>194</v>
-      </c>
       <c r="R3" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="S3" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="S3" s="94" t="s">
+      <c r="T3" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="T3" s="94" t="s">
-        <v>194</v>
-      </c>
       <c r="U3" s="94" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y3" s="126"/>
       <c r="AB3" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AC3" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AC3" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="AD3" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH3" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="AE3" t="s">
-        <v>216</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="AI3" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="95" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="F4" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="G4" s="96" t="s">
         <v>195</v>
       </c>
-      <c r="D4" s="94" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="94" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="94" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="96" t="s">
-        <v>196</v>
-      </c>
       <c r="K4" s="97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L4" s="98">
         <v>1.4285714285714286</v>
@@ -5895,7 +5887,7 @@
     </row>
     <row r="5" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C5" s="97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="99">
         <v>15472.073727176739</v>
@@ -5910,7 +5902,7 @@
         <v>45269.678921539591</v>
       </c>
       <c r="K5" s="102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L5" s="103">
         <v>1</v>
@@ -5944,7 +5936,7 @@
         <v>90.104603265666654</v>
       </c>
       <c r="AA5" s="128" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AB5">
         <f>AVERAGE(AH5:AI5)</f>
@@ -5965,7 +5957,7 @@
     </row>
     <row r="6" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C6" s="102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="104">
         <v>9537.7783975583752</v>
@@ -5980,7 +5972,7 @@
         <v>26430.9709418846</v>
       </c>
       <c r="K6" s="107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L6" s="108">
         <v>1</v>
@@ -6014,7 +6006,7 @@
         <v>115.45560966933333</v>
       </c>
       <c r="AA6" s="131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB6">
         <f t="shared" ref="AB6:AB19" si="1">AVERAGE(AH6:AI6)</f>
@@ -6035,7 +6027,7 @@
     </row>
     <row r="7" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C7" s="107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="109">
         <v>17545.09295382088</v>
@@ -6050,7 +6042,7 @@
         <v>51677.889576076108</v>
       </c>
       <c r="K7" s="102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L7" s="103">
         <v>1</v>
@@ -6084,7 +6076,7 @@
         <v>139.59487310199998</v>
       </c>
       <c r="AA7" s="131" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AB7">
         <f t="shared" si="1"/>
@@ -6105,7 +6097,7 @@
     </row>
     <row r="8" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C8" s="102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="104">
         <v>49768.849685929476</v>
@@ -6120,7 +6112,7 @@
         <v>123159.54010496697</v>
       </c>
       <c r="K8" s="107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L8" s="108">
         <v>0.62350597609561753</v>
@@ -6154,7 +6146,7 @@
         <v>188.85972977266667</v>
       </c>
       <c r="AA8" s="131" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB8">
         <f t="shared" si="1"/>
@@ -6175,7 +6167,7 @@
     </row>
     <row r="9" spans="3:35" ht="15" x14ac:dyDescent="0.25">
       <c r="C9" s="107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="109">
         <v>282151.52747564798</v>
@@ -6190,10 +6182,10 @@
         <v>592375.26452582516</v>
       </c>
       <c r="I9" s="112" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L9" s="103">
         <v>0.64275466284074612</v>
@@ -6227,7 +6219,7 @@
         <v>260.5202750266667</v>
       </c>
       <c r="AA9" s="131" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AB9">
         <f t="shared" si="1"/>
@@ -6248,7 +6240,7 @@
     </row>
     <row r="10" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="102" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="104">
         <v>187627.02237661046</v>
@@ -6263,7 +6255,7 @@
         <v>398034.15543850785</v>
       </c>
       <c r="K10" s="107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L10" s="108">
         <v>0.65947786606129399</v>
@@ -6297,7 +6289,7 @@
         <v>337.60044621333333</v>
       </c>
       <c r="AA10" s="131" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AB10">
         <f t="shared" si="1"/>
@@ -6318,7 +6310,7 @@
     </row>
     <row r="11" spans="3:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C11" s="107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D11" s="109">
         <v>101418.89596184672</v>
@@ -6333,7 +6325,7 @@
         <v>208583.47042416356</v>
       </c>
       <c r="K11" s="102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L11" s="103">
         <v>0.67760942760942755</v>
@@ -6367,7 +6359,7 @@
         <v>413.55162632333332</v>
       </c>
       <c r="AA11" s="131" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AB11">
         <f t="shared" si="1"/>
@@ -6388,7 +6380,7 @@
     </row>
     <row r="12" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="104">
         <v>50123.806027321167</v>
@@ -6403,7 +6395,7 @@
         <v>105695.98501717232</v>
       </c>
       <c r="K12" s="113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L12" s="114">
         <v>0.56219445953286251</v>
@@ -6437,7 +6429,7 @@
         <v>626.50035470099999</v>
       </c>
       <c r="AA12" s="131" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AB12">
         <f t="shared" si="1"/>
@@ -6458,7 +6450,7 @@
     </row>
     <row r="13" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="117" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" s="118">
         <v>52706.674394088106</v>
@@ -6482,7 +6474,7 @@
         <v>0.71303848954914961</v>
       </c>
       <c r="AA13" s="131" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AB13">
         <f t="shared" si="1"/>
@@ -6503,7 +6495,7 @@
     </row>
     <row r="14" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="120" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="145">
         <f>SUM(D5:D13)</f>
@@ -6521,7 +6513,7 @@
         <v>1697580.3349999997</v>
       </c>
       <c r="AA14" s="131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AB14">
         <f t="shared" si="1"/>
@@ -6542,10 +6534,10 @@
     </row>
     <row r="15" spans="3:35" x14ac:dyDescent="0.2">
       <c r="L15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AA15" s="131" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AB15">
         <f t="shared" si="1"/>
@@ -6566,10 +6558,10 @@
     </row>
     <row r="16" spans="3:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L16" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AA16" s="131" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AB16">
         <f t="shared" si="1"/>
@@ -6590,46 +6582,46 @@
     </row>
     <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="G17" s="94" t="s">
-        <v>194</v>
-      </c>
       <c r="H17" s="94" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L17" s="123" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="V17" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="W17" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA17" s="131" t="s">
         <v>160</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="V17" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="W17" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA17" s="131" t="s">
-        <v>161</v>
       </c>
       <c r="AB17">
         <f t="shared" si="1"/>
@@ -6650,7 +6642,7 @@
     </row>
     <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F18" s="145">
         <f>SUM(D5:D8)</f>
@@ -6665,10 +6657,10 @@
         <v>50844.518002144141</v>
       </c>
       <c r="L18" s="122" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O18" s="97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P18">
         <f>1-U4/$U$12</f>
@@ -6703,7 +6695,7 @@
         <v>0.39867861447009212</v>
       </c>
       <c r="AA18" s="131" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB18">
         <f t="shared" si="1"/>
@@ -6724,7 +6716,7 @@
     </row>
     <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F19" s="145">
         <f>D9</f>
@@ -6739,7 +6731,7 @@
         <v>58904.8034364337</v>
       </c>
       <c r="O19" s="102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P19">
         <f t="shared" ref="P19:P25" si="4">1-U5/$U$12</f>
@@ -6770,7 +6762,7 @@
         <v>0.21957362207234754</v>
       </c>
       <c r="AA19" s="136" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AB19">
         <f t="shared" si="1"/>
@@ -6791,7 +6783,7 @@
     </row>
     <row r="20" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F20" s="145">
         <f>SUM(D10:D13)</f>
@@ -6806,7 +6798,7 @@
         <v>97049.563561422125</v>
       </c>
       <c r="O20" s="107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P20" s="124">
         <f t="shared" si="4"/>
@@ -6833,7 +6825,7 @@
         <v>0.17292371056513256</v>
       </c>
       <c r="Y20" s="139" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -6843,7 +6835,7 @@
       </c>
       <c r="G21" s="85"/>
       <c r="O21" s="102" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P21" s="124">
         <f t="shared" si="4"/>
@@ -6866,21 +6858,21 @@
         <v>0.26085421561265365</v>
       </c>
       <c r="Y21" s="140" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="F22" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="G22" s="94" t="s">
-        <v>194</v>
-      </c>
       <c r="H22" s="94" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O22" s="107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P22" s="124">
         <f t="shared" si="4"/>
@@ -6901,7 +6893,7 @@
     </row>
     <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F23" s="165">
         <f>F18/$D$14</f>
@@ -6916,7 +6908,7 @@
         <v>0.24586456547937455</v>
       </c>
       <c r="O23" s="102" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P23" s="124">
         <f t="shared" si="4"/>
@@ -6933,7 +6925,7 @@
     </row>
     <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24" s="165">
         <f t="shared" ref="F24:F25" si="11">F19/$D$14</f>
@@ -6948,7 +6940,7 @@
         <v>0.28484101080348528</v>
       </c>
       <c r="O24" s="107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P24" s="124">
         <f t="shared" si="4"/>
@@ -6961,7 +6953,7 @@
     </row>
     <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F25" s="165">
         <f t="shared" si="11"/>
@@ -6976,7 +6968,7 @@
         <v>0.46929442371714014</v>
       </c>
       <c r="O25" s="102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P25" s="93">
         <f t="shared" si="4"/>
@@ -6995,116 +6987,116 @@
     </row>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="123" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C29" s="186" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D29" s="187"/>
       <c r="E29" s="187"/>
       <c r="F29" s="187"/>
       <c r="G29" s="188"/>
       <c r="H29" s="186" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I29" s="187"/>
       <c r="J29" s="187"/>
       <c r="K29" s="187"/>
       <c r="L29" s="188"/>
       <c r="M29" s="180" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N29" s="181"/>
       <c r="O29" s="181"/>
       <c r="P29" s="180" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q29" s="181"/>
       <c r="R29" s="181"/>
       <c r="S29" s="180" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T29" s="181"/>
       <c r="U29" s="181"/>
       <c r="V29" s="180" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W29" s="181"/>
       <c r="X29" s="181"/>
     </row>
     <row r="30" spans="1:35" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="122" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C30" s="141"/>
       <c r="D30" s="141"/>
       <c r="E30" s="142" t="s">
+        <v>199</v>
+      </c>
+      <c r="F30" s="142" t="s">
+        <v>198</v>
+      </c>
+      <c r="G30" s="142" t="s">
         <v>200</v>
       </c>
-      <c r="F30" s="142" t="s">
-        <v>199</v>
-      </c>
-      <c r="G30" s="142" t="s">
-        <v>201</v>
-      </c>
       <c r="H30" s="142" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" s="142" t="s">
+        <v>133</v>
+      </c>
+      <c r="J30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="I30" s="142" t="s">
+      <c r="K30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="J30" s="142" t="s">
-        <v>135</v>
-      </c>
-      <c r="K30" s="142" t="s">
-        <v>135</v>
-      </c>
       <c r="L30" s="142" t="s">
+        <v>132</v>
+      </c>
+      <c r="M30" s="142" t="s">
         <v>133</v>
       </c>
-      <c r="M30" s="142" t="s">
+      <c r="N30" s="142" t="s">
         <v>134</v>
       </c>
-      <c r="N30" s="142" t="s">
-        <v>135</v>
-      </c>
       <c r="O30" s="142" t="s">
+        <v>132</v>
+      </c>
+      <c r="P30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="P30" s="150" t="s">
+      <c r="Q30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="Q30" s="150" t="s">
-        <v>135</v>
-      </c>
       <c r="R30" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="S30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="S30" s="150" t="s">
+      <c r="T30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="T30" s="150" t="s">
-        <v>135</v>
-      </c>
       <c r="U30" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="V30" s="150" t="s">
         <v>133</v>
       </c>
-      <c r="V30" s="150" t="s">
+      <c r="W30" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="W30" s="150" t="s">
-        <v>135</v>
-      </c>
       <c r="X30" s="150" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AA30" s="143" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C31" s="146" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D31" s="146"/>
       <c r="E31" s="146">
@@ -7143,7 +7135,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="C32" s="147" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D32" s="147"/>
       <c r="E32" s="147">
@@ -7182,7 +7174,7 @@
     </row>
     <row r="33" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C33" s="147" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D33" s="147"/>
       <c r="E33" s="147">
@@ -7219,12 +7211,12 @@
       <c r="T33" s="147"/>
       <c r="U33" s="147"/>
       <c r="AA33" s="143" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C34" s="147" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D34" s="147"/>
       <c r="E34" s="147">
@@ -7263,7 +7255,7 @@
     </row>
     <row r="35" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C35" s="147" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D35" s="147"/>
       <c r="E35" s="147">
@@ -7302,7 +7294,7 @@
     </row>
     <row r="36" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C36" s="147" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D36" s="147"/>
       <c r="E36" s="147">
@@ -7341,7 +7333,7 @@
     </row>
     <row r="37" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C37" s="148" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D37" s="148"/>
       <c r="E37" s="148">
@@ -7410,7 +7402,7 @@
     </row>
     <row r="38" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C38" s="146" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D38" s="146"/>
       <c r="E38" s="146">
@@ -7479,7 +7471,7 @@
     </row>
     <row r="39" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C39" s="148" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D39" s="148"/>
       <c r="E39" s="148">
@@ -7550,7 +7542,7 @@
     </row>
     <row r="40" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C40" s="147" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D40" s="147"/>
       <c r="E40" s="147">
@@ -7598,7 +7590,7 @@
     </row>
     <row r="41" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C41" s="146" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" s="146"/>
       <c r="E41" s="146">
@@ -7667,7 +7659,7 @@
     </row>
     <row r="42" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C42" s="148" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D42" s="148"/>
       <c r="E42" s="148">
@@ -7742,7 +7734,7 @@
     </row>
     <row r="43" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C43" s="147" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D43" s="147"/>
       <c r="E43" s="147">
@@ -7790,7 +7782,7 @@
     </row>
     <row r="44" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C44" s="146" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D44" s="146"/>
       <c r="E44" s="146">
@@ -7859,7 +7851,7 @@
     </row>
     <row r="45" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C45" s="147" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D45" s="147"/>
       <c r="E45" s="147">
@@ -7912,7 +7904,7 @@
     </row>
     <row r="46" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C46" s="148" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D46" s="148"/>
       <c r="E46" s="148">
@@ -7987,7 +7979,7 @@
     </row>
     <row r="47" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C47" s="147" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" s="147"/>
       <c r="E47" s="147">
@@ -8035,7 +8027,7 @@
     </row>
     <row r="48" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C48" s="146" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D48" s="146"/>
       <c r="E48" s="146">
@@ -8104,7 +8096,7 @@
     </row>
     <row r="49" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C49" s="147" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D49" s="147"/>
       <c r="E49" s="147">
@@ -8157,7 +8149,7 @@
     </row>
     <row r="50" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C50" s="147" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D50" s="147"/>
       <c r="E50" s="147">
@@ -8209,7 +8201,7 @@
     </row>
     <row r="51" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C51" s="148" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D51" s="148"/>
       <c r="E51" s="148">
@@ -8280,7 +8272,7 @@
     </row>
     <row r="52" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C52" s="147" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D52" s="147"/>
       <c r="E52" s="147">
@@ -8328,7 +8320,7 @@
     </row>
     <row r="53" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C53" s="146" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D53" s="146"/>
       <c r="E53" s="146">
@@ -8397,7 +8389,7 @@
     </row>
     <row r="54" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C54" s="147" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D54" s="147"/>
       <c r="E54" s="147">
@@ -8449,7 +8441,7 @@
     </row>
     <row r="55" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C55" s="147" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D55" s="147"/>
       <c r="E55" s="147">
@@ -8506,7 +8498,7 @@
     </row>
     <row r="56" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C56" s="147" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D56" s="147"/>
       <c r="E56" s="147">
@@ -8560,7 +8552,7 @@
     </row>
     <row r="57" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C57" s="149" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57" s="149"/>
       <c r="E57" s="149"/>
@@ -8654,7 +8646,7 @@
     </row>
     <row r="60" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S60" s="158">
         <f>SUM(S38,S41,S44,S48,S53,S57)</f>

</xml_diff>

<commit_message>
Internal Temperatures Updated in Retrofit savings
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017E8587-D8D2-479E-B68F-8B5B57673F64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6DB148-D2AB-4AA9-818C-8DC02B271D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="224">
   <si>
     <t>Document type:</t>
   </si>
@@ -772,17 +772,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1846,499 +1853,518 @@
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="45" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="27" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="17" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="18" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="18" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="18" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="18" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="18" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="18" borderId="28" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="17" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="23" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="23" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="14"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="38" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="39" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="8"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="8"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="46" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="47" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="10" fontId="41" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="42" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="42" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="42" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="42" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="43" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="43" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="43" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="43" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="15" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="15" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="15" borderId="49" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="10" fillId="15" borderId="49" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="15" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="10" fillId="15" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="29" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3319,15 +3345,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>45242</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>50006</xdr:rowOff>
+      <xdr:colOff>245267</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>78581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>547686</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>116681</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>138111</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>78581</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3344,8 +3370,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="18595180" y="4050506"/>
-          <a:ext cx="7789069" cy="828675"/>
+          <a:off x="19904867" y="4298156"/>
+          <a:ext cx="7817644" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4945,7 +4971,7 @@
   </sheetPr>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
@@ -5143,7 +5169,7 @@
       </c>
       <c r="N7" s="80">
         <f>U7</f>
-        <v>5.9072960538612464E-3</v>
+        <v>3.4901289446216035E-3</v>
       </c>
       <c r="O7" s="161">
         <f>Data!U59/1000</f>
@@ -5160,11 +5186,11 @@
       </c>
       <c r="T7" s="163">
         <f>Data!X59</f>
-        <v>0.36920600336632792</v>
+        <v>0.21813305903885022</v>
       </c>
       <c r="U7" s="85">
         <f>S7*T7</f>
-        <v>5.9072960538612464E-3</v>
+        <v>3.4901289446216035E-3</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5207,7 +5233,7 @@
       </c>
       <c r="N8" s="88">
         <f t="shared" ref="N8:N12" si="4">U8</f>
-        <v>8.1965689357556444E-3</v>
+        <v>5.6512839012265283E-3</v>
       </c>
       <c r="O8" s="162">
         <f>Data!U60/1000</f>
@@ -5224,11 +5250,11 @@
       </c>
       <c r="T8" s="164">
         <f>Data!X60</f>
-        <v>0.51228555848472779</v>
+        <v>0.35320524382665802</v>
       </c>
       <c r="U8" s="86">
         <f t="shared" ref="U8:U12" si="5">S8*T8</f>
-        <v>8.1965689357556444E-3</v>
+        <v>5.6512839012265283E-3</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5271,7 +5297,7 @@
       </c>
       <c r="N9" s="80">
         <f t="shared" si="4"/>
-        <v>9.413814304323951E-3</v>
+        <v>5.4263583940724319E-3</v>
       </c>
       <c r="O9" s="161">
         <f>Data!S59/1000</f>
@@ -5288,11 +5314,11 @@
       </c>
       <c r="T9" s="163">
         <f>Data!V59</f>
-        <v>0.3499559220938272</v>
+        <v>0.20172336037443986</v>
       </c>
       <c r="U9" s="85">
         <f t="shared" si="5"/>
-        <v>9.413814304323951E-3</v>
+        <v>5.4263583940724319E-3</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5335,7 +5361,7 @@
       </c>
       <c r="N10" s="88">
         <f t="shared" si="4"/>
-        <v>1.5328198459374942E-2</v>
+        <v>1.0838038529806422E-2</v>
       </c>
       <c r="O10" s="162">
         <f>Data!S60/1000</f>
@@ -5352,11 +5378,11 @@
       </c>
       <c r="T10" s="164">
         <f>Data!V60</f>
-        <v>0.56982150406598298</v>
+        <v>0.40290106058759934</v>
       </c>
       <c r="U10" s="86">
         <f t="shared" si="5"/>
-        <v>1.5328198459374942E-2</v>
+        <v>1.0838038529806422E-2</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5399,7 +5425,7 @@
       </c>
       <c r="N11" s="80">
         <f t="shared" si="4"/>
-        <v>1.6649605686878701E-2</v>
+        <v>9.5809185652412903E-3</v>
       </c>
       <c r="O11" s="161">
         <f>Data!T59/1000</f>
@@ -5416,11 +5442,11 @@
       </c>
       <c r="T11" s="163">
         <f>Data!W59</f>
-        <v>0.34759093292022342</v>
+        <v>0.2000191767273756</v>
       </c>
       <c r="U11" s="85">
         <f t="shared" si="5"/>
-        <v>1.6649605686878701E-2</v>
+        <v>9.5809185652412903E-3</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5463,7 +5489,7 @@
       </c>
       <c r="N12" s="88">
         <f t="shared" si="4"/>
-        <v>2.7503185042088787E-2</v>
+        <v>1.9597778365928669E-2</v>
       </c>
       <c r="O12" s="162">
         <f>Data!T60/1000</f>
@@ -5480,11 +5506,11 @@
       </c>
       <c r="T12" s="164">
         <f>Data!W60</f>
-        <v>0.57417922843609159</v>
+        <v>0.40913942308828122</v>
       </c>
       <c r="U12" s="86">
         <f t="shared" si="5"/>
-        <v>2.7503185042088787E-2</v>
+        <v>1.9597778365928669E-2</v>
       </c>
     </row>
     <row r="19" spans="22:26" x14ac:dyDescent="0.2">
@@ -5726,10 +5752,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
-  <dimension ref="A1:AI60"/>
+  <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5752,10 +5778,12 @@
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="21" width="12.28515625" customWidth="1"/>
     <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L2" s="183" t="s">
         <v>201</v>
       </c>
@@ -5775,7 +5803,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="3:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="182" t="s">
         <v>190</v>
       </c>
@@ -5826,14 +5854,25 @@
       <c r="AE3" t="s">
         <v>215</v>
       </c>
+      <c r="AF3" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="AH3" s="5" t="s">
         <v>133</v>
       </c>
       <c r="AI3" s="5" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AN3" s="193" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO3" s="193"/>
+      <c r="AP3" s="193"/>
+    </row>
+    <row r="4" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="95" t="s">
         <v>194</v>
       </c>
@@ -5884,8 +5923,17 @@
         <v>54.181824878333337</v>
       </c>
       <c r="Y4" s="127"/>
-    </row>
-    <row r="5" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AN4" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO4" s="94" t="s">
+        <v>192</v>
+      </c>
+      <c r="AP4" s="94" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="97" t="s">
         <v>145</v>
       </c>
@@ -5938,14 +5986,22 @@
       <c r="AA5" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="AB5">
-        <f>AVERAGE(AH5:AI5)</f>
-        <v>235</v>
-      </c>
-      <c r="AC5" s="129">
+      <c r="AB5" s="194">
+        <f>AVERAGE(AH5:AI5)*AO5</f>
+        <v>323.125</v>
+      </c>
+      <c r="AC5" s="195">
+        <f>AF5*AP5</f>
+        <v>539.15574963609902</v>
+      </c>
+      <c r="AD5" s="195">
+        <f>AG5*AN5</f>
+        <v>200</v>
+      </c>
+      <c r="AF5" s="129">
         <v>400</v>
       </c>
-      <c r="AD5" s="129">
+      <c r="AG5" s="129">
         <v>140</v>
       </c>
       <c r="AH5" s="130">
@@ -5954,8 +6010,20 @@
       <c r="AI5" s="129">
         <v>280</v>
       </c>
-    </row>
-    <row r="6" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM5" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN5" s="189">
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AO5" s="189">
+        <v>1.375</v>
+      </c>
+      <c r="AP5" s="189">
+        <v>1.3478893740902476</v>
+      </c>
+    </row>
+    <row r="6" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="102" t="s">
         <v>148</v>
       </c>
@@ -6008,14 +6076,22 @@
       <c r="AA6" s="131" t="s">
         <v>146</v>
       </c>
-      <c r="AB6">
-        <f t="shared" ref="AB6:AB19" si="1">AVERAGE(AH6:AI6)</f>
-        <v>470</v>
-      </c>
-      <c r="AC6" s="132">
+      <c r="AB6" s="194">
+        <f t="shared" ref="AB6:AB19" si="1">AVERAGE(AH6:AI6)*AO6</f>
+        <v>646.25</v>
+      </c>
+      <c r="AC6" s="195">
+        <f t="shared" ref="AC6:AC19" si="2">AF6*AP6</f>
+        <v>1078.311499272198</v>
+      </c>
+      <c r="AD6" s="195">
+        <f t="shared" ref="AD6:AD19" si="3">AG6*AN6</f>
+        <v>400</v>
+      </c>
+      <c r="AF6" s="132">
         <v>800</v>
       </c>
-      <c r="AD6" s="132">
+      <c r="AG6" s="132">
         <v>280</v>
       </c>
       <c r="AH6" s="133">
@@ -6024,8 +6100,20 @@
       <c r="AI6" s="132">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM6" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN6" s="189">
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AO6" s="189">
+        <v>1.375</v>
+      </c>
+      <c r="AP6" s="189">
+        <v>1.3478893740902476</v>
+      </c>
+    </row>
+    <row r="7" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="107" t="s">
         <v>149</v>
       </c>
@@ -6078,14 +6166,22 @@
       <c r="AA7" s="131" t="s">
         <v>147</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="194">
         <f t="shared" si="1"/>
-        <v>585</v>
-      </c>
-      <c r="AC7" s="132">
+        <v>804.375</v>
+      </c>
+      <c r="AC7" s="195">
+        <f t="shared" si="2"/>
+        <v>1213.1004366812228</v>
+      </c>
+      <c r="AD7" s="195">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="AF7" s="132">
         <v>900</v>
       </c>
-      <c r="AD7" s="132">
+      <c r="AG7" s="132">
         <v>350</v>
       </c>
       <c r="AH7" s="133">
@@ -6094,8 +6190,20 @@
       <c r="AI7" s="132">
         <v>700</v>
       </c>
-    </row>
-    <row r="8" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM7" s="97" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN7" s="189">
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="AO7" s="189">
+        <v>1.375</v>
+      </c>
+      <c r="AP7" s="189">
+        <v>1.3478893740902476</v>
+      </c>
+    </row>
+    <row r="8" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C8" s="102" t="s">
         <v>150</v>
       </c>
@@ -6148,14 +6256,22 @@
       <c r="AA8" s="131" t="s">
         <v>148</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="194">
         <f t="shared" si="1"/>
         <v>745</v>
       </c>
-      <c r="AC8" s="134">
+      <c r="AC8" s="195">
+        <f t="shared" si="2"/>
         <v>1200</v>
       </c>
-      <c r="AD8" s="132">
+      <c r="AD8" s="195">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+      <c r="AF8" s="134">
+        <v>1200</v>
+      </c>
+      <c r="AG8" s="132">
         <v>440</v>
       </c>
       <c r="AH8" s="133">
@@ -6164,8 +6280,20 @@
       <c r="AI8" s="132">
         <v>900</v>
       </c>
-    </row>
-    <row r="9" spans="3:35" ht="15" x14ac:dyDescent="0.25">
+      <c r="AM8" s="102" t="s">
+        <v>148</v>
+      </c>
+      <c r="AN8" s="190">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="190">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="107" t="s">
         <v>152</v>
       </c>
@@ -6221,14 +6349,22 @@
       <c r="AA9" s="131" t="s">
         <v>149</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="194">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
-      <c r="AC9" s="134">
+      <c r="AC9" s="195">
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
-      <c r="AD9" s="132">
+      <c r="AD9" s="195">
+        <f t="shared" si="3"/>
+        <v>570</v>
+      </c>
+      <c r="AF9" s="134">
+        <v>1500</v>
+      </c>
+      <c r="AG9" s="132">
         <v>570</v>
       </c>
       <c r="AH9" s="133">
@@ -6237,8 +6373,20 @@
       <c r="AI9" s="134">
         <v>1100</v>
       </c>
-    </row>
-    <row r="10" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM9" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="AN9" s="191">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="191">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="102" t="s">
         <v>156</v>
       </c>
@@ -6291,14 +6439,22 @@
       <c r="AA10" s="131" t="s">
         <v>150</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="194">
         <f t="shared" si="1"/>
         <v>1150</v>
       </c>
-      <c r="AC10" s="134">
+      <c r="AC10" s="195">
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
-      <c r="AD10" s="132">
+      <c r="AD10" s="195">
+        <f t="shared" si="3"/>
+        <v>700</v>
+      </c>
+      <c r="AF10" s="134">
+        <v>1900</v>
+      </c>
+      <c r="AG10" s="132">
         <v>700</v>
       </c>
       <c r="AH10" s="133">
@@ -6307,8 +6463,20 @@
       <c r="AI10" s="134">
         <v>1400</v>
       </c>
-    </row>
-    <row r="11" spans="3:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM10" s="102" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN10" s="190">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="190">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C11" s="107" t="s">
         <v>159</v>
       </c>
@@ -6361,14 +6529,22 @@
       <c r="AA11" s="131" t="s">
         <v>151</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="194">
         <f t="shared" si="1"/>
-        <v>1350</v>
-      </c>
-      <c r="AC11" s="134">
+        <v>862.03259827420902</v>
+      </c>
+      <c r="AC11" s="195">
+        <f t="shared" si="2"/>
+        <v>1432.4324324324325</v>
+      </c>
+      <c r="AD11" s="195">
+        <f t="shared" si="3"/>
+        <v>498.80478087649402</v>
+      </c>
+      <c r="AF11" s="134">
         <v>2200</v>
       </c>
-      <c r="AD11" s="132">
+      <c r="AG11" s="132">
         <v>800</v>
       </c>
       <c r="AH11" s="135">
@@ -6377,8 +6553,20 @@
       <c r="AI11" s="134">
         <v>1600</v>
       </c>
-    </row>
-    <row r="12" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM11" s="107" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN11" s="191">
+        <v>0.62350597609561753</v>
+      </c>
+      <c r="AO11" s="191">
+        <v>0.63854266538830295</v>
+      </c>
+      <c r="AP11" s="191">
+        <v>0.65110565110565111</v>
+      </c>
+    </row>
+    <row r="12" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="102" t="s">
         <v>161</v>
       </c>
@@ -6431,14 +6619,22 @@
       <c r="AA12" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="194">
         <f t="shared" si="1"/>
-        <v>1600</v>
-      </c>
-      <c r="AC12" s="134">
+        <v>1021.6682646212847</v>
+      </c>
+      <c r="AC12" s="195">
+        <f t="shared" si="2"/>
+        <v>1692.874692874693</v>
+      </c>
+      <c r="AD12" s="195">
+        <f t="shared" si="3"/>
+        <v>623.50597609561748</v>
+      </c>
+      <c r="AF12" s="134">
         <v>2600</v>
       </c>
-      <c r="AD12" s="134">
+      <c r="AG12" s="134">
         <v>1000</v>
       </c>
       <c r="AH12" s="135">
@@ -6447,8 +6643,18 @@
       <c r="AI12" s="134">
         <v>1900</v>
       </c>
-    </row>
-    <row r="13" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM12" s="107"/>
+      <c r="AN12" s="191">
+        <v>0.62350597609561753</v>
+      </c>
+      <c r="AO12" s="191">
+        <v>0.63854266538830295</v>
+      </c>
+      <c r="AP12" s="191">
+        <v>0.65110565110565111</v>
+      </c>
+    </row>
+    <row r="13" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="117" t="s">
         <v>162</v>
       </c>
@@ -6476,14 +6682,22 @@
       <c r="AA13" s="131" t="s">
         <v>154</v>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="194">
         <f t="shared" si="1"/>
-        <v>1850</v>
-      </c>
-      <c r="AC13" s="134">
+        <v>1181.3039309683604</v>
+      </c>
+      <c r="AC13" s="195">
+        <f t="shared" si="2"/>
+        <v>1888.2063882063883</v>
+      </c>
+      <c r="AD13" s="195">
+        <f t="shared" si="3"/>
+        <v>685.85657370517924</v>
+      </c>
+      <c r="AF13" s="134">
         <v>2900</v>
       </c>
-      <c r="AD13" s="134">
+      <c r="AG13" s="134">
         <v>1100</v>
       </c>
       <c r="AH13" s="135">
@@ -6492,8 +6706,18 @@
       <c r="AI13" s="134">
         <v>2200</v>
       </c>
-    </row>
-    <row r="14" spans="3:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM13" s="107"/>
+      <c r="AN13" s="191">
+        <v>0.62350597609561753</v>
+      </c>
+      <c r="AO13" s="191">
+        <v>0.63854266538830295</v>
+      </c>
+      <c r="AP13" s="191">
+        <v>0.65110565110565111</v>
+      </c>
+    </row>
+    <row r="14" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C14" s="120" t="s">
         <v>197</v>
       </c>
@@ -6502,11 +6726,11 @@
         <v>766351.72099999979</v>
       </c>
       <c r="E14" s="145">
-        <f t="shared" ref="E14:F14" si="2">SUM(E5:E13)</f>
+        <f t="shared" ref="E14:F14" si="4">SUM(E5:E13)</f>
         <v>724429.72899999993</v>
       </c>
       <c r="F14" s="145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>206798.88499999998</v>
       </c>
       <c r="G14" s="121">
@@ -6515,14 +6739,22 @@
       <c r="AA14" s="131" t="s">
         <v>155</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="194">
         <f t="shared" si="1"/>
-        <v>2150</v>
-      </c>
-      <c r="AC14" s="134">
+        <v>1433.8643942200815</v>
+      </c>
+      <c r="AC14" s="195">
+        <f t="shared" si="2"/>
+        <v>2364.0040444893834</v>
+      </c>
+      <c r="AD14" s="195">
+        <f t="shared" si="3"/>
+        <v>835.58106169296991</v>
+      </c>
+      <c r="AF14" s="134">
         <v>3500</v>
       </c>
-      <c r="AD14" s="134">
+      <c r="AG14" s="134">
         <v>1300</v>
       </c>
       <c r="AH14" s="135">
@@ -6531,22 +6763,42 @@
       <c r="AI14" s="134">
         <v>2600</v>
       </c>
-    </row>
-    <row r="15" spans="3:35" x14ac:dyDescent="0.2">
+      <c r="AM14" s="102" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN14" s="190">
+        <v>0.64275466284074612</v>
+      </c>
+      <c r="AO14" s="190">
+        <v>0.6669136717302705</v>
+      </c>
+      <c r="AP14" s="190">
+        <v>0.67542972699696668</v>
+      </c>
+    </row>
+    <row r="15" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L15" t="s">
         <v>211</v>
       </c>
       <c r="AA15" s="131" t="s">
         <v>157</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="194">
         <f t="shared" si="1"/>
-        <v>2550</v>
-      </c>
-      <c r="AC15" s="134">
+        <v>1700.6298629121898</v>
+      </c>
+      <c r="AC15" s="195">
+        <f t="shared" si="2"/>
+        <v>2769.2618806875635</v>
+      </c>
+      <c r="AD15" s="195">
+        <f t="shared" si="3"/>
+        <v>964.13199426111919</v>
+      </c>
+      <c r="AF15" s="134">
         <v>4100</v>
       </c>
-      <c r="AD15" s="134">
+      <c r="AG15" s="134">
         <v>1500</v>
       </c>
       <c r="AH15" s="135">
@@ -6555,22 +6807,40 @@
       <c r="AI15" s="134">
         <v>3100</v>
       </c>
-    </row>
-    <row r="16" spans="3:35" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM15" s="102"/>
+      <c r="AN15" s="190">
+        <v>0.64275466284074612</v>
+      </c>
+      <c r="AO15" s="190">
+        <v>0.6669136717302705</v>
+      </c>
+      <c r="AP15" s="190">
+        <v>0.67542972699696668</v>
+      </c>
+    </row>
+    <row r="16" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L16" s="5" t="s">
         <v>214</v>
       </c>
       <c r="AA16" s="131" t="s">
         <v>158</v>
       </c>
-      <c r="AB16">
+      <c r="AB16" s="194">
         <f t="shared" si="1"/>
-        <v>2900</v>
-      </c>
-      <c r="AC16" s="134">
+        <v>1978.8338900698452</v>
+      </c>
+      <c r="AC16" s="195">
+        <f t="shared" si="2"/>
+        <v>3233.030303030303</v>
+      </c>
+      <c r="AD16" s="195">
+        <f t="shared" si="3"/>
+        <v>1187.0601589103292</v>
+      </c>
+      <c r="AF16" s="134">
         <v>4700</v>
       </c>
-      <c r="AD16" s="134">
+      <c r="AG16" s="134">
         <v>1800</v>
       </c>
       <c r="AH16" s="135">
@@ -6579,8 +6849,20 @@
       <c r="AI16" s="134">
         <v>3500</v>
       </c>
-    </row>
-    <row r="17" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM16" s="107" t="s">
+        <v>159</v>
+      </c>
+      <c r="AN16" s="191">
+        <v>0.65947786606129399</v>
+      </c>
+      <c r="AO16" s="191">
+        <v>0.68235651381718798</v>
+      </c>
+      <c r="AP16" s="191">
+        <v>0.68787878787878787</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F17" s="94" t="s">
         <v>192</v>
       </c>
@@ -6623,14 +6905,22 @@
       <c r="AA17" s="131" t="s">
         <v>160</v>
       </c>
-      <c r="AB17">
+      <c r="AB17" s="194">
         <f t="shared" si="1"/>
-        <v>3300</v>
-      </c>
-      <c r="AC17" s="134">
+        <v>2251.7764955967205</v>
+      </c>
+      <c r="AC17" s="195">
+        <f t="shared" si="2"/>
+        <v>3645.7575757575755</v>
+      </c>
+      <c r="AD17" s="195">
+        <f t="shared" si="3"/>
+        <v>1318.955732122588</v>
+      </c>
+      <c r="AF17" s="134">
         <v>5300</v>
       </c>
-      <c r="AD17" s="134">
+      <c r="AG17" s="134">
         <v>2000</v>
       </c>
       <c r="AH17" s="135">
@@ -6639,8 +6929,18 @@
       <c r="AI17" s="134">
         <v>4000</v>
       </c>
-    </row>
-    <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM17" s="107"/>
+      <c r="AN17" s="191">
+        <v>0.65947786606129399</v>
+      </c>
+      <c r="AO17" s="191">
+        <v>0.68235651381718798</v>
+      </c>
+      <c r="AP17" s="191">
+        <v>0.68787878787878787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>220</v>
       </c>
@@ -6697,14 +6997,22 @@
       <c r="AA18" s="131" t="s">
         <v>161</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="194">
         <f t="shared" si="1"/>
-        <v>3950</v>
-      </c>
-      <c r="AC18" s="134">
+        <v>2739.9647887323945</v>
+      </c>
+      <c r="AC18" s="195">
+        <f t="shared" si="2"/>
+        <v>4403.3907830648186</v>
+      </c>
+      <c r="AD18" s="195">
+        <f t="shared" si="3"/>
+        <v>1626.2626262626261</v>
+      </c>
+      <c r="AF18" s="134">
         <v>6300</v>
       </c>
-      <c r="AD18" s="134">
+      <c r="AG18" s="134">
         <v>2400</v>
       </c>
       <c r="AH18" s="135">
@@ -6713,8 +7021,20 @@
       <c r="AI18" s="134">
         <v>4700</v>
       </c>
-    </row>
-    <row r="19" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AM18" s="102" t="s">
+        <v>161</v>
+      </c>
+      <c r="AN18" s="190">
+        <v>0.67760942760942755</v>
+      </c>
+      <c r="AO18" s="190">
+        <v>0.69366197183098599</v>
+      </c>
+      <c r="AP18" s="190">
+        <v>0.69895091794679653</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>221</v>
       </c>
@@ -6723,38 +7043,38 @@
         <v>282151.52747564798</v>
       </c>
       <c r="G19" s="145">
-        <f t="shared" ref="G19:H19" si="3">E9</f>
+        <f t="shared" ref="G19:H19" si="5">E9</f>
         <v>251318.93361374349</v>
       </c>
       <c r="H19" s="145">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>58904.8034364337</v>
       </c>
       <c r="O19" s="102" t="s">
         <v>148</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P25" si="4">1-U5/$U$12</f>
+        <f t="shared" ref="P19:P25" si="6">1-U5/$U$12</f>
         <v>0.85617788946237794</v>
       </c>
       <c r="Q19" s="124">
-        <f t="shared" ref="Q19:Q24" si="5">1-U5/$U$11</f>
+        <f t="shared" ref="Q19:Q24" si="7">1-U5/$U$11</f>
         <v>0.78212006063973538</v>
       </c>
       <c r="R19" s="124">
-        <f t="shared" ref="R19:R23" si="6">1-U5/$U$10</f>
+        <f t="shared" ref="R19:R23" si="8">1-U5/$U$10</f>
         <v>0.73310283124232423</v>
       </c>
       <c r="S19" s="124">
-        <f t="shared" ref="S19:S22" si="7">1-U5/$U$9</f>
+        <f t="shared" ref="S19:S22" si="9">1-U5/$U$9</f>
         <v>0.65413592759164874</v>
       </c>
       <c r="T19" s="124">
-        <f t="shared" ref="T19:T21" si="8">1-U5/$U$8</f>
+        <f t="shared" ref="T19:T21" si="10">1-U5/$U$8</f>
         <v>0.5229019792936962</v>
       </c>
       <c r="U19" s="124">
-        <f t="shared" ref="U19:U20" si="9">1-U5/$U$7</f>
+        <f t="shared" ref="U19:U20" si="11">1-U5/$U$7</f>
         <v>0.35452784716650365</v>
       </c>
       <c r="V19" s="93">
@@ -6764,14 +7084,22 @@
       <c r="AA19" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="194">
         <f t="shared" si="1"/>
-        <v>4950</v>
-      </c>
-      <c r="AC19" s="137">
+        <v>2702.039715087416</v>
+      </c>
+      <c r="AC19" s="195">
+        <f t="shared" si="2"/>
+        <v>4397.9254406488853</v>
+      </c>
+      <c r="AD19" s="195">
+        <f t="shared" si="3"/>
+        <v>1686.5833785985876</v>
+      </c>
+      <c r="AF19" s="137">
         <v>7900</v>
       </c>
-      <c r="AD19" s="137">
+      <c r="AG19" s="137">
         <v>3000</v>
       </c>
       <c r="AH19" s="138">
@@ -6780,8 +7108,20 @@
       <c r="AI19" s="137">
         <v>5900</v>
       </c>
-    </row>
-    <row r="20" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+      <c r="AM19" s="113" t="s">
+        <v>162</v>
+      </c>
+      <c r="AN19" s="192">
+        <v>0.56219445953286251</v>
+      </c>
+      <c r="AO19" s="192">
+        <v>0.54586660910856888</v>
+      </c>
+      <c r="AP19" s="192">
+        <v>0.55669942286694751</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>222</v>
       </c>
@@ -6790,45 +7130,45 @@
         <v>391876.39875986642</v>
       </c>
       <c r="G20" s="145">
-        <f t="shared" ref="G20:H20" si="10">SUM(E10:E13)</f>
+        <f t="shared" ref="G20:H20" si="12">SUM(E10:E13)</f>
         <v>369741.02860841871</v>
       </c>
       <c r="H20" s="145">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>97049.563561422125</v>
       </c>
       <c r="O20" s="107" t="s">
         <v>149</v>
       </c>
       <c r="P20" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.81571341691508692</v>
       </c>
       <c r="Q20" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.72081935526215313</v>
       </c>
       <c r="R20" s="124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.658011086879975</v>
       </c>
       <c r="S20" s="124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.55682677804053693</v>
       </c>
       <c r="T20" s="124">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.388670047297489</v>
       </c>
       <c r="U20" s="93">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.17292371056513256</v>
       </c>
       <c r="Y20" s="139" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F21" s="145">
         <f>SUM(F18:F20)</f>
         <v>766351.7209999999</v>
@@ -6838,30 +7178,30 @@
         <v>150</v>
       </c>
       <c r="P21" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.77718309007403152</v>
       </c>
       <c r="Q21" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.66244873864222598</v>
       </c>
       <c r="R21" s="124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.58650862382513413</v>
       </c>
       <c r="S21" s="124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.46416887097285942</v>
       </c>
       <c r="T21" s="93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.26085421561265365</v>
       </c>
       <c r="Y21" s="140" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="F22" s="94" t="s">
         <v>192</v>
       </c>
@@ -6875,23 +7215,23 @@
         <v>152</v>
       </c>
       <c r="P22" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.69854808803292578</v>
       </c>
       <c r="Q22" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.54332248321275467</v>
       </c>
       <c r="R22" s="124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.44058210855170443</v>
       </c>
       <c r="S22" s="93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.27506705666829534</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>220</v>
       </c>
@@ -6911,81 +7251,81 @@
         <v>156</v>
       </c>
       <c r="P23" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.58416579803693625</v>
       </c>
       <c r="Q23" s="124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.37004171077063985</v>
       </c>
       <c r="R23" s="93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.22831774084196221</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>221</v>
       </c>
       <c r="F24" s="165">
-        <f t="shared" ref="F24:F25" si="11">F19/$D$14</f>
+        <f t="shared" ref="F24:F25" si="13">F19/$D$14</f>
         <v>0.36817497729041837</v>
       </c>
       <c r="G24" s="165">
-        <f t="shared" ref="G24:G25" si="12">G19/$E$14</f>
+        <f t="shared" ref="G24:G25" si="14">G19/$E$14</f>
         <v>0.34691968530979972</v>
       </c>
       <c r="H24" s="165">
-        <f t="shared" ref="H24:H25" si="13">H19/$F$14</f>
+        <f t="shared" ref="H24:H25" si="15">H19/$F$14</f>
         <v>0.28484101080348528</v>
       </c>
       <c r="O24" s="107" t="s">
         <v>159</v>
       </c>
       <c r="P24" s="124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.46113287298224337</v>
       </c>
       <c r="Q24" s="93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.18365586126511313</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>222</v>
       </c>
       <c r="F25" s="165">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.51135319204152541</v>
       </c>
       <c r="G25" s="165">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.5103890878675118</v>
       </c>
       <c r="H25" s="165">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.46929442371714014</v>
       </c>
       <c r="O25" s="102" t="s">
         <v>161</v>
       </c>
       <c r="P25" s="93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.33990200768409362</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C27" s="92"/>
     </row>
-    <row r="28" spans="1:35" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C28" s="91"/>
       <c r="H28" s="144"/>
       <c r="I28" s="144"/>
       <c r="J28" s="144"/>
     </row>
-    <row r="29" spans="1:35" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="123" t="s">
         <v>204</v>
       </c>
@@ -7024,7 +7364,7 @@
       <c r="W29" s="181"/>
       <c r="X29" s="181"/>
     </row>
-    <row r="30" spans="1:35" ht="21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="122" t="s">
         <v>203</v>
       </c>
@@ -7094,7 +7434,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C31" s="146" t="s">
         <v>163</v>
       </c>
@@ -7106,7 +7446,7 @@
         <v>6086</v>
       </c>
       <c r="G31" s="146">
-        <f t="shared" ref="G31:G56" si="14">SUM(E31:F31)</f>
+        <f t="shared" ref="G31:G56" si="16">SUM(E31:F31)</f>
         <v>21064</v>
       </c>
       <c r="H31" s="146"/>
@@ -7115,7 +7455,7 @@
       <c r="K31" s="146"/>
       <c r="L31" s="146"/>
       <c r="M31" s="146">
-        <f t="shared" ref="M31:M44" si="15">AVERAGE(G31:I31)</f>
+        <f t="shared" ref="M31:M44" si="17">AVERAGE(G31:I31)</f>
         <v>21064</v>
       </c>
       <c r="N31" s="146">
@@ -7133,7 +7473,7 @@
       <c r="T31" s="146"/>
       <c r="U31" s="146"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C32" s="147" t="s">
         <v>164</v>
       </c>
@@ -7145,7 +7485,7 @@
         <v>6086</v>
       </c>
       <c r="G32" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30424</v>
       </c>
       <c r="H32" s="147"/>
@@ -7154,15 +7494,15 @@
       <c r="K32" s="147"/>
       <c r="L32" s="147"/>
       <c r="M32" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="N32" s="147">
-        <f t="shared" ref="N32:N57" si="16">AVERAGE(G32*1.1,J32:K32)</f>
+        <f t="shared" ref="N32:N57" si="18">AVERAGE(G32*1.1,J32:K32)</f>
         <v>33466.400000000001</v>
       </c>
       <c r="O32" s="147">
-        <f t="shared" ref="O32:O57" si="17">AVERAGE(G32*0.9,L32)</f>
+        <f t="shared" ref="O32:O57" si="19">AVERAGE(G32*0.9,L32)</f>
         <v>27381.600000000002</v>
       </c>
       <c r="P32" s="152"/>
@@ -7184,7 +7524,7 @@
         <v>6086</v>
       </c>
       <c r="G33" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30424</v>
       </c>
       <c r="H33" s="147"/>
@@ -7193,15 +7533,15 @@
       <c r="K33" s="147"/>
       <c r="L33" s="147"/>
       <c r="M33" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="N33" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O33" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P33" s="152"/>
@@ -7226,7 +7566,7 @@
         <v>6086</v>
       </c>
       <c r="G34" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32297</v>
       </c>
       <c r="H34" s="147"/>
@@ -7235,15 +7575,15 @@
       <c r="K34" s="147"/>
       <c r="L34" s="147"/>
       <c r="M34" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>32297</v>
       </c>
       <c r="N34" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>35526.700000000004</v>
       </c>
       <c r="O34" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>29067.3</v>
       </c>
       <c r="P34" s="152"/>
@@ -7265,7 +7605,7 @@
         <v>6086</v>
       </c>
       <c r="G35" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>34169</v>
       </c>
       <c r="H35" s="147"/>
@@ -7274,15 +7614,15 @@
       <c r="K35" s="147"/>
       <c r="L35" s="147"/>
       <c r="M35" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>34169</v>
       </c>
       <c r="N35" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>37585.9</v>
       </c>
       <c r="O35" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>30752.100000000002</v>
       </c>
       <c r="P35" s="152"/>
@@ -7304,7 +7644,7 @@
         <v>6086</v>
       </c>
       <c r="G36" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>36041</v>
       </c>
       <c r="H36" s="147"/>
@@ -7313,15 +7653,15 @@
       <c r="K36" s="147"/>
       <c r="L36" s="147"/>
       <c r="M36" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>36041</v>
       </c>
       <c r="N36" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>39645.100000000006</v>
       </c>
       <c r="O36" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>32436.9</v>
       </c>
       <c r="P36" s="152"/>
@@ -7343,7 +7683,7 @@
         <v>6086</v>
       </c>
       <c r="G37" s="148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>21064</v>
       </c>
       <c r="H37" s="148"/>
@@ -7352,11 +7692,11 @@
       <c r="K37" s="148"/>
       <c r="L37" s="148"/>
       <c r="M37" s="148">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>21064</v>
       </c>
       <c r="N37" s="148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>23170.400000000001</v>
       </c>
       <c r="O37" s="148">
@@ -7365,15 +7705,15 @@
       </c>
       <c r="P37" s="153">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$8:$AB$10))</f>
-        <v>0.5465729349736379</v>
+        <v>0.37653778558875217</v>
       </c>
       <c r="Q37" s="153">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$8:$AC$10))</f>
-        <v>0.54347826086956519</v>
+        <v>0.38465919878488697</v>
       </c>
       <c r="R37" s="153">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$8:$AD$10))</f>
-        <v>0.54970760233918126</v>
+        <v>0.35672514619883033</v>
       </c>
       <c r="S37" s="148">
         <f>SUM(D6:D8)/SUM(D6:D13)*M37</f>
@@ -7389,15 +7729,15 @@
       </c>
       <c r="V37" s="153">
         <f>SUM(D6:D8)/SUM(D6:D13)*P37</f>
-        <v>5.5941149660532832E-2</v>
+        <v>3.8538235738807589E-2</v>
       </c>
       <c r="W37" s="153">
         <f>SUM(E6:E8)/SUM(E6:E13)*Q37</f>
-        <v>6.4063307550126458E-2</v>
+        <v>4.5342274618884251E-2</v>
       </c>
       <c r="X37" s="153">
         <f>SUM(F6:F8)/SUM(F6:F13)*R37</f>
-        <v>0.11537126038340646</v>
+        <v>7.4868583865827593E-2</v>
       </c>
     </row>
     <row r="38" spans="3:27" x14ac:dyDescent="0.2">
@@ -7412,7 +7752,7 @@
         <v>6086</v>
       </c>
       <c r="G38" s="146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30424</v>
       </c>
       <c r="H38" s="146"/>
@@ -7421,52 +7761,52 @@
       <c r="K38" s="146"/>
       <c r="L38" s="146"/>
       <c r="M38" s="146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="N38" s="146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O38" s="146">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P38" s="154">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$11:$AB$13))</f>
-        <v>0.73124999999999996</v>
+        <v>0.42128964902402399</v>
       </c>
       <c r="Q38" s="154">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$11:$AC$13))</f>
-        <v>0.72727272727272729</v>
+        <v>0.43541237538106614</v>
       </c>
       <c r="R38" s="154">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$11:$AD$13))</f>
-        <v>0.73448275862068968</v>
+        <v>0.39164922331166674</v>
       </c>
       <c r="S38" s="146">
         <f>SUM(D9)/SUM(D6:D13)*M38</f>
         <v>11432.162401919726</v>
       </c>
       <c r="T38" s="146">
-        <f t="shared" ref="T38:U38" si="18">SUM(E9)/SUM(E6:E13)*N38</f>
+        <f t="shared" ref="T38:U38" si="20">SUM(E9)/SUM(E6:E13)*N38</f>
         <v>11946.208000785055</v>
       </c>
       <c r="U38" s="146">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8171.5871871879508</v>
       </c>
       <c r="V38" s="154">
         <f>SUM(D9)/SUM(D6:D13)*P37</f>
-        <v>0.20538096756220545</v>
+        <v>0.1414883353704261</v>
       </c>
       <c r="W38" s="154">
-        <f t="shared" ref="W38:X38" si="19">SUM(E9)/SUM(E6:E13)*Q37</f>
-        <v>0.19400067973408391</v>
+        <f t="shared" ref="W38:X38" si="21">SUM(E9)/SUM(E6:E13)*Q37</f>
+        <v>0.13730842869563459</v>
       </c>
       <c r="X38" s="154">
-        <f t="shared" si="19"/>
-        <v>0.16405117304959033</v>
+        <f t="shared" si="21"/>
+        <v>0.10645873995771285</v>
       </c>
     </row>
     <row r="39" spans="3:27" x14ac:dyDescent="0.2">
@@ -7481,7 +7821,7 @@
         <v>5326</v>
       </c>
       <c r="G39" s="148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>12815</v>
       </c>
       <c r="H39" s="148">
@@ -7496,7 +7836,7 @@
         <v>9007.5</v>
       </c>
       <c r="N39" s="148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>14096.500000000002</v>
       </c>
       <c r="O39" s="148">
@@ -7505,15 +7845,15 @@
       </c>
       <c r="P39" s="153">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$11:$AB$13))</f>
-        <v>0.40729166666666661</v>
+        <v>7.1779592092092059E-2</v>
       </c>
       <c r="Q39" s="153">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$11:$AC$13))</f>
-        <v>0.40259740259740262</v>
+        <v>8.2479784366576991E-2</v>
       </c>
       <c r="R39" s="153">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$11:$AD$13))</f>
-        <v>0.41034482758620683</v>
+        <v>5.4291065329954646E-2</v>
       </c>
       <c r="S39" s="148">
         <f>D9/SUM(D6:D13)*M39</f>
@@ -7529,15 +7869,15 @@
       </c>
       <c r="V39" s="153">
         <f>D9/SUM(D6:D13)*P39</f>
-        <v>0.15304445432165026</v>
+        <v>2.6971994278870277E-2</v>
       </c>
       <c r="W39" s="153">
-        <f t="shared" ref="W39:X39" si="20">E9/SUM(E6:E13)*Q39</f>
-        <v>0.14371167236405388</v>
+        <f t="shared" ref="W39:X39" si="22">E9/SUM(E6:E13)*Q39</f>
+        <v>2.9442086985843354E-2</v>
       </c>
       <c r="X39" s="153">
-        <f t="shared" si="20"/>
-        <v>0.12246065005084789</v>
+        <f t="shared" si="22"/>
+        <v>1.6202273564329378E-2</v>
       </c>
     </row>
     <row r="40" spans="3:27" x14ac:dyDescent="0.2">
@@ -7552,7 +7892,7 @@
         <v>6086</v>
       </c>
       <c r="G40" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>30424</v>
       </c>
       <c r="H40" s="147"/>
@@ -7561,28 +7901,28 @@
       <c r="K40" s="147"/>
       <c r="L40" s="147"/>
       <c r="M40" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30424</v>
       </c>
       <c r="N40" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>33466.400000000001</v>
       </c>
       <c r="O40" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>27381.600000000002</v>
       </c>
       <c r="P40" s="155">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$14:$AB$15))</f>
-        <v>0.81702127659574475</v>
+        <v>0.62274615839243497</v>
       </c>
       <c r="Q40" s="155">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$14:$AC$15))</f>
-        <v>0.81578947368421051</v>
+        <v>0.63238897979724307</v>
       </c>
       <c r="R40" s="155">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$14:$AD$15))</f>
-        <v>0.81666666666666665</v>
+        <v>0.59252763605442182</v>
       </c>
       <c r="S40" s="147"/>
       <c r="T40" s="147"/>
@@ -7600,7 +7940,7 @@
         <v>5326</v>
       </c>
       <c r="G41" s="146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>12815</v>
       </c>
       <c r="H41" s="146"/>
@@ -7609,52 +7949,52 @@
       <c r="K41" s="146"/>
       <c r="L41" s="146"/>
       <c r="M41" s="146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>12815</v>
       </c>
       <c r="N41" s="146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>14096.500000000002</v>
       </c>
       <c r="O41" s="146">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>11533.5</v>
       </c>
       <c r="P41" s="154">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$14:$AB$15))</f>
-        <v>0.59645390070921978</v>
+        <v>0.39490504334121357</v>
       </c>
       <c r="Q41" s="154">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$14:$AC$15))</f>
-        <v>0.59649122807017552</v>
+        <v>0.40258955772665206</v>
       </c>
       <c r="R41" s="154">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$14:$AD$15))</f>
-        <v>0.59285714285714286</v>
+        <v>0.36656568877551032</v>
       </c>
       <c r="S41" s="146">
         <f>SUM(D10)/SUM(D6:D13)*M41</f>
         <v>3202.1646884279426</v>
       </c>
       <c r="T41" s="146">
-        <f t="shared" ref="T41:U41" si="21">SUM(E10)/SUM(E6:E13)*N41</f>
+        <f t="shared" ref="T41:U41" si="23">SUM(E10)/SUM(E6:E13)*N41</f>
         <v>3337.0202528302325</v>
       </c>
       <c r="U41" s="146">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2555.819902348102</v>
       </c>
       <c r="V41" s="154">
         <f>SUM(D10)/SUM(D6:D13)*P41</f>
-        <v>0.14903968935826528</v>
+        <v>9.8677408120900534E-2</v>
       </c>
       <c r="W41" s="154">
-        <f t="shared" ref="W41:X41" si="22">SUM(E10)/SUM(E6:E13)*Q41</f>
-        <v>0.14120549843619004</v>
+        <f t="shared" ref="W41:X41" si="24">SUM(E10)/SUM(E6:E13)*Q41</f>
+        <v>9.5303763892583535E-2</v>
       </c>
       <c r="X41" s="154">
-        <f t="shared" si="22"/>
-        <v>0.13137695278653641</v>
+        <f t="shared" si="24"/>
+        <v>8.1230839111318301E-2</v>
       </c>
     </row>
     <row r="42" spans="3:27" x14ac:dyDescent="0.2">
@@ -7669,7 +8009,7 @@
         <v>4565</v>
       </c>
       <c r="G42" s="148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8309</v>
       </c>
       <c r="H42" s="148">
@@ -7684,28 +8024,28 @@
       <c r="K42" s="148"/>
       <c r="L42" s="148"/>
       <c r="M42" s="148">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>7536.333333333333</v>
       </c>
       <c r="N42" s="148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>19569.95</v>
       </c>
       <c r="O42" s="148">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>7478.1</v>
       </c>
       <c r="P42" s="153">
         <f>1-(AVERAGE(AB11:AB13)/AVERAGE($AB$14:$AB$15))</f>
-        <v>0.31914893617021278</v>
+        <v>0.34811284959507149</v>
       </c>
       <c r="Q42" s="153">
         <f>1-(AVERAGE(AC11:AC13)/AVERAGE($AC$14:$AC$15))</f>
-        <v>0.32456140350877194</v>
+        <v>0.34888579881488802</v>
       </c>
       <c r="R42" s="153">
         <f>1-(AVERAGE(AD11:AD13)/AVERAGE($AD$14:$AD$15))</f>
-        <v>0.30952380952380953</v>
+        <v>0.33020162123614405</v>
       </c>
       <c r="S42" s="148">
         <f>D10/SUM(D6:D13)*M42</f>
@@ -7721,15 +8061,15 @@
       </c>
       <c r="V42" s="153">
         <f>D10/SUM(D6:D13)*P42</f>
-        <v>7.9747752926539114E-2</v>
+        <v>8.6985148229525189E-2</v>
       </c>
       <c r="W42" s="153">
-        <f t="shared" ref="W42:X42" si="23">E10/SUM(E6:E13)*Q42</f>
-        <v>7.6832403560868096E-2</v>
+        <f t="shared" ref="W42:X42" si="25">E10/SUM(E6:E13)*Q42</f>
+        <v>8.2590641405322962E-2</v>
       </c>
       <c r="X42" s="153">
-        <f t="shared" si="23"/>
-        <v>6.8590376956826238E-2</v>
+        <f t="shared" si="25"/>
+        <v>7.3172573402951982E-2</v>
       </c>
     </row>
     <row r="43" spans="3:27" x14ac:dyDescent="0.2">
@@ -7744,7 +8084,7 @@
         <v>6086</v>
       </c>
       <c r="G43" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32297</v>
       </c>
       <c r="H43" s="147"/>
@@ -7753,28 +8093,28 @@
       <c r="K43" s="147"/>
       <c r="L43" s="147"/>
       <c r="M43" s="147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>32297</v>
       </c>
       <c r="N43" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>35526.700000000004</v>
       </c>
       <c r="O43" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>29067.3</v>
       </c>
       <c r="P43" s="155">
         <f>1-(AVERAGE(AB5:AB7)/AVERAGE($AB$16:$AB$17))</f>
-        <v>0.8612903225806452</v>
+        <v>0.72048950572088954</v>
       </c>
       <c r="Q43" s="155">
         <f>1-(AVERAGE(AC5:AC7)/AVERAGE($AC$16:$AC$17))</f>
-        <v>0.86</v>
+        <v>0.72567185426004643</v>
       </c>
       <c r="R43" s="155">
         <f>1-(AVERAGE(AD5:AD7)/AVERAGE($AD$16:$AD$17))</f>
-        <v>0.86491228070175441</v>
+        <v>0.70737083673038015</v>
       </c>
       <c r="S43" s="147"/>
       <c r="T43" s="147"/>
@@ -7792,7 +8132,7 @@
         <v>5326</v>
       </c>
       <c r="G44" s="146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>20304</v>
       </c>
       <c r="H44" s="146"/>
@@ -7801,52 +8141,52 @@
       <c r="K44" s="146"/>
       <c r="L44" s="146"/>
       <c r="M44" s="146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>20304</v>
       </c>
       <c r="N44" s="146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>22334.400000000001</v>
       </c>
       <c r="O44" s="146">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>18273.600000000002</v>
       </c>
       <c r="P44" s="154">
         <f>1-(AVERAGE(AB8:AB10)/AVERAGE($AB$16:$AB$17))</f>
-        <v>0.69408602150537635</v>
+        <v>0.55168013743533795</v>
       </c>
       <c r="Q44" s="154">
         <f>1-(AVERAGE(AC8:AC10)/AVERAGE($AC$16:$AC$17))</f>
-        <v>0.69333333333333336</v>
+        <v>0.55418502202643172</v>
       </c>
       <c r="R44" s="154">
         <f>1-(AVERAGE(AD8:AD10)/AVERAGE($AD$16:$AD$17))</f>
-        <v>0.7</v>
+        <v>0.5450946643717729</v>
       </c>
       <c r="S44" s="146">
         <f>SUM(D11)/SUM(D6:D13)*M44</f>
         <v>2742.3958967170497</v>
       </c>
       <c r="T44" s="146">
-        <f t="shared" ref="T44:U44" si="24">SUM(E11)/SUM(E6:E13)*N44</f>
+        <f t="shared" ref="T44:U44" si="26">SUM(E11)/SUM(E6:E13)*N44</f>
         <v>2582.1231033841427</v>
       </c>
       <c r="U44" s="146">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>2385.6110070402383</v>
       </c>
       <c r="V44" s="154">
         <f>SUM(D11)/SUM(D6:D13)*P44</f>
-        <v>9.3747963817228427E-2</v>
+        <v>7.4513659633715965E-2</v>
       </c>
       <c r="W44" s="154">
-        <f t="shared" ref="W44:X44" si="25">SUM(E11)/SUM(E6:E13)*Q44</f>
-        <v>8.0157605234362189E-2</v>
+        <f t="shared" ref="W44:X44" si="27">SUM(E11)/SUM(E6:E13)*Q44</f>
+        <v>6.4070400320756282E-2</v>
       </c>
       <c r="X44" s="154">
-        <f t="shared" si="25"/>
-        <v>9.1384713736109291E-2</v>
+        <f t="shared" si="27"/>
+        <v>7.1161885518135765E-2</v>
       </c>
     </row>
     <row r="45" spans="3:27" x14ac:dyDescent="0.2">
@@ -7861,7 +8201,7 @@
         <v>4565</v>
       </c>
       <c r="G45" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>13926</v>
       </c>
       <c r="H45" s="147">
@@ -7875,28 +8215,28 @@
       </c>
       <c r="L45" s="147"/>
       <c r="M45" s="147">
-        <f t="shared" ref="M45:M57" si="26">AVERAGE(G45:I45)</f>
+        <f t="shared" ref="M45:M57" si="28">AVERAGE(G45:I45)</f>
         <v>19363</v>
       </c>
       <c r="N45" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>15409.3</v>
       </c>
       <c r="O45" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>12533.4</v>
       </c>
       <c r="P45" s="155">
         <f>1-(AVERAGE(AB11:AB13)/AVERAGE($AB$16:$AB$17))</f>
-        <v>0.4838709677419355</v>
+        <v>0.51701141372756654</v>
       </c>
       <c r="Q45" s="155">
         <f>1-(AVERAGE(AC11:AC13)/AVERAGE($AC$16:$AC$17))</f>
-        <v>0.48666666666666669</v>
+        <v>0.51410882247886636</v>
       </c>
       <c r="R45" s="155">
         <f>1-(AVERAGE(AD11:AD13)/AVERAGE($AD$16:$AD$17))</f>
-        <v>0.49122807017543857</v>
+        <v>0.51897955179312949</v>
       </c>
       <c r="S45" s="147"/>
       <c r="T45" s="147"/>
@@ -7914,7 +8254,7 @@
         <v>3804</v>
       </c>
       <c r="G46" s="148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>13165</v>
       </c>
       <c r="H46" s="148">
@@ -7929,28 +8269,28 @@
       </c>
       <c r="L46" s="148"/>
       <c r="M46" s="148">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>12682.5</v>
       </c>
       <c r="N46" s="148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>10160.5</v>
       </c>
       <c r="O46" s="148">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>11848.5</v>
       </c>
       <c r="P46" s="153">
         <f>1-(AVERAGE(AB14:AB15)/AVERAGE($AB$16:$AB$17))</f>
-        <v>0.24193548387096775</v>
+        <v>0.25909172166928174</v>
       </c>
       <c r="Q46" s="153">
         <f>1-(AVERAGE(AC14:AC15)/AVERAGE($AC$16:$AC$17))</f>
-        <v>0.24</v>
+        <v>0.25375429281568596</v>
       </c>
       <c r="R46" s="153">
         <f>1-(AVERAGE(AD14:AD15)/AVERAGE($AD$16:$AD$17))</f>
-        <v>0.26315789473684215</v>
+        <v>0.28184291951465146</v>
       </c>
       <c r="S46" s="148">
         <f>D11/SUM(D6:D13)*M46</f>
@@ -7966,15 +8306,15 @@
       </c>
       <c r="V46" s="153">
         <f>D11/SUM(D6:D13)*P46</f>
-        <v>3.2677446721729508E-2</v>
+        <v>3.4994684514341713E-2</v>
       </c>
       <c r="W46" s="153">
-        <f t="shared" ref="W46:X46" si="27">E11/SUM(E6:E13)*Q46</f>
-        <v>2.774686335035614E-2</v>
+        <f t="shared" ref="W46:X46" si="29">E11/SUM(E6:E13)*Q46</f>
+        <v>2.9337023697179571E-2</v>
       </c>
       <c r="X46" s="153">
-        <f t="shared" si="27"/>
-        <v>3.4355155539890714E-2</v>
+        <f t="shared" si="29"/>
+        <v>3.6794477883422452E-2</v>
       </c>
     </row>
     <row r="47" spans="3:27" x14ac:dyDescent="0.2">
@@ -7989,7 +8329,7 @@
         <v>6086</v>
       </c>
       <c r="G47" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>34169</v>
       </c>
       <c r="H47" s="147"/>
@@ -7998,28 +8338,28 @@
       <c r="K47" s="147"/>
       <c r="L47" s="147"/>
       <c r="M47" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>34169</v>
       </c>
       <c r="N47" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>37585.9</v>
       </c>
       <c r="O47" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>30752.100000000002</v>
       </c>
       <c r="P47" s="155">
         <f>1-(AVERAGE(AB5:AB7)/$AB$18)</f>
-        <v>0.89113924050632909</v>
+        <v>0.7842125554199062</v>
       </c>
       <c r="Q47" s="155">
         <f>1-(AVERAGE(AC5:AC7)/$AC$18)</f>
-        <v>0.88888888888888884</v>
+        <v>0.78572817895429459</v>
       </c>
       <c r="R47" s="155">
         <f>1-(AVERAGE(AD5:AD7)/$AD$18)</f>
-        <v>0.89305555555555549</v>
+        <v>0.77453416149068322</v>
       </c>
       <c r="S47" s="147"/>
       <c r="T47" s="147"/>
@@ -8037,7 +8377,7 @@
         <v>5326</v>
       </c>
       <c r="G48" s="146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>22176</v>
       </c>
       <c r="H48" s="146"/>
@@ -8046,52 +8386,52 @@
       <c r="K48" s="146"/>
       <c r="L48" s="146"/>
       <c r="M48" s="146">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>22176</v>
       </c>
       <c r="N48" s="146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>24393.600000000002</v>
       </c>
       <c r="O48" s="146">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>19958.400000000001</v>
       </c>
       <c r="P48" s="154">
         <f>1-(AVERAGE(AB8:AB10)/$AB$18)</f>
-        <v>0.75991561181434597</v>
+        <v>0.65388849621966627</v>
       </c>
       <c r="Q48" s="154">
         <f>1-(AVERAGE(AC8:AC10)/$AC$18)</f>
-        <v>0.75661375661375663</v>
+        <v>0.65178349847339401</v>
       </c>
       <c r="R48" s="154">
         <f>1-(AVERAGE(AD8:AD10)/$AD$18)</f>
-        <v>0.76249999999999996</v>
+        <v>0.64950310559006208</v>
       </c>
       <c r="S48" s="146">
         <f>SUM(D12)/SUM(D6:D13)*M48</f>
         <v>1480.3244787616509</v>
       </c>
       <c r="T48" s="146">
-        <f t="shared" ref="T48:U48" si="28">SUM(E12)/SUM(E6:E13)*N48</f>
+        <f t="shared" ref="T48:U48" si="30">SUM(E12)/SUM(E6:E13)*N48</f>
         <v>1498.1922676437027</v>
       </c>
       <c r="U48" s="146">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>1246.8867413583491</v>
       </c>
       <c r="V48" s="154">
         <f>SUM(D12)/SUM(D6:D13)*P48</f>
-        <v>5.0726987822957821E-2</v>
+        <v>4.3649312199432591E-2</v>
       </c>
       <c r="W48" s="154">
-        <f t="shared" ref="W48:X48" si="29">SUM(E12)/SUM(E6:E13)*Q48</f>
-        <v>4.6469273897726641E-2</v>
+        <f t="shared" ref="W48:X48" si="31">SUM(E12)/SUM(E6:E13)*Q48</f>
+        <v>4.0030868653687851E-2</v>
       </c>
       <c r="X48" s="154">
-        <f t="shared" si="29"/>
-        <v>4.7636641228041378E-2</v>
+        <f t="shared" si="31"/>
+        <v>4.0577241203268805E-2</v>
       </c>
     </row>
     <row r="49" spans="3:24" x14ac:dyDescent="0.2">
@@ -8106,7 +8446,7 @@
         <v>4565</v>
       </c>
       <c r="G49" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>15798</v>
       </c>
       <c r="H49" s="147">
@@ -8120,28 +8460,28 @@
       <c r="K49" s="147"/>
       <c r="L49" s="147"/>
       <c r="M49" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>13399</v>
       </c>
       <c r="N49" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>26376.400000000001</v>
       </c>
       <c r="O49" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>14218.2</v>
       </c>
       <c r="P49" s="155">
         <f>1-(AVERAGE(AB11:AB13)/$AB$18)</f>
-        <v>0.59493670886075956</v>
+        <v>0.62712357880557112</v>
       </c>
       <c r="Q49" s="155">
         <f>1-(AVERAGE(AC11:AC13)/$AC$18)</f>
-        <v>0.59259259259259256</v>
+        <v>0.62048083999303505</v>
       </c>
       <c r="R49" s="155">
         <f>1-(AVERAGE(AD11:AD13)/$AD$18)</f>
-        <v>0.59722222222222232</v>
+        <v>0.62938185147608328</v>
       </c>
       <c r="S49" s="147"/>
       <c r="T49" s="147"/>
@@ -8159,7 +8499,7 @@
         <v>3804</v>
       </c>
       <c r="G50" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>11293</v>
       </c>
       <c r="H50" s="147">
@@ -8172,28 +8512,28 @@
       <c r="K50" s="147"/>
       <c r="L50" s="147"/>
       <c r="M50" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>10146.5</v>
       </c>
       <c r="N50" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>15711.150000000001</v>
       </c>
       <c r="O50" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>10163.700000000001</v>
       </c>
       <c r="P50" s="155">
         <f>1-(AVERAGE(AB14:AB15)/$AB$18)</f>
-        <v>0.40506329113924056</v>
+        <v>0.42800464625999812</v>
       </c>
       <c r="Q50" s="155">
         <f>1-(AVERAGE(AC14:AC15)/$AC$18)</f>
-        <v>0.39682539682539686</v>
+        <v>0.41712351025950434</v>
       </c>
       <c r="R50" s="155">
         <f>1-(AVERAGE(AD14:AD15)/$AD$18)</f>
-        <v>0.41666666666666663</v>
+        <v>0.44667207285883592</v>
       </c>
       <c r="S50" s="147"/>
       <c r="T50" s="147"/>
@@ -8211,7 +8551,7 @@
         <v>3043</v>
       </c>
       <c r="G51" s="148">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8660</v>
       </c>
       <c r="H51" s="148">
@@ -8222,28 +8562,28 @@
       <c r="K51" s="148"/>
       <c r="L51" s="148"/>
       <c r="M51" s="148">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>4830</v>
       </c>
       <c r="N51" s="148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9526</v>
       </c>
       <c r="O51" s="148">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>7794</v>
       </c>
       <c r="P51" s="153">
         <f>1-(AVERAGE(AB16:AB17)/$AB$18)</f>
-        <v>0.21518987341772156</v>
+        <v>0.2279808844507456</v>
       </c>
       <c r="Q51" s="153">
         <f>1-(AVERAGE(AC16:AC17)/$AC$18)</f>
-        <v>0.20634920634920639</v>
+        <v>0.21892148372984621</v>
       </c>
       <c r="R51" s="153">
         <f>1-(AVERAGE(AD16:AD17)/$AD$18)</f>
-        <v>0.20833333333333337</v>
+        <v>0.22951685337807815</v>
       </c>
       <c r="S51" s="148">
         <f>D12/SUM(D6:D13)*M51</f>
@@ -8259,15 +8599,15 @@
       </c>
       <c r="V51" s="153">
         <f>D12/SUM(D6:D13)*P51</f>
-        <v>1.4364666179738198E-2</v>
+        <v>1.5218510278777514E-2</v>
       </c>
       <c r="W51" s="153">
-        <f t="shared" ref="W51:X51" si="30">E12/SUM(E6:E13)*Q51</f>
-        <v>1.2673438335743631E-2</v>
+        <f t="shared" ref="W51:X51" si="32">E12/SUM(E6:E13)*Q51</f>
+        <v>1.344559532603397E-2</v>
       </c>
       <c r="X51" s="153">
-        <f t="shared" si="30"/>
-        <v>1.30154757453665E-2</v>
+        <f t="shared" si="32"/>
+        <v>1.4338900983817031E-2</v>
       </c>
     </row>
     <row r="52" spans="3:24" x14ac:dyDescent="0.2">
@@ -8282,7 +8622,7 @@
         <v>6086</v>
       </c>
       <c r="G52" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>36041</v>
       </c>
       <c r="H52" s="147"/>
@@ -8291,28 +8631,28 @@
       <c r="K52" s="147"/>
       <c r="L52" s="147"/>
       <c r="M52" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>36041</v>
       </c>
       <c r="N52" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>39645.100000000006</v>
       </c>
       <c r="O52" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>32436.9</v>
       </c>
       <c r="P52" s="155">
         <f>1-(AVERAGE(AB5:AB7)/$AB$19)</f>
-        <v>0.91313131313131313</v>
+        <v>0.7811838232063617</v>
       </c>
       <c r="Q52" s="155">
         <f>1-(AVERAGE(AC5:AC7)/$AC$19)</f>
-        <v>0.91139240506329111</v>
+        <v>0.78546190139049687</v>
       </c>
       <c r="R52" s="155">
         <f>1-(AVERAGE(AD5:AD7)/$AD$19)</f>
-        <v>0.91444444444444439</v>
+        <v>0.78259796027911965</v>
       </c>
       <c r="S52" s="147"/>
       <c r="T52" s="147"/>
@@ -8330,7 +8670,7 @@
         <v>5326</v>
       </c>
       <c r="G53" s="146">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>22176</v>
       </c>
       <c r="H53" s="146"/>
@@ -8339,52 +8679,52 @@
       <c r="K53" s="146"/>
       <c r="L53" s="146"/>
       <c r="M53" s="146">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>22176</v>
       </c>
       <c r="N53" s="146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>24393.600000000002</v>
       </c>
       <c r="O53" s="146">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>19958.400000000001</v>
       </c>
       <c r="P53" s="154">
         <f>1-(AVERAGE(AB8:AB10)/$AB$19)</f>
-        <v>0.80841750841750848</v>
+        <v>0.64903057196453795</v>
       </c>
       <c r="Q53" s="154">
         <f>1-(AVERAGE(AC8:AC10)/$AC$19)</f>
-        <v>0.80590717299578063</v>
+        <v>0.6513507666225693</v>
       </c>
       <c r="R53" s="154">
         <f>1-(AVERAGE(AD8:AD10)/$AD$19)</f>
-        <v>0.81</v>
+        <v>0.66203864734299511</v>
       </c>
       <c r="S53" s="146">
         <f>SUM(D13)/SUM(D6:D13)*M48</f>
         <v>1556.6052637176085</v>
       </c>
       <c r="T53" s="146">
-        <f t="shared" ref="T53:U53" si="31">SUM(E13)/SUM(E6:E13)*N48</f>
+        <f t="shared" ref="T53:U53" si="33">SUM(E13)/SUM(E6:E13)*N48</f>
         <v>2717.5942751454008</v>
       </c>
       <c r="U53" s="146">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1538.1025473834977</v>
       </c>
       <c r="V53" s="154">
         <f>SUM(D13)/SUM(D6:D13)*P53</f>
-        <v>5.6745443221688667E-2</v>
+        <v>4.5557557929006579E-2</v>
       </c>
       <c r="W53" s="154">
-        <f t="shared" ref="W53:X53" si="32">SUM(E13)/SUM(E6:E13)*Q53</f>
-        <v>8.9782923374653489E-2</v>
+        <f t="shared" ref="W53:X53" si="34">SUM(E13)/SUM(E6:E13)*Q53</f>
+        <v>7.2564406831507527E-2</v>
       </c>
       <c r="X53" s="154">
-        <f t="shared" si="32"/>
-        <v>6.2422992994460136E-2</v>
+        <f t="shared" si="34"/>
+        <v>5.1020288697720552E-2</v>
       </c>
     </row>
     <row r="54" spans="3:24" x14ac:dyDescent="0.2">
@@ -8399,7 +8739,7 @@
         <v>4565</v>
       </c>
       <c r="G54" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>15798</v>
       </c>
       <c r="H54" s="147"/>
@@ -8412,28 +8752,28 @@
         <v>8100</v>
       </c>
       <c r="M54" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>19649</v>
       </c>
       <c r="N54" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>17377.800000000003</v>
       </c>
       <c r="O54" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>11159.1</v>
       </c>
       <c r="P54" s="155">
         <f>1-(AVERAGE(AB11:AB13)/$AB$19)</f>
-        <v>0.67676767676767668</v>
+        <v>0.6218899896561173</v>
       </c>
       <c r="Q54" s="155">
         <f>1-(AVERAGE(AC11:AC13)/$AC$19)</f>
-        <v>0.67510548523206748</v>
+        <v>0.62000920804046178</v>
       </c>
       <c r="R54" s="155">
         <f>1-(AVERAGE(AD11:AD13)/$AD$19)</f>
-        <v>0.67777777777777781</v>
+        <v>0.64263703104917957</v>
       </c>
       <c r="S54" s="147"/>
       <c r="T54" s="147"/>
@@ -8451,7 +8791,7 @@
         <v>3804</v>
       </c>
       <c r="G55" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>11293</v>
       </c>
       <c r="H55" s="147">
@@ -8469,28 +8809,28 @@
         <v>4400</v>
       </c>
       <c r="M55" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>18864.333333333332</v>
       </c>
       <c r="N55" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>21853.15</v>
       </c>
       <c r="O55" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>7281.85</v>
       </c>
       <c r="P55" s="155">
         <f>1-(AVERAGE(AB14:AB15)/$AB$19)</f>
-        <v>0.5252525252525253</v>
+        <v>0.41997627946951466</v>
       </c>
       <c r="Q55" s="155">
         <f>1-(AVERAGE(AC14:AC15)/$AC$19)</f>
-        <v>0.51898734177215189</v>
+        <v>0.41639916428192481</v>
       </c>
       <c r="R55" s="155">
         <f>1-(AVERAGE(AD14:AD15)/$AD$19)</f>
-        <v>0.53333333333333333</v>
+        <v>0.46646187825902119</v>
       </c>
       <c r="S55" s="147"/>
       <c r="T55" s="147"/>
@@ -8508,7 +8848,7 @@
         <v>3043</v>
       </c>
       <c r="G56" s="147">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8660</v>
       </c>
       <c r="H56" s="147">
@@ -8523,28 +8863,28 @@
       </c>
       <c r="L56" s="147"/>
       <c r="M56" s="147">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>12830</v>
       </c>
       <c r="N56" s="147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>17208.666666666668</v>
       </c>
       <c r="O56" s="147">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>7794</v>
       </c>
       <c r="P56" s="155">
         <f>1-(AVERAGE(AB16:AB17)/$AB$19)</f>
-        <v>0.3737373737373737</v>
+        <v>0.21714504008878011</v>
       </c>
       <c r="Q56" s="155">
         <f>1-(AVERAGE(AC16:AC17)/$AC$19)</f>
-        <v>0.36708860759493667</v>
+        <v>0.21795083026999229</v>
       </c>
       <c r="R56" s="155">
         <f>1-(AVERAGE(AD16:AD17)/$AD$19)</f>
-        <v>0.3666666666666667</v>
+        <v>0.25707322779523334</v>
       </c>
       <c r="S56" s="147"/>
       <c r="T56" s="147"/>
@@ -8570,28 +8910,28 @@
         <v>2200</v>
       </c>
       <c r="M57" s="149">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>2128</v>
       </c>
       <c r="N57" s="149">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1600</v>
       </c>
       <c r="O57" s="149">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1100</v>
       </c>
       <c r="P57" s="153">
         <f>1-(AB18/$AB$19)</f>
-        <v>0.20202020202020199</v>
+        <v>-1.4035720286869058E-2</v>
       </c>
       <c r="Q57" s="153">
         <f>1-(AC18/$AC$19)</f>
-        <v>0.20253164556962022</v>
+        <v>-1.2427092022566644E-3</v>
       </c>
       <c r="R57" s="153">
         <f>1-(AD18/$AD$19)</f>
-        <v>0.19999999999999996</v>
+        <v>3.5765057987280247E-2</v>
       </c>
       <c r="S57" s="148">
         <f>D13/SUM(D6:D13)*M57</f>
@@ -8607,15 +8947,15 @@
       </c>
       <c r="V57" s="153">
         <f>D13/SUM(D6:D13)*P57</f>
-        <v>1.4180452283637315E-2</v>
+        <v>-9.8521266588241329E-4</v>
       </c>
       <c r="W57" s="153">
-        <f t="shared" ref="W57:X57" si="33">E13/SUM(E6:E13)*Q57</f>
-        <v>2.2563247759075217E-2</v>
+        <f t="shared" ref="W57:X57" si="35">E13/SUM(E6:E13)*Q57</f>
+        <v>-1.3844530588856169E-4</v>
       </c>
       <c r="X57" s="153">
-        <f t="shared" si="33"/>
-        <v>1.5413084689990152E-2</v>
+        <f t="shared" si="35"/>
+        <v>2.7562493385017966E-3</v>
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.2">
@@ -8624,24 +8964,24 @@
         <v>9608.4735804205193</v>
       </c>
       <c r="T59" s="157">
-        <f t="shared" ref="T59:U59" si="34">SUM(T37,T39,T42,T46,T51,T57)</f>
+        <f t="shared" ref="T59:U59" si="36">SUM(T37,T39,T42,T46,T51,T57)</f>
         <v>14333.869646601945</v>
       </c>
       <c r="U59" s="157">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>11196.414691601361</v>
       </c>
       <c r="V59" s="156">
         <f>SUM(V37,V39,V42,V46,V51,V57)</f>
-        <v>0.3499559220938272</v>
+        <v>0.20172336037443986</v>
       </c>
       <c r="W59" s="156">
-        <f t="shared" ref="W59:X59" si="35">SUM(W37,W39,W42,W46,W51,W57)</f>
-        <v>0.34759093292022342</v>
+        <f t="shared" ref="W59:X59" si="37">SUM(W37,W39,W42,W46,W51,W57)</f>
+        <v>0.2000191767273756</v>
       </c>
       <c r="X59" s="156">
-        <f t="shared" si="35"/>
-        <v>0.36920600336632792</v>
+        <f t="shared" si="37"/>
+        <v>0.21813305903885022</v>
       </c>
     </row>
     <row r="60" spans="3:24" x14ac:dyDescent="0.2">
@@ -8653,24 +8993,24 @@
         <v>20563.0239417189</v>
       </c>
       <c r="T60" s="158">
-        <f t="shared" ref="T60:X60" si="36">SUM(T38,T41,T44,T48,T53,T57)</f>
+        <f t="shared" ref="T60:X60" si="38">SUM(T38,T41,T44,T48,T53,T57)</f>
         <v>22259.387557085229</v>
       </c>
       <c r="U60" s="158">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>15982.779351113084</v>
       </c>
       <c r="V60" s="159">
-        <f t="shared" si="36"/>
-        <v>0.56982150406598298</v>
+        <f t="shared" si="38"/>
+        <v>0.40290106058759934</v>
       </c>
       <c r="W60" s="159">
-        <f t="shared" si="36"/>
-        <v>0.57417922843609159</v>
+        <f t="shared" si="38"/>
+        <v>0.40913942308828122</v>
       </c>
       <c r="X60" s="159">
-        <f t="shared" si="36"/>
-        <v>0.51228555848472779</v>
+        <f t="shared" si="38"/>
+        <v>0.35320524382665802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update before changing to main
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRes_RSD-Retrofit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CE220-6AC4-43DA-A646-51B43AD8C58F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED8A81-A060-4CA1-A2DC-B8D02B90A671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -5023,7 +5023,7 @@
   </sheetPr>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7:S12"/>
     </sheetView>
   </sheetViews>
@@ -5806,8 +5806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O59" sqref="M59:O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9331,16 +9331,28 @@
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="M59" s="144">
+        <f t="shared" ref="M59:N59" si="50">AVERAGE(M38,M40:M41,M43:M45,M47:M50,M53:M56)</f>
+        <v>21359.773809523809</v>
+      </c>
+      <c r="N59" s="144">
+        <f t="shared" si="50"/>
+        <v>24228.569047619047</v>
+      </c>
+      <c r="O59" s="144">
+        <f>AVERAGE(O38,O40:O41,O43:O45,O47:O50,O53:O56)</f>
+        <v>17675.482142857145</v>
+      </c>
       <c r="S59" s="155">
         <f>SUM(S37,S39,S42,S46,S51,S57)</f>
         <v>9608.4735804205193</v>
       </c>
       <c r="T59" s="155">
-        <f t="shared" ref="T59:U59" si="50">SUM(T37,T39,T42,T46,T51,T57)</f>
+        <f t="shared" ref="T59:U59" si="51">SUM(T37,T39,T42,T46,T51,T57)</f>
         <v>14333.869646601945</v>
       </c>
       <c r="U59" s="155">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>11196.414691601361</v>
       </c>
       <c r="V59" s="154">
@@ -9348,11 +9360,11 @@
         <v>0.20172336037443986</v>
       </c>
       <c r="W59" s="154">
-        <f t="shared" ref="W59:X59" si="51">SUM(W37,W39,W42,W46,W51,W57)</f>
+        <f t="shared" ref="W59:X59" si="52">SUM(W37,W39,W42,W46,W51,W57)</f>
         <v>0.2000191767273756</v>
       </c>
       <c r="X59" s="154">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0.21813305903885022</v>
       </c>
     </row>

</xml_diff>